<commit_message>
add buenos aires surprise songs
</commit_message>
<xml_diff>
--- a/data-raw/surprise-songs.xlsx
+++ b/data-raw/surprise-songs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakethompson/Documents/GIT/packages/taylor/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66AE71EB-0619-F04B-B356-EE4921ACC798}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{126CEFCD-3904-C84D-A35F-19E59AA91CB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="14400" windowHeight="17500" xr2:uid="{23F40540-2069-D04D-A50F-51228CFC4AB9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="156">
   <si>
     <t>date</t>
   </si>
@@ -474,6 +474,36 @@
   </si>
   <si>
     <t>North America</t>
+  </si>
+  <si>
+    <t>South America</t>
+  </si>
+  <si>
+    <t>Buenos Aires, Argentina</t>
+  </si>
+  <si>
+    <t>Rio de Janeiro, Brazil</t>
+  </si>
+  <si>
+    <t>São Paulo, Brazil</t>
+  </si>
+  <si>
+    <t>The Very First Night (Taylor's Version) [From The Vault]</t>
+  </si>
+  <si>
+    <t>Labyrinth</t>
+  </si>
+  <si>
+    <t>Is It Over Now? (Taylor's Version) [From The Vault]</t>
+  </si>
+  <si>
+    <t>End Game</t>
+  </si>
+  <si>
+    <t>Better Than Revenge (Taylor's Version)</t>
+  </si>
+  <si>
+    <t>"Slut!" (Taylor's Version) [From The Vault]</t>
   </si>
 </sst>
 </file>
@@ -829,17 +859,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04F0F9D9-7CA5-0C41-BC65-3D3349CBCA23}">
-  <dimension ref="A1:H115"/>
+  <dimension ref="A1:H133"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A96" sqref="A96"/>
+    <sheetView tabSelected="1" topLeftCell="C106" workbookViewId="0">
+      <selection activeCell="F122" sqref="F122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.1640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="52.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.5" bestFit="1" customWidth="1"/>
@@ -3520,6 +3550,312 @@
         <v>75</v>
       </c>
     </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>146</v>
+      </c>
+      <c r="B116" s="1">
+        <v>45239</v>
+      </c>
+      <c r="C116" t="s">
+        <v>147</v>
+      </c>
+      <c r="D116">
+        <v>1</v>
+      </c>
+      <c r="E116" t="s">
+        <v>144</v>
+      </c>
+      <c r="F116" t="s">
+        <v>7</v>
+      </c>
+      <c r="G116" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>146</v>
+      </c>
+      <c r="B117" s="1">
+        <v>45239</v>
+      </c>
+      <c r="C117" t="s">
+        <v>147</v>
+      </c>
+      <c r="D117">
+        <v>1</v>
+      </c>
+      <c r="E117" t="s">
+        <v>144</v>
+      </c>
+      <c r="F117" t="s">
+        <v>8</v>
+      </c>
+      <c r="G117" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>146</v>
+      </c>
+      <c r="B118" s="1">
+        <v>45241</v>
+      </c>
+      <c r="C118" t="s">
+        <v>147</v>
+      </c>
+      <c r="D118">
+        <v>2</v>
+      </c>
+      <c r="E118" t="s">
+        <v>141</v>
+      </c>
+      <c r="F118" t="s">
+        <v>7</v>
+      </c>
+      <c r="G118" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>146</v>
+      </c>
+      <c r="B119" s="1">
+        <v>45241</v>
+      </c>
+      <c r="C119" t="s">
+        <v>147</v>
+      </c>
+      <c r="D119">
+        <v>2</v>
+      </c>
+      <c r="E119" t="s">
+        <v>141</v>
+      </c>
+      <c r="F119" t="s">
+        <v>8</v>
+      </c>
+      <c r="G119" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>146</v>
+      </c>
+      <c r="B120" s="1">
+        <v>45242</v>
+      </c>
+      <c r="C120" t="s">
+        <v>147</v>
+      </c>
+      <c r="D120">
+        <v>3</v>
+      </c>
+      <c r="E120" t="s">
+        <v>143</v>
+      </c>
+      <c r="F120" t="s">
+        <v>7</v>
+      </c>
+      <c r="G120" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>146</v>
+      </c>
+      <c r="B121" s="1">
+        <v>45242</v>
+      </c>
+      <c r="C121" t="s">
+        <v>147</v>
+      </c>
+      <c r="D121">
+        <v>3</v>
+      </c>
+      <c r="E121" t="s">
+        <v>143</v>
+      </c>
+      <c r="F121" t="s">
+        <v>8</v>
+      </c>
+      <c r="G121" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>146</v>
+      </c>
+      <c r="B122" s="1">
+        <v>45247</v>
+      </c>
+      <c r="C122" t="s">
+        <v>148</v>
+      </c>
+      <c r="D122">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>146</v>
+      </c>
+      <c r="B123" s="1">
+        <v>45247</v>
+      </c>
+      <c r="C123" t="s">
+        <v>148</v>
+      </c>
+      <c r="D123">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>146</v>
+      </c>
+      <c r="B124" s="1">
+        <v>45248</v>
+      </c>
+      <c r="C124" t="s">
+        <v>148</v>
+      </c>
+      <c r="D124">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>146</v>
+      </c>
+      <c r="B125" s="1">
+        <v>45248</v>
+      </c>
+      <c r="C125" t="s">
+        <v>148</v>
+      </c>
+      <c r="D125">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>146</v>
+      </c>
+      <c r="B126" s="1">
+        <v>45249</v>
+      </c>
+      <c r="C126" t="s">
+        <v>148</v>
+      </c>
+      <c r="D126">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>146</v>
+      </c>
+      <c r="B127" s="1">
+        <v>45249</v>
+      </c>
+      <c r="C127" t="s">
+        <v>148</v>
+      </c>
+      <c r="D127">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>146</v>
+      </c>
+      <c r="B128" s="1">
+        <v>45254</v>
+      </c>
+      <c r="C128" t="s">
+        <v>149</v>
+      </c>
+      <c r="D128">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>146</v>
+      </c>
+      <c r="B129" s="1">
+        <v>45254</v>
+      </c>
+      <c r="C129" t="s">
+        <v>149</v>
+      </c>
+      <c r="D129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>146</v>
+      </c>
+      <c r="B130" s="1">
+        <v>45255</v>
+      </c>
+      <c r="C130" t="s">
+        <v>149</v>
+      </c>
+      <c r="D130">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>146</v>
+      </c>
+      <c r="B131" s="1">
+        <v>45255</v>
+      </c>
+      <c r="C131" t="s">
+        <v>149</v>
+      </c>
+      <c r="D131">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>146</v>
+      </c>
+      <c r="B132" s="1">
+        <v>45256</v>
+      </c>
+      <c r="C132" t="s">
+        <v>149</v>
+      </c>
+      <c r="D132">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>146</v>
+      </c>
+      <c r="B133" s="1">
+        <v>45256</v>
+      </c>
+      <c r="C133" t="s">
+        <v>149</v>
+      </c>
+      <c r="D133">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add rio surprise songs
</commit_message>
<xml_diff>
--- a/data-raw/surprise-songs.xlsx
+++ b/data-raw/surprise-songs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakethompson/Documents/GIT/packages/taylor/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{126CEFCD-3904-C84D-A35F-19E59AA91CB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9EE2A98-CC5D-F34F-A7AF-B96DCB0AC2CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="14400" windowHeight="17500" xr2:uid="{23F40540-2069-D04D-A50F-51228CFC4AB9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="162">
   <si>
     <t>date</t>
   </si>
@@ -504,6 +504,24 @@
   </si>
   <si>
     <t>"Slut!" (Taylor's Version) [From The Vault]</t>
+  </si>
+  <si>
+    <t>Stay Beautiful</t>
+  </si>
+  <si>
+    <t>Suburban Legends (Taylor's Version) [From The Vault]</t>
+  </si>
+  <si>
+    <t>Dancing With Our Hands Tied</t>
+  </si>
+  <si>
+    <t>Bigger Than The Whole Sky</t>
+  </si>
+  <si>
+    <t>ME!</t>
+  </si>
+  <si>
+    <t>So It Goes...</t>
   </si>
 </sst>
 </file>
@@ -861,8 +879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04F0F9D9-7CA5-0C41-BC65-3D3349CBCA23}">
   <dimension ref="A1:H133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C106" workbookViewId="0">
-      <selection activeCell="F122" sqref="F122"/>
+    <sheetView tabSelected="1" topLeftCell="C103" workbookViewId="0">
+      <selection activeCell="G123" sqref="G123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3701,6 +3719,15 @@
       <c r="D122">
         <v>1</v>
       </c>
+      <c r="E122" t="s">
+        <v>143</v>
+      </c>
+      <c r="F122" t="s">
+        <v>7</v>
+      </c>
+      <c r="G122" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
@@ -3715,19 +3742,37 @@
       <c r="D123">
         <v>1</v>
       </c>
+      <c r="E123" t="s">
+        <v>143</v>
+      </c>
+      <c r="F123" t="s">
+        <v>8</v>
+      </c>
+      <c r="G123" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>146</v>
       </c>
       <c r="B124" s="1">
-        <v>45248</v>
+        <v>45249</v>
       </c>
       <c r="C124" t="s">
         <v>148</v>
       </c>
       <c r="D124">
         <v>2</v>
+      </c>
+      <c r="E124" t="s">
+        <v>144</v>
+      </c>
+      <c r="F124" t="s">
+        <v>7</v>
+      </c>
+      <c r="G124" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.2">
@@ -3735,13 +3780,22 @@
         <v>146</v>
       </c>
       <c r="B125" s="1">
-        <v>45248</v>
+        <v>45249</v>
       </c>
       <c r="C125" t="s">
         <v>148</v>
       </c>
       <c r="D125">
         <v>2</v>
+      </c>
+      <c r="E125" t="s">
+        <v>144</v>
+      </c>
+      <c r="F125" t="s">
+        <v>8</v>
+      </c>
+      <c r="G125" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.2">
@@ -3749,13 +3803,22 @@
         <v>146</v>
       </c>
       <c r="B126" s="1">
-        <v>45249</v>
+        <v>45250</v>
       </c>
       <c r="C126" t="s">
         <v>148</v>
       </c>
       <c r="D126">
         <v>3</v>
+      </c>
+      <c r="E126" t="s">
+        <v>142</v>
+      </c>
+      <c r="F126" t="s">
+        <v>7</v>
+      </c>
+      <c r="G126" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.2">
@@ -3763,13 +3826,22 @@
         <v>146</v>
       </c>
       <c r="B127" s="1">
-        <v>45249</v>
+        <v>45250</v>
       </c>
       <c r="C127" t="s">
         <v>148</v>
       </c>
       <c r="D127">
         <v>3</v>
+      </c>
+      <c r="E127" t="s">
+        <v>142</v>
+      </c>
+      <c r="F127" t="s">
+        <v>8</v>
+      </c>
+      <c r="G127" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
finish south american surprise songs
</commit_message>
<xml_diff>
--- a/data-raw/surprise-songs.xlsx
+++ b/data-raw/surprise-songs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakethompson/Documents/GIT/packages/taylor/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9EE2A98-CC5D-F34F-A7AF-B96DCB0AC2CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33598DDC-3087-9249-B453-AB86C6CFBB0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="14400" windowHeight="17500" xr2:uid="{23F40540-2069-D04D-A50F-51228CFC4AB9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="168">
   <si>
     <t>date</t>
   </si>
@@ -522,6 +522,24 @@
   </si>
   <si>
     <t>So It Goes...</t>
+  </si>
+  <si>
+    <t>it's time to go</t>
+  </si>
+  <si>
+    <t>Now That We Don't Talk (Taylor's Version) [From The Vault]</t>
+  </si>
+  <si>
+    <t>Innocent (Taylor's Version)</t>
+  </si>
+  <si>
+    <t>Untouchable (Taylor's Version)</t>
+  </si>
+  <si>
+    <t>Safe &amp; Sound (Taylor's Version)</t>
+  </si>
+  <si>
+    <t>Say Don't Go (Taylor's Version) [From The Vault]</t>
   </si>
 </sst>
 </file>
@@ -880,7 +898,7 @@
   <dimension ref="A1:H133"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C103" workbookViewId="0">
-      <selection activeCell="G123" sqref="G123"/>
+      <selection activeCell="G133" sqref="G133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3857,8 +3875,17 @@
       <c r="D128">
         <v>1</v>
       </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E128" t="s">
+        <v>144</v>
+      </c>
+      <c r="F128" t="s">
+        <v>7</v>
+      </c>
+      <c r="G128" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>146</v>
       </c>
@@ -3871,8 +3898,17 @@
       <c r="D129">
         <v>1</v>
       </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E129" t="s">
+        <v>144</v>
+      </c>
+      <c r="F129" t="s">
+        <v>8</v>
+      </c>
+      <c r="G129" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>146</v>
       </c>
@@ -3885,8 +3921,17 @@
       <c r="D130">
         <v>2</v>
       </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E130" t="s">
+        <v>143</v>
+      </c>
+      <c r="F130" t="s">
+        <v>7</v>
+      </c>
+      <c r="G130" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>146</v>
       </c>
@@ -3899,8 +3944,17 @@
       <c r="D131">
         <v>2</v>
       </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E131" t="s">
+        <v>143</v>
+      </c>
+      <c r="F131" t="s">
+        <v>8</v>
+      </c>
+      <c r="G131" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>146</v>
       </c>
@@ -3913,8 +3967,17 @@
       <c r="D132">
         <v>3</v>
       </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E132" t="s">
+        <v>142</v>
+      </c>
+      <c r="F132" t="s">
+        <v>7</v>
+      </c>
+      <c r="G132" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>146</v>
       </c>
@@ -3926,6 +3989,15 @@
       </c>
       <c r="D133">
         <v>3</v>
+      </c>
+      <c r="E133" t="s">
+        <v>142</v>
+      </c>
+      <c r="F133" t="s">
+        <v>8</v>
+      </c>
+      <c r="G133" t="s">
+        <v>162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
start adding eras tour data for asia-pacific
</commit_message>
<xml_diff>
--- a/data-raw/surprise-songs.xlsx
+++ b/data-raw/surprise-songs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakethompson/Documents/GIT/packages/taylor/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33598DDC-3087-9249-B453-AB86C6CFBB0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FBB81D1-B754-7241-9D0E-AA13937CC815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="14400" windowHeight="17500" xr2:uid="{23F40540-2069-D04D-A50F-51228CFC4AB9}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="15660" windowHeight="17500" xr2:uid="{23F40540-2069-D04D-A50F-51228CFC4AB9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1199" uniqueCount="203">
   <si>
     <t>date</t>
   </si>
@@ -473,9 +473,6 @@
     <t>blue</t>
   </si>
   <si>
-    <t>North America</t>
-  </si>
-  <si>
     <t>South America</t>
   </si>
   <si>
@@ -540,14 +537,123 @@
   </si>
   <si>
     <t>Say Don't Go (Taylor's Version) [From The Vault]</t>
+  </si>
+  <si>
+    <t>Asia-Pacific</t>
+  </si>
+  <si>
+    <t>Tokyo, Japan</t>
+  </si>
+  <si>
+    <t>Melbourne, Australia</t>
+  </si>
+  <si>
+    <t>Sydney, Australia</t>
+  </si>
+  <si>
+    <t>Singapore</t>
+  </si>
+  <si>
+    <t>Superman (Taylor's Version)</t>
+  </si>
+  <si>
+    <t>The Outside</t>
+  </si>
+  <si>
+    <t>Electric Touch (Taylor's Version) [From The Vault]</t>
+  </si>
+  <si>
+    <t>Dear Reader</t>
+  </si>
+  <si>
+    <t>Eyes Open (Taylor's Version)</t>
+  </si>
+  <si>
+    <t>Paris, France</t>
+  </si>
+  <si>
+    <t>Stockholm, Sweden</t>
+  </si>
+  <si>
+    <t>Lisbon, Portugal</t>
+  </si>
+  <si>
+    <t>Madrid, Spain</t>
+  </si>
+  <si>
+    <t>Lyon, France</t>
+  </si>
+  <si>
+    <t>Edinburgh, Scotland</t>
+  </si>
+  <si>
+    <t>Liverpool, England</t>
+  </si>
+  <si>
+    <t>Cardiff, Wales</t>
+  </si>
+  <si>
+    <t>London, England</t>
+  </si>
+  <si>
+    <t>Dublin, Ireland</t>
+  </si>
+  <si>
+    <t>Amsterdam, Netherlands</t>
+  </si>
+  <si>
+    <t>Milan, Italy</t>
+  </si>
+  <si>
+    <t>Gelsenkirchen, Germany</t>
+  </si>
+  <si>
+    <t>Hamburg, Germany</t>
+  </si>
+  <si>
+    <t>Munich, Germany</t>
+  </si>
+  <si>
+    <t>Warsaw, Poland</t>
+  </si>
+  <si>
+    <t>Vienna, Austria</t>
+  </si>
+  <si>
+    <t>Miami, FL</t>
+  </si>
+  <si>
+    <t>New Orleans, LA</t>
+  </si>
+  <si>
+    <t>Indianapolis, IN</t>
+  </si>
+  <si>
+    <t>Toronto, Canada</t>
+  </si>
+  <si>
+    <t>Vancouver, Canada</t>
+  </si>
+  <si>
+    <t>Europe</t>
+  </si>
+  <si>
+    <t>Zürich, Switzerland</t>
+  </si>
+  <si>
+    <t>North America (Leg 1)</t>
+  </si>
+  <si>
+    <t>North America (Leg 2)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -578,9 +684,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -895,15 +1002,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04F0F9D9-7CA5-0C41-BC65-3D3349CBCA23}">
-  <dimension ref="A1:H133"/>
+  <dimension ref="A1:H303"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C103" workbookViewId="0">
-      <selection activeCell="G133" sqref="G133"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A289" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C304" sqref="C304"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.1640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="52.5" bestFit="1" customWidth="1"/>
@@ -939,7 +1047,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B2" s="1">
         <v>45002</v>
@@ -962,7 +1070,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B3" s="1">
         <v>45002</v>
@@ -985,7 +1093,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B4" s="1">
         <v>45003</v>
@@ -1008,7 +1116,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B5" s="1">
         <v>45003</v>
@@ -1031,7 +1139,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B6" s="1">
         <v>45009</v>
@@ -1054,7 +1162,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B7" s="1">
         <v>45009</v>
@@ -1077,7 +1185,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B8" s="1">
         <v>45010</v>
@@ -1103,7 +1211,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B9" s="1">
         <v>45010</v>
@@ -1126,7 +1234,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B10" s="1">
         <v>45016</v>
@@ -1149,7 +1257,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B11" s="1">
         <v>45016</v>
@@ -1172,7 +1280,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B12" s="1">
         <v>45017</v>
@@ -1195,7 +1303,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B13" s="1">
         <v>45017</v>
@@ -1218,7 +1326,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B14" s="1">
         <v>45018</v>
@@ -1241,7 +1349,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B15" s="1">
         <v>45018</v>
@@ -1264,7 +1372,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B16" s="1">
         <v>45029</v>
@@ -1287,7 +1395,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B17" s="1">
         <v>45029</v>
@@ -1310,7 +1418,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B18" s="1">
         <v>45030</v>
@@ -1336,7 +1444,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B19" s="1">
         <v>45030</v>
@@ -1359,7 +1467,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B20" s="1">
         <v>45031</v>
@@ -1385,7 +1493,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B21" s="1">
         <v>45031</v>
@@ -1408,7 +1516,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B22" s="1">
         <v>45037</v>
@@ -1431,7 +1539,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B23" s="1">
         <v>45037</v>
@@ -1454,7 +1562,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B24" s="1">
         <v>45038</v>
@@ -1477,7 +1585,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B25" s="1">
         <v>45038</v>
@@ -1500,7 +1608,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B26" s="1">
         <v>45039</v>
@@ -1523,7 +1631,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B27" s="1">
         <v>45039</v>
@@ -1546,7 +1654,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B28" s="1">
         <v>45044</v>
@@ -1569,7 +1677,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B29" s="1">
         <v>45044</v>
@@ -1592,7 +1700,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B30" s="1">
         <v>45045</v>
@@ -1615,7 +1723,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B31" s="1">
         <v>45045</v>
@@ -1638,7 +1746,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B32" s="1">
         <v>45046</v>
@@ -1661,7 +1769,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B33" s="1">
         <v>45046</v>
@@ -1684,7 +1792,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B34" s="1">
         <v>45051</v>
@@ -1707,7 +1815,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B35" s="1">
         <v>45051</v>
@@ -1730,7 +1838,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B36" s="1">
         <v>45052</v>
@@ -1753,7 +1861,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B37" s="1">
         <v>45052</v>
@@ -1776,7 +1884,7 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B38" s="1">
         <v>45053</v>
@@ -1802,7 +1910,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B39" s="1">
         <v>45053</v>
@@ -1825,7 +1933,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B40" s="1">
         <v>45058</v>
@@ -1848,7 +1956,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B41" s="1">
         <v>45058</v>
@@ -1871,7 +1979,7 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B42" s="1">
         <v>45059</v>
@@ -1894,7 +2002,7 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B43" s="1">
         <v>45059</v>
@@ -1917,7 +2025,7 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B44" s="1">
         <v>45060</v>
@@ -1940,7 +2048,7 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B45" s="1">
         <v>45060</v>
@@ -1963,7 +2071,7 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B46" s="1">
         <v>45065</v>
@@ -1986,7 +2094,7 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B47" s="1">
         <v>45065</v>
@@ -2009,7 +2117,7 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B48" s="1">
         <v>45066</v>
@@ -2032,7 +2140,7 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B49" s="1">
         <v>45066</v>
@@ -2055,7 +2163,7 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B50" s="1">
         <v>45067</v>
@@ -2078,7 +2186,7 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B51" s="1">
         <v>45067</v>
@@ -2101,7 +2209,7 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B52" s="1">
         <v>45072</v>
@@ -2127,7 +2235,7 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B53" s="1">
         <v>45072</v>
@@ -2150,7 +2258,7 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B54" s="1">
         <v>45073</v>
@@ -2173,7 +2281,7 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B55" s="1">
         <v>45073</v>
@@ -2196,7 +2304,7 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B56" s="1">
         <v>45074</v>
@@ -2219,7 +2327,7 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B57" s="1">
         <v>45074</v>
@@ -2242,7 +2350,7 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B58" s="1">
         <v>45079</v>
@@ -2265,7 +2373,7 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B59" s="1">
         <v>45079</v>
@@ -2288,7 +2396,7 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B60" s="1">
         <v>45080</v>
@@ -2314,7 +2422,7 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B61" s="1">
         <v>45080</v>
@@ -2337,7 +2445,7 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B62" s="1">
         <v>45081</v>
@@ -2360,7 +2468,7 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B63" s="1">
         <v>45081</v>
@@ -2383,7 +2491,7 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B64" s="1">
         <v>45086</v>
@@ -2406,7 +2514,7 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B65" s="1">
         <v>45086</v>
@@ -2429,7 +2537,7 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B66" s="1">
         <v>45087</v>
@@ -2452,7 +2560,7 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B67" s="1">
         <v>45087</v>
@@ -2475,7 +2583,7 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B68" s="1">
         <v>45093</v>
@@ -2498,7 +2606,7 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B69" s="1">
         <v>45093</v>
@@ -2521,7 +2629,7 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B70" s="1">
         <v>45094</v>
@@ -2547,7 +2655,7 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B71" s="1">
         <v>45094</v>
@@ -2570,7 +2678,7 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B72" s="1">
         <v>45100</v>
@@ -2593,7 +2701,7 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B73" s="1">
         <v>45100</v>
@@ -2616,7 +2724,7 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B74" s="1">
         <v>45101</v>
@@ -2639,7 +2747,7 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B75" s="1">
         <v>45101</v>
@@ -2662,7 +2770,7 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B76" s="1">
         <v>45107</v>
@@ -2685,7 +2793,7 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B77" s="1">
         <v>45107</v>
@@ -2708,7 +2816,7 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B78" s="1">
         <v>45108</v>
@@ -2734,7 +2842,7 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B79" s="1">
         <v>45108</v>
@@ -2757,7 +2865,7 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B80" s="1">
         <v>45114</v>
@@ -2780,7 +2888,7 @@
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B81" s="1">
         <v>45114</v>
@@ -2803,7 +2911,7 @@
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B82" s="1">
         <v>45115</v>
@@ -2826,7 +2934,7 @@
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B83" s="1">
         <v>45115</v>
@@ -2849,7 +2957,7 @@
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B84" s="1">
         <v>45121</v>
@@ -2872,7 +2980,7 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B85" s="1">
         <v>45121</v>
@@ -2895,7 +3003,7 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B86" s="1">
         <v>45122</v>
@@ -2918,7 +3026,7 @@
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B87" s="1">
         <v>45122</v>
@@ -2941,7 +3049,7 @@
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B88" s="1">
         <v>45129</v>
@@ -2964,7 +3072,7 @@
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B89" s="1">
         <v>45129</v>
@@ -2987,7 +3095,7 @@
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B90" s="1">
         <v>45130</v>
@@ -3010,7 +3118,7 @@
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B91" s="1">
         <v>45130</v>
@@ -3033,7 +3141,7 @@
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B92" s="1">
         <v>45135</v>
@@ -3059,7 +3167,7 @@
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B93" s="1">
         <v>45135</v>
@@ -3082,7 +3190,7 @@
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B94" s="1">
         <v>45136</v>
@@ -3105,7 +3213,7 @@
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B95" s="1">
         <v>45136</v>
@@ -3128,7 +3236,7 @@
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B96" s="1">
         <v>45141</v>
@@ -3151,7 +3259,7 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B97" s="1">
         <v>45141</v>
@@ -3174,7 +3282,7 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B98" s="1">
         <v>45142</v>
@@ -3197,7 +3305,7 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B99" s="1">
         <v>45142</v>
@@ -3220,7 +3328,7 @@
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B100" s="1">
         <v>45143</v>
@@ -3243,7 +3351,7 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B101" s="1">
         <v>45143</v>
@@ -3266,7 +3374,7 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B102" s="1">
         <v>45145</v>
@@ -3289,7 +3397,7 @@
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B103" s="1">
         <v>45145</v>
@@ -3312,7 +3420,7 @@
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B104" s="1">
         <v>45146</v>
@@ -3335,7 +3443,7 @@
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B105" s="1">
         <v>45146</v>
@@ -3358,7 +3466,7 @@
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B106" s="1">
         <v>45147</v>
@@ -3381,7 +3489,7 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B107" s="1">
         <v>45147</v>
@@ -3404,7 +3512,7 @@
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B108" s="1">
         <v>45162</v>
@@ -3427,7 +3535,7 @@
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B109" s="1">
         <v>45162</v>
@@ -3450,7 +3558,7 @@
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B110" s="1">
         <v>45163</v>
@@ -3473,7 +3581,7 @@
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B111" s="1">
         <v>45163</v>
@@ -3496,7 +3604,7 @@
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B112" s="1">
         <v>45164</v>
@@ -3519,7 +3627,7 @@
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B113" s="1">
         <v>45164</v>
@@ -3542,7 +3650,7 @@
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B114" s="1">
         <v>45165</v>
@@ -3565,7 +3673,7 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="B115" s="1">
         <v>45165</v>
@@ -3588,13 +3696,13 @@
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B116" s="1">
         <v>45239</v>
       </c>
       <c r="C116" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D116">
         <v>1</v>
@@ -3606,18 +3714,18 @@
         <v>7</v>
       </c>
       <c r="G116" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B117" s="1">
         <v>45239</v>
       </c>
       <c r="C117" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D117">
         <v>1</v>
@@ -3629,18 +3737,18 @@
         <v>8</v>
       </c>
       <c r="G117" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B118" s="1">
         <v>45241</v>
       </c>
       <c r="C118" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D118">
         <v>2</v>
@@ -3652,18 +3760,18 @@
         <v>7</v>
       </c>
       <c r="G118" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B119" s="1">
         <v>45241</v>
       </c>
       <c r="C119" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D119">
         <v>2</v>
@@ -3675,18 +3783,18 @@
         <v>8</v>
       </c>
       <c r="G119" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B120" s="1">
         <v>45242</v>
       </c>
       <c r="C120" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D120">
         <v>3</v>
@@ -3698,18 +3806,18 @@
         <v>7</v>
       </c>
       <c r="G120" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B121" s="1">
         <v>45242</v>
       </c>
       <c r="C121" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D121">
         <v>3</v>
@@ -3721,18 +3829,18 @@
         <v>8</v>
       </c>
       <c r="G121" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B122" s="1">
         <v>45247</v>
       </c>
       <c r="C122" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D122">
         <v>1</v>
@@ -3744,18 +3852,18 @@
         <v>7</v>
       </c>
       <c r="G122" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B123" s="1">
         <v>45247</v>
       </c>
       <c r="C123" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D123">
         <v>1</v>
@@ -3767,18 +3875,18 @@
         <v>8</v>
       </c>
       <c r="G123" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B124" s="1">
         <v>45249</v>
       </c>
       <c r="C124" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D124">
         <v>2</v>
@@ -3790,18 +3898,18 @@
         <v>7</v>
       </c>
       <c r="G124" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B125" s="1">
         <v>45249</v>
       </c>
       <c r="C125" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D125">
         <v>2</v>
@@ -3813,18 +3921,18 @@
         <v>8</v>
       </c>
       <c r="G125" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B126" s="1">
         <v>45250</v>
       </c>
       <c r="C126" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D126">
         <v>3</v>
@@ -3836,18 +3944,18 @@
         <v>7</v>
       </c>
       <c r="G126" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B127" s="1">
         <v>45250</v>
       </c>
       <c r="C127" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D127">
         <v>3</v>
@@ -3859,18 +3967,18 @@
         <v>8</v>
       </c>
       <c r="G127" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B128" s="1">
         <v>45254</v>
       </c>
       <c r="C128" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D128">
         <v>1</v>
@@ -3882,18 +3990,18 @@
         <v>7</v>
       </c>
       <c r="G128" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B129" s="1">
         <v>45254</v>
       </c>
       <c r="C129" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D129">
         <v>1</v>
@@ -3905,18 +4013,18 @@
         <v>8</v>
       </c>
       <c r="G129" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B130" s="1">
         <v>45255</v>
       </c>
       <c r="C130" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D130">
         <v>2</v>
@@ -3928,18 +4036,18 @@
         <v>7</v>
       </c>
       <c r="G130" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B131" s="1">
         <v>45255</v>
       </c>
       <c r="C131" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D131">
         <v>2</v>
@@ -3951,18 +4059,18 @@
         <v>8</v>
       </c>
       <c r="G131" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B132" s="1">
         <v>45256</v>
       </c>
       <c r="C132" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D132">
         <v>3</v>
@@ -3974,18 +4082,18 @@
         <v>7</v>
       </c>
       <c r="G132" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B133" s="1">
         <v>45256</v>
       </c>
       <c r="C133" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D133">
         <v>3</v>
@@ -3997,7 +4105,2933 @@
         <v>8</v>
       </c>
       <c r="G133" t="s">
-        <v>162</v>
+        <v>161</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>167</v>
+      </c>
+      <c r="B134" s="1">
+        <v>45329</v>
+      </c>
+      <c r="C134" t="s">
+        <v>168</v>
+      </c>
+      <c r="D134">
+        <v>1</v>
+      </c>
+      <c r="E134" t="s">
+        <v>144</v>
+      </c>
+      <c r="F134" t="s">
+        <v>7</v>
+      </c>
+      <c r="G134" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>167</v>
+      </c>
+      <c r="B135" s="1">
+        <v>45329</v>
+      </c>
+      <c r="C135" t="s">
+        <v>168</v>
+      </c>
+      <c r="D135">
+        <v>1</v>
+      </c>
+      <c r="E135" t="s">
+        <v>144</v>
+      </c>
+      <c r="F135" t="s">
+        <v>8</v>
+      </c>
+      <c r="G135" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>167</v>
+      </c>
+      <c r="B136" s="1">
+        <v>45330</v>
+      </c>
+      <c r="C136" t="s">
+        <v>168</v>
+      </c>
+      <c r="D136">
+        <v>2</v>
+      </c>
+      <c r="E136" t="s">
+        <v>143</v>
+      </c>
+      <c r="F136" t="s">
+        <v>7</v>
+      </c>
+      <c r="G136" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>167</v>
+      </c>
+      <c r="B137" s="1">
+        <v>45330</v>
+      </c>
+      <c r="C137" t="s">
+        <v>168</v>
+      </c>
+      <c r="D137">
+        <v>2</v>
+      </c>
+      <c r="E137" t="s">
+        <v>143</v>
+      </c>
+      <c r="F137" t="s">
+        <v>8</v>
+      </c>
+      <c r="G137" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>167</v>
+      </c>
+      <c r="B138" s="1">
+        <v>45331</v>
+      </c>
+      <c r="C138" t="s">
+        <v>168</v>
+      </c>
+      <c r="D138">
+        <v>3</v>
+      </c>
+      <c r="E138" t="s">
+        <v>141</v>
+      </c>
+      <c r="F138" t="s">
+        <v>7</v>
+      </c>
+      <c r="G138" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>167</v>
+      </c>
+      <c r="B139" s="1">
+        <v>45331</v>
+      </c>
+      <c r="C139" t="s">
+        <v>168</v>
+      </c>
+      <c r="D139">
+        <v>3</v>
+      </c>
+      <c r="E139" t="s">
+        <v>141</v>
+      </c>
+      <c r="F139" t="s">
+        <v>8</v>
+      </c>
+      <c r="G139" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>167</v>
+      </c>
+      <c r="B140" s="1">
+        <v>45332</v>
+      </c>
+      <c r="C140" t="s">
+        <v>168</v>
+      </c>
+      <c r="D140">
+        <v>4</v>
+      </c>
+      <c r="F140" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>167</v>
+      </c>
+      <c r="B141" s="1">
+        <v>45332</v>
+      </c>
+      <c r="C141" t="s">
+        <v>168</v>
+      </c>
+      <c r="D141">
+        <v>4</v>
+      </c>
+      <c r="F141" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>167</v>
+      </c>
+      <c r="B142" s="1">
+        <v>45338</v>
+      </c>
+      <c r="C142" t="s">
+        <v>169</v>
+      </c>
+      <c r="D142">
+        <v>1</v>
+      </c>
+      <c r="F142" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>167</v>
+      </c>
+      <c r="B143" s="1">
+        <v>45338</v>
+      </c>
+      <c r="C143" t="s">
+        <v>169</v>
+      </c>
+      <c r="D143">
+        <v>1</v>
+      </c>
+      <c r="F143" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>167</v>
+      </c>
+      <c r="B144" s="1">
+        <v>45339</v>
+      </c>
+      <c r="C144" t="s">
+        <v>169</v>
+      </c>
+      <c r="D144">
+        <v>2</v>
+      </c>
+      <c r="F144" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>167</v>
+      </c>
+      <c r="B145" s="1">
+        <v>45339</v>
+      </c>
+      <c r="C145" t="s">
+        <v>169</v>
+      </c>
+      <c r="D145">
+        <v>2</v>
+      </c>
+      <c r="F145" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>167</v>
+      </c>
+      <c r="B146" s="1">
+        <v>45340</v>
+      </c>
+      <c r="C146" t="s">
+        <v>169</v>
+      </c>
+      <c r="D146">
+        <v>3</v>
+      </c>
+      <c r="F146" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>167</v>
+      </c>
+      <c r="B147" s="1">
+        <v>45340</v>
+      </c>
+      <c r="C147" t="s">
+        <v>169</v>
+      </c>
+      <c r="D147">
+        <v>3</v>
+      </c>
+      <c r="F147" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>167</v>
+      </c>
+      <c r="B148" s="1">
+        <v>45345</v>
+      </c>
+      <c r="C148" t="s">
+        <v>170</v>
+      </c>
+      <c r="D148">
+        <v>1</v>
+      </c>
+      <c r="F148" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>167</v>
+      </c>
+      <c r="B149" s="1">
+        <v>45345</v>
+      </c>
+      <c r="C149" t="s">
+        <v>170</v>
+      </c>
+      <c r="D149">
+        <v>1</v>
+      </c>
+      <c r="F149" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>167</v>
+      </c>
+      <c r="B150" s="1">
+        <v>45346</v>
+      </c>
+      <c r="C150" t="s">
+        <v>170</v>
+      </c>
+      <c r="D150">
+        <v>2</v>
+      </c>
+      <c r="F150" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>167</v>
+      </c>
+      <c r="B151" s="1">
+        <v>45346</v>
+      </c>
+      <c r="C151" t="s">
+        <v>170</v>
+      </c>
+      <c r="D151">
+        <v>2</v>
+      </c>
+      <c r="F151" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>167</v>
+      </c>
+      <c r="B152" s="1">
+        <v>45347</v>
+      </c>
+      <c r="C152" t="s">
+        <v>170</v>
+      </c>
+      <c r="D152">
+        <v>3</v>
+      </c>
+      <c r="F152" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
+        <v>167</v>
+      </c>
+      <c r="B153" s="1">
+        <v>45347</v>
+      </c>
+      <c r="C153" t="s">
+        <v>170</v>
+      </c>
+      <c r="D153">
+        <v>3</v>
+      </c>
+      <c r="F153" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
+        <v>167</v>
+      </c>
+      <c r="B154" s="1">
+        <v>45348</v>
+      </c>
+      <c r="C154" t="s">
+        <v>170</v>
+      </c>
+      <c r="D154">
+        <v>4</v>
+      </c>
+      <c r="F154" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
+        <v>167</v>
+      </c>
+      <c r="B155" s="1">
+        <v>45348</v>
+      </c>
+      <c r="C155" t="s">
+        <v>170</v>
+      </c>
+      <c r="D155">
+        <v>4</v>
+      </c>
+      <c r="F155" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
+        <v>167</v>
+      </c>
+      <c r="B156" s="1">
+        <v>45353</v>
+      </c>
+      <c r="C156" t="s">
+        <v>171</v>
+      </c>
+      <c r="D156">
+        <v>1</v>
+      </c>
+      <c r="F156" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>167</v>
+      </c>
+      <c r="B157" s="1">
+        <v>45353</v>
+      </c>
+      <c r="C157" t="s">
+        <v>171</v>
+      </c>
+      <c r="D157">
+        <v>1</v>
+      </c>
+      <c r="F157" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
+        <v>167</v>
+      </c>
+      <c r="B158" s="1">
+        <v>45354</v>
+      </c>
+      <c r="C158" t="s">
+        <v>171</v>
+      </c>
+      <c r="D158">
+        <v>2</v>
+      </c>
+      <c r="F158" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
+        <v>167</v>
+      </c>
+      <c r="B159" s="1">
+        <v>45354</v>
+      </c>
+      <c r="C159" t="s">
+        <v>171</v>
+      </c>
+      <c r="D159">
+        <v>2</v>
+      </c>
+      <c r="F159" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>167</v>
+      </c>
+      <c r="B160" s="1">
+        <v>45355</v>
+      </c>
+      <c r="C160" t="s">
+        <v>171</v>
+      </c>
+      <c r="D160">
+        <v>3</v>
+      </c>
+      <c r="F160" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
+        <v>167</v>
+      </c>
+      <c r="B161" s="1">
+        <v>45355</v>
+      </c>
+      <c r="C161" t="s">
+        <v>171</v>
+      </c>
+      <c r="D161">
+        <v>3</v>
+      </c>
+      <c r="F161" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
+        <v>167</v>
+      </c>
+      <c r="B162" s="1">
+        <v>45358</v>
+      </c>
+      <c r="C162" t="s">
+        <v>171</v>
+      </c>
+      <c r="D162">
+        <v>4</v>
+      </c>
+      <c r="F162" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
+        <v>167</v>
+      </c>
+      <c r="B163" s="1">
+        <v>45358</v>
+      </c>
+      <c r="C163" t="s">
+        <v>171</v>
+      </c>
+      <c r="D163">
+        <v>4</v>
+      </c>
+      <c r="F163" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A164" t="s">
+        <v>167</v>
+      </c>
+      <c r="B164" s="1">
+        <v>45359</v>
+      </c>
+      <c r="C164" t="s">
+        <v>171</v>
+      </c>
+      <c r="D164">
+        <v>5</v>
+      </c>
+      <c r="F164" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A165" t="s">
+        <v>167</v>
+      </c>
+      <c r="B165" s="1">
+        <v>45359</v>
+      </c>
+      <c r="C165" t="s">
+        <v>171</v>
+      </c>
+      <c r="D165">
+        <v>5</v>
+      </c>
+      <c r="F165" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A166" t="s">
+        <v>167</v>
+      </c>
+      <c r="B166" s="1">
+        <v>45360</v>
+      </c>
+      <c r="C166" t="s">
+        <v>171</v>
+      </c>
+      <c r="D166">
+        <v>6</v>
+      </c>
+      <c r="F166" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
+        <v>167</v>
+      </c>
+      <c r="B167" s="1">
+        <v>45360</v>
+      </c>
+      <c r="C167" t="s">
+        <v>171</v>
+      </c>
+      <c r="D167">
+        <v>6</v>
+      </c>
+      <c r="F167" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A168" t="s">
+        <v>199</v>
+      </c>
+      <c r="B168" s="2">
+        <v>45421</v>
+      </c>
+      <c r="C168" t="s">
+        <v>177</v>
+      </c>
+      <c r="D168">
+        <v>1</v>
+      </c>
+      <c r="F168" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A169" t="s">
+        <v>199</v>
+      </c>
+      <c r="B169" s="2">
+        <v>45421</v>
+      </c>
+      <c r="C169" t="s">
+        <v>177</v>
+      </c>
+      <c r="D169">
+        <v>1</v>
+      </c>
+      <c r="F169" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A170" t="s">
+        <v>199</v>
+      </c>
+      <c r="B170" s="2">
+        <v>45422</v>
+      </c>
+      <c r="C170" t="s">
+        <v>177</v>
+      </c>
+      <c r="D170">
+        <v>2</v>
+      </c>
+      <c r="F170" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A171" t="s">
+        <v>199</v>
+      </c>
+      <c r="B171" s="2">
+        <v>45422</v>
+      </c>
+      <c r="C171" t="s">
+        <v>177</v>
+      </c>
+      <c r="D171">
+        <v>2</v>
+      </c>
+      <c r="F171" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A172" t="s">
+        <v>199</v>
+      </c>
+      <c r="B172" s="2">
+        <v>45423</v>
+      </c>
+      <c r="C172" t="s">
+        <v>177</v>
+      </c>
+      <c r="D172">
+        <v>3</v>
+      </c>
+      <c r="F172" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A173" t="s">
+        <v>199</v>
+      </c>
+      <c r="B173" s="2">
+        <v>45423</v>
+      </c>
+      <c r="C173" t="s">
+        <v>177</v>
+      </c>
+      <c r="D173">
+        <v>3</v>
+      </c>
+      <c r="F173" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A174" t="s">
+        <v>199</v>
+      </c>
+      <c r="B174" s="2">
+        <v>45424</v>
+      </c>
+      <c r="C174" t="s">
+        <v>177</v>
+      </c>
+      <c r="D174">
+        <v>4</v>
+      </c>
+      <c r="F174" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A175" t="s">
+        <v>199</v>
+      </c>
+      <c r="B175" s="2">
+        <v>45424</v>
+      </c>
+      <c r="C175" t="s">
+        <v>177</v>
+      </c>
+      <c r="D175">
+        <v>4</v>
+      </c>
+      <c r="F175" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A176" t="s">
+        <v>199</v>
+      </c>
+      <c r="B176" s="2">
+        <v>45429</v>
+      </c>
+      <c r="C176" t="s">
+        <v>178</v>
+      </c>
+      <c r="D176">
+        <v>1</v>
+      </c>
+      <c r="F176" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A177" t="s">
+        <v>199</v>
+      </c>
+      <c r="B177" s="2">
+        <v>45429</v>
+      </c>
+      <c r="C177" t="s">
+        <v>178</v>
+      </c>
+      <c r="D177">
+        <v>1</v>
+      </c>
+      <c r="F177" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A178" t="s">
+        <v>199</v>
+      </c>
+      <c r="B178" s="2">
+        <v>45430</v>
+      </c>
+      <c r="C178" t="s">
+        <v>178</v>
+      </c>
+      <c r="D178">
+        <v>2</v>
+      </c>
+      <c r="F178" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A179" t="s">
+        <v>199</v>
+      </c>
+      <c r="B179" s="2">
+        <v>45430</v>
+      </c>
+      <c r="C179" t="s">
+        <v>178</v>
+      </c>
+      <c r="D179">
+        <v>2</v>
+      </c>
+      <c r="F179" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A180" t="s">
+        <v>199</v>
+      </c>
+      <c r="B180" s="2">
+        <v>45431</v>
+      </c>
+      <c r="C180" t="s">
+        <v>178</v>
+      </c>
+      <c r="D180">
+        <v>3</v>
+      </c>
+      <c r="F180" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A181" t="s">
+        <v>199</v>
+      </c>
+      <c r="B181" s="2">
+        <v>45431</v>
+      </c>
+      <c r="C181" t="s">
+        <v>178</v>
+      </c>
+      <c r="D181">
+        <v>3</v>
+      </c>
+      <c r="F181" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A182" t="s">
+        <v>199</v>
+      </c>
+      <c r="B182" s="2">
+        <v>45436</v>
+      </c>
+      <c r="C182" t="s">
+        <v>179</v>
+      </c>
+      <c r="D182">
+        <v>1</v>
+      </c>
+      <c r="F182" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A183" t="s">
+        <v>199</v>
+      </c>
+      <c r="B183" s="2">
+        <v>45436</v>
+      </c>
+      <c r="C183" t="s">
+        <v>179</v>
+      </c>
+      <c r="D183">
+        <v>1</v>
+      </c>
+      <c r="F183" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A184" t="s">
+        <v>199</v>
+      </c>
+      <c r="B184" s="2">
+        <v>45437</v>
+      </c>
+      <c r="C184" t="s">
+        <v>179</v>
+      </c>
+      <c r="D184">
+        <v>2</v>
+      </c>
+      <c r="F184" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A185" t="s">
+        <v>199</v>
+      </c>
+      <c r="B185" s="2">
+        <v>45437</v>
+      </c>
+      <c r="C185" t="s">
+        <v>179</v>
+      </c>
+      <c r="D185">
+        <v>2</v>
+      </c>
+      <c r="F185" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A186" t="s">
+        <v>199</v>
+      </c>
+      <c r="B186" s="2">
+        <v>45442</v>
+      </c>
+      <c r="C186" t="s">
+        <v>180</v>
+      </c>
+      <c r="D186">
+        <v>1</v>
+      </c>
+      <c r="F186" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A187" t="s">
+        <v>199</v>
+      </c>
+      <c r="B187" s="2">
+        <v>45442</v>
+      </c>
+      <c r="C187" t="s">
+        <v>180</v>
+      </c>
+      <c r="D187">
+        <v>1</v>
+      </c>
+      <c r="F187" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A188" t="s">
+        <v>199</v>
+      </c>
+      <c r="B188" s="2">
+        <v>45445</v>
+      </c>
+      <c r="C188" t="s">
+        <v>181</v>
+      </c>
+      <c r="D188">
+        <v>1</v>
+      </c>
+      <c r="F188" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A189" t="s">
+        <v>199</v>
+      </c>
+      <c r="B189" s="2">
+        <v>45445</v>
+      </c>
+      <c r="C189" t="s">
+        <v>181</v>
+      </c>
+      <c r="D189">
+        <v>1</v>
+      </c>
+      <c r="F189" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A190" t="s">
+        <v>199</v>
+      </c>
+      <c r="B190" s="2">
+        <v>45446</v>
+      </c>
+      <c r="C190" t="s">
+        <v>181</v>
+      </c>
+      <c r="D190">
+        <v>2</v>
+      </c>
+      <c r="F190" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A191" t="s">
+        <v>199</v>
+      </c>
+      <c r="B191" s="2">
+        <v>45446</v>
+      </c>
+      <c r="C191" t="s">
+        <v>181</v>
+      </c>
+      <c r="D191">
+        <v>2</v>
+      </c>
+      <c r="F191" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A192" t="s">
+        <v>199</v>
+      </c>
+      <c r="B192" s="2">
+        <v>45450</v>
+      </c>
+      <c r="C192" t="s">
+        <v>182</v>
+      </c>
+      <c r="D192">
+        <v>1</v>
+      </c>
+      <c r="F192" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A193" t="s">
+        <v>199</v>
+      </c>
+      <c r="B193" s="2">
+        <v>45450</v>
+      </c>
+      <c r="C193" t="s">
+        <v>182</v>
+      </c>
+      <c r="D193">
+        <v>1</v>
+      </c>
+      <c r="F193" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A194" t="s">
+        <v>199</v>
+      </c>
+      <c r="B194" s="2">
+        <v>45451</v>
+      </c>
+      <c r="C194" t="s">
+        <v>182</v>
+      </c>
+      <c r="D194">
+        <v>2</v>
+      </c>
+      <c r="F194" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A195" t="s">
+        <v>199</v>
+      </c>
+      <c r="B195" s="2">
+        <v>45451</v>
+      </c>
+      <c r="C195" t="s">
+        <v>182</v>
+      </c>
+      <c r="D195">
+        <v>2</v>
+      </c>
+      <c r="F195" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A196" t="s">
+        <v>199</v>
+      </c>
+      <c r="B196" s="2">
+        <v>45452</v>
+      </c>
+      <c r="C196" t="s">
+        <v>182</v>
+      </c>
+      <c r="D196">
+        <v>3</v>
+      </c>
+      <c r="F196" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A197" t="s">
+        <v>199</v>
+      </c>
+      <c r="B197" s="2">
+        <v>45452</v>
+      </c>
+      <c r="C197" t="s">
+        <v>182</v>
+      </c>
+      <c r="D197">
+        <v>3</v>
+      </c>
+      <c r="F197" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A198" t="s">
+        <v>199</v>
+      </c>
+      <c r="B198" s="2">
+        <v>45456</v>
+      </c>
+      <c r="C198" t="s">
+        <v>183</v>
+      </c>
+      <c r="D198">
+        <v>1</v>
+      </c>
+      <c r="F198" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A199" t="s">
+        <v>199</v>
+      </c>
+      <c r="B199" s="2">
+        <v>45456</v>
+      </c>
+      <c r="C199" t="s">
+        <v>183</v>
+      </c>
+      <c r="D199">
+        <v>1</v>
+      </c>
+      <c r="F199" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A200" t="s">
+        <v>199</v>
+      </c>
+      <c r="B200" s="2">
+        <v>45457</v>
+      </c>
+      <c r="C200" t="s">
+        <v>183</v>
+      </c>
+      <c r="D200">
+        <v>2</v>
+      </c>
+      <c r="F200" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A201" t="s">
+        <v>199</v>
+      </c>
+      <c r="B201" s="2">
+        <v>45457</v>
+      </c>
+      <c r="C201" t="s">
+        <v>183</v>
+      </c>
+      <c r="D201">
+        <v>2</v>
+      </c>
+      <c r="F201" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A202" t="s">
+        <v>199</v>
+      </c>
+      <c r="B202" s="2">
+        <v>45458</v>
+      </c>
+      <c r="C202" t="s">
+        <v>183</v>
+      </c>
+      <c r="D202">
+        <v>3</v>
+      </c>
+      <c r="F202" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A203" t="s">
+        <v>199</v>
+      </c>
+      <c r="B203" s="2">
+        <v>45458</v>
+      </c>
+      <c r="C203" t="s">
+        <v>183</v>
+      </c>
+      <c r="D203">
+        <v>3</v>
+      </c>
+      <c r="F203" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A204" t="s">
+        <v>199</v>
+      </c>
+      <c r="B204" s="2">
+        <v>45461</v>
+      </c>
+      <c r="C204" t="s">
+        <v>184</v>
+      </c>
+      <c r="D204">
+        <v>1</v>
+      </c>
+      <c r="F204" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A205" t="s">
+        <v>199</v>
+      </c>
+      <c r="B205" s="2">
+        <v>45461</v>
+      </c>
+      <c r="C205" t="s">
+        <v>184</v>
+      </c>
+      <c r="D205">
+        <v>1</v>
+      </c>
+      <c r="F205" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A206" t="s">
+        <v>199</v>
+      </c>
+      <c r="B206" s="2">
+        <v>45464</v>
+      </c>
+      <c r="C206" t="s">
+        <v>185</v>
+      </c>
+      <c r="D206">
+        <v>1</v>
+      </c>
+      <c r="F206" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A207" t="s">
+        <v>199</v>
+      </c>
+      <c r="B207" s="2">
+        <v>45464</v>
+      </c>
+      <c r="C207" t="s">
+        <v>185</v>
+      </c>
+      <c r="D207">
+        <v>1</v>
+      </c>
+      <c r="F207" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A208" t="s">
+        <v>199</v>
+      </c>
+      <c r="B208" s="2">
+        <v>45465</v>
+      </c>
+      <c r="C208" t="s">
+        <v>185</v>
+      </c>
+      <c r="D208">
+        <v>2</v>
+      </c>
+      <c r="F208" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A209" t="s">
+        <v>199</v>
+      </c>
+      <c r="B209" s="2">
+        <v>45465</v>
+      </c>
+      <c r="C209" t="s">
+        <v>185</v>
+      </c>
+      <c r="D209">
+        <v>2</v>
+      </c>
+      <c r="F209" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A210" t="s">
+        <v>199</v>
+      </c>
+      <c r="B210" s="2">
+        <v>45466</v>
+      </c>
+      <c r="C210" t="s">
+        <v>185</v>
+      </c>
+      <c r="D210">
+        <v>3</v>
+      </c>
+      <c r="F210" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A211" t="s">
+        <v>199</v>
+      </c>
+      <c r="B211" s="2">
+        <v>45466</v>
+      </c>
+      <c r="C211" t="s">
+        <v>185</v>
+      </c>
+      <c r="D211">
+        <v>3</v>
+      </c>
+      <c r="F211" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A212" t="s">
+        <v>199</v>
+      </c>
+      <c r="B212" s="2">
+        <v>45471</v>
+      </c>
+      <c r="C212" t="s">
+        <v>186</v>
+      </c>
+      <c r="D212">
+        <v>1</v>
+      </c>
+      <c r="F212" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A213" t="s">
+        <v>199</v>
+      </c>
+      <c r="B213" s="2">
+        <v>45471</v>
+      </c>
+      <c r="C213" t="s">
+        <v>186</v>
+      </c>
+      <c r="D213">
+        <v>1</v>
+      </c>
+      <c r="F213" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A214" t="s">
+        <v>199</v>
+      </c>
+      <c r="B214" s="2">
+        <v>45472</v>
+      </c>
+      <c r="C214" t="s">
+        <v>186</v>
+      </c>
+      <c r="D214">
+        <v>2</v>
+      </c>
+      <c r="F214" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A215" t="s">
+        <v>199</v>
+      </c>
+      <c r="B215" s="2">
+        <v>45472</v>
+      </c>
+      <c r="C215" t="s">
+        <v>186</v>
+      </c>
+      <c r="D215">
+        <v>2</v>
+      </c>
+      <c r="F215" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A216" t="s">
+        <v>199</v>
+      </c>
+      <c r="B216" s="2">
+        <v>45473</v>
+      </c>
+      <c r="C216" t="s">
+        <v>186</v>
+      </c>
+      <c r="D216">
+        <v>3</v>
+      </c>
+      <c r="F216" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A217" t="s">
+        <v>199</v>
+      </c>
+      <c r="B217" s="2">
+        <v>45473</v>
+      </c>
+      <c r="C217" t="s">
+        <v>186</v>
+      </c>
+      <c r="D217">
+        <v>3</v>
+      </c>
+      <c r="F217" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A218" t="s">
+        <v>199</v>
+      </c>
+      <c r="B218" s="2">
+        <v>45477</v>
+      </c>
+      <c r="C218" t="s">
+        <v>187</v>
+      </c>
+      <c r="D218">
+        <v>1</v>
+      </c>
+      <c r="F218" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A219" t="s">
+        <v>199</v>
+      </c>
+      <c r="B219" s="2">
+        <v>45477</v>
+      </c>
+      <c r="C219" t="s">
+        <v>187</v>
+      </c>
+      <c r="D219">
+        <v>1</v>
+      </c>
+      <c r="F219" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A220" t="s">
+        <v>199</v>
+      </c>
+      <c r="B220" s="2">
+        <v>45478</v>
+      </c>
+      <c r="C220" t="s">
+        <v>187</v>
+      </c>
+      <c r="D220">
+        <v>2</v>
+      </c>
+      <c r="F220" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A221" t="s">
+        <v>199</v>
+      </c>
+      <c r="B221" s="2">
+        <v>45478</v>
+      </c>
+      <c r="C221" t="s">
+        <v>187</v>
+      </c>
+      <c r="D221">
+        <v>2</v>
+      </c>
+      <c r="F221" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A222" t="s">
+        <v>199</v>
+      </c>
+      <c r="B222" s="2">
+        <v>45479</v>
+      </c>
+      <c r="C222" t="s">
+        <v>187</v>
+      </c>
+      <c r="D222">
+        <v>3</v>
+      </c>
+      <c r="F222" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A223" t="s">
+        <v>199</v>
+      </c>
+      <c r="B223" s="2">
+        <v>45479</v>
+      </c>
+      <c r="C223" t="s">
+        <v>187</v>
+      </c>
+      <c r="D223">
+        <v>3</v>
+      </c>
+      <c r="F223" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A224" t="s">
+        <v>199</v>
+      </c>
+      <c r="B224" s="2">
+        <v>45482</v>
+      </c>
+      <c r="C224" t="s">
+        <v>200</v>
+      </c>
+      <c r="D224">
+        <v>1</v>
+      </c>
+      <c r="F224" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="225" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A225" t="s">
+        <v>199</v>
+      </c>
+      <c r="B225" s="2">
+        <v>45482</v>
+      </c>
+      <c r="C225" t="s">
+        <v>200</v>
+      </c>
+      <c r="D225">
+        <v>1</v>
+      </c>
+      <c r="F225" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A226" t="s">
+        <v>199</v>
+      </c>
+      <c r="B226" s="2">
+        <v>45483</v>
+      </c>
+      <c r="C226" t="s">
+        <v>200</v>
+      </c>
+      <c r="D226">
+        <v>2</v>
+      </c>
+      <c r="F226" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A227" t="s">
+        <v>199</v>
+      </c>
+      <c r="B227" s="2">
+        <v>45483</v>
+      </c>
+      <c r="C227" t="s">
+        <v>200</v>
+      </c>
+      <c r="D227">
+        <v>2</v>
+      </c>
+      <c r="F227" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="228" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A228" t="s">
+        <v>199</v>
+      </c>
+      <c r="B228" s="2">
+        <v>45486</v>
+      </c>
+      <c r="C228" t="s">
+        <v>188</v>
+      </c>
+      <c r="D228">
+        <v>1</v>
+      </c>
+      <c r="F228" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A229" t="s">
+        <v>199</v>
+      </c>
+      <c r="B229" s="2">
+        <v>45486</v>
+      </c>
+      <c r="C229" t="s">
+        <v>188</v>
+      </c>
+      <c r="D229">
+        <v>1</v>
+      </c>
+      <c r="F229" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A230" t="s">
+        <v>199</v>
+      </c>
+      <c r="B230" s="2">
+        <v>45487</v>
+      </c>
+      <c r="C230" t="s">
+        <v>188</v>
+      </c>
+      <c r="D230">
+        <v>2</v>
+      </c>
+      <c r="F230" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A231" t="s">
+        <v>199</v>
+      </c>
+      <c r="B231" s="2">
+        <v>45487</v>
+      </c>
+      <c r="C231" t="s">
+        <v>188</v>
+      </c>
+      <c r="D231">
+        <v>2</v>
+      </c>
+      <c r="F231" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="232" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A232" t="s">
+        <v>199</v>
+      </c>
+      <c r="B232" s="2">
+        <v>45490</v>
+      </c>
+      <c r="C232" t="s">
+        <v>189</v>
+      </c>
+      <c r="D232">
+        <v>1</v>
+      </c>
+      <c r="F232" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="233" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A233" t="s">
+        <v>199</v>
+      </c>
+      <c r="B233" s="2">
+        <v>45490</v>
+      </c>
+      <c r="C233" t="s">
+        <v>189</v>
+      </c>
+      <c r="D233">
+        <v>1</v>
+      </c>
+      <c r="F233" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="234" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A234" t="s">
+        <v>199</v>
+      </c>
+      <c r="B234" s="2">
+        <v>45491</v>
+      </c>
+      <c r="C234" t="s">
+        <v>189</v>
+      </c>
+      <c r="D234">
+        <v>2</v>
+      </c>
+      <c r="F234" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="235" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A235" t="s">
+        <v>199</v>
+      </c>
+      <c r="B235" s="2">
+        <v>45491</v>
+      </c>
+      <c r="C235" t="s">
+        <v>189</v>
+      </c>
+      <c r="D235">
+        <v>2</v>
+      </c>
+      <c r="F235" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="236" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A236" t="s">
+        <v>199</v>
+      </c>
+      <c r="B236" s="2">
+        <v>45492</v>
+      </c>
+      <c r="C236" t="s">
+        <v>189</v>
+      </c>
+      <c r="D236">
+        <v>3</v>
+      </c>
+      <c r="F236" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="237" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A237" t="s">
+        <v>199</v>
+      </c>
+      <c r="B237" s="2">
+        <v>45492</v>
+      </c>
+      <c r="C237" t="s">
+        <v>189</v>
+      </c>
+      <c r="D237">
+        <v>3</v>
+      </c>
+      <c r="F237" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="238" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A238" t="s">
+        <v>199</v>
+      </c>
+      <c r="B238" s="2">
+        <v>45496</v>
+      </c>
+      <c r="C238" t="s">
+        <v>190</v>
+      </c>
+      <c r="D238">
+        <v>1</v>
+      </c>
+      <c r="F238" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="239" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A239" t="s">
+        <v>199</v>
+      </c>
+      <c r="B239" s="2">
+        <v>45496</v>
+      </c>
+      <c r="C239" t="s">
+        <v>190</v>
+      </c>
+      <c r="D239">
+        <v>1</v>
+      </c>
+      <c r="F239" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="240" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A240" t="s">
+        <v>199</v>
+      </c>
+      <c r="B240" s="2">
+        <v>45497</v>
+      </c>
+      <c r="C240" t="s">
+        <v>190</v>
+      </c>
+      <c r="D240">
+        <v>2</v>
+      </c>
+      <c r="F240" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="241" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A241" t="s">
+        <v>199</v>
+      </c>
+      <c r="B241" s="2">
+        <v>45497</v>
+      </c>
+      <c r="C241" t="s">
+        <v>190</v>
+      </c>
+      <c r="D241">
+        <v>2</v>
+      </c>
+      <c r="F241" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="242" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A242" t="s">
+        <v>199</v>
+      </c>
+      <c r="B242" s="2">
+        <v>45500</v>
+      </c>
+      <c r="C242" t="s">
+        <v>191</v>
+      </c>
+      <c r="D242">
+        <v>1</v>
+      </c>
+      <c r="F242" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="243" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A243" t="s">
+        <v>199</v>
+      </c>
+      <c r="B243" s="2">
+        <v>45500</v>
+      </c>
+      <c r="C243" t="s">
+        <v>191</v>
+      </c>
+      <c r="D243">
+        <v>1</v>
+      </c>
+      <c r="F243" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="244" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A244" t="s">
+        <v>199</v>
+      </c>
+      <c r="B244" s="2">
+        <v>45501</v>
+      </c>
+      <c r="C244" t="s">
+        <v>191</v>
+      </c>
+      <c r="D244">
+        <v>2</v>
+      </c>
+      <c r="F244" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="245" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A245" t="s">
+        <v>199</v>
+      </c>
+      <c r="B245" s="2">
+        <v>45501</v>
+      </c>
+      <c r="C245" t="s">
+        <v>191</v>
+      </c>
+      <c r="D245">
+        <v>2</v>
+      </c>
+      <c r="F245" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="246" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A246" t="s">
+        <v>199</v>
+      </c>
+      <c r="B246" s="2">
+        <v>45505</v>
+      </c>
+      <c r="C246" t="s">
+        <v>192</v>
+      </c>
+      <c r="D246">
+        <v>1</v>
+      </c>
+      <c r="F246" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="247" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A247" t="s">
+        <v>199</v>
+      </c>
+      <c r="B247" s="2">
+        <v>45505</v>
+      </c>
+      <c r="C247" t="s">
+        <v>192</v>
+      </c>
+      <c r="D247">
+        <v>1</v>
+      </c>
+      <c r="F247" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="248" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A248" t="s">
+        <v>199</v>
+      </c>
+      <c r="B248" s="2">
+        <v>45506</v>
+      </c>
+      <c r="C248" t="s">
+        <v>192</v>
+      </c>
+      <c r="D248">
+        <v>2</v>
+      </c>
+      <c r="F248" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="249" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A249" t="s">
+        <v>199</v>
+      </c>
+      <c r="B249" s="2">
+        <v>45506</v>
+      </c>
+      <c r="C249" t="s">
+        <v>192</v>
+      </c>
+      <c r="D249">
+        <v>2</v>
+      </c>
+      <c r="F249" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="250" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A250" t="s">
+        <v>199</v>
+      </c>
+      <c r="B250" s="2">
+        <v>45507</v>
+      </c>
+      <c r="C250" t="s">
+        <v>192</v>
+      </c>
+      <c r="D250">
+        <v>3</v>
+      </c>
+      <c r="F250" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="251" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A251" t="s">
+        <v>199</v>
+      </c>
+      <c r="B251" s="2">
+        <v>45507</v>
+      </c>
+      <c r="C251" t="s">
+        <v>192</v>
+      </c>
+      <c r="D251">
+        <v>3</v>
+      </c>
+      <c r="F251" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="252" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A252" t="s">
+        <v>199</v>
+      </c>
+      <c r="B252" s="2">
+        <v>45512</v>
+      </c>
+      <c r="C252" t="s">
+        <v>193</v>
+      </c>
+      <c r="D252">
+        <v>1</v>
+      </c>
+      <c r="F252" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="253" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A253" t="s">
+        <v>199</v>
+      </c>
+      <c r="B253" s="2">
+        <v>45512</v>
+      </c>
+      <c r="C253" t="s">
+        <v>193</v>
+      </c>
+      <c r="D253">
+        <v>1</v>
+      </c>
+      <c r="F253" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="254" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A254" t="s">
+        <v>199</v>
+      </c>
+      <c r="B254" s="2">
+        <v>45513</v>
+      </c>
+      <c r="C254" t="s">
+        <v>193</v>
+      </c>
+      <c r="D254">
+        <v>2</v>
+      </c>
+      <c r="F254" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="255" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A255" t="s">
+        <v>199</v>
+      </c>
+      <c r="B255" s="2">
+        <v>45513</v>
+      </c>
+      <c r="C255" t="s">
+        <v>193</v>
+      </c>
+      <c r="D255">
+        <v>2</v>
+      </c>
+      <c r="F255" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="256" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A256" t="s">
+        <v>199</v>
+      </c>
+      <c r="B256" s="2">
+        <v>45514</v>
+      </c>
+      <c r="C256" t="s">
+        <v>193</v>
+      </c>
+      <c r="D256">
+        <v>3</v>
+      </c>
+      <c r="F256" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="257" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A257" t="s">
+        <v>199</v>
+      </c>
+      <c r="B257" s="2">
+        <v>45514</v>
+      </c>
+      <c r="C257" t="s">
+        <v>193</v>
+      </c>
+      <c r="D257">
+        <v>3</v>
+      </c>
+      <c r="F257" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="258" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A258" t="s">
+        <v>199</v>
+      </c>
+      <c r="B258" s="2">
+        <v>45519</v>
+      </c>
+      <c r="C258" t="s">
+        <v>185</v>
+      </c>
+      <c r="D258">
+        <v>4</v>
+      </c>
+      <c r="F258" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="259" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A259" t="s">
+        <v>199</v>
+      </c>
+      <c r="B259" s="2">
+        <v>45519</v>
+      </c>
+      <c r="C259" t="s">
+        <v>185</v>
+      </c>
+      <c r="D259">
+        <v>4</v>
+      </c>
+      <c r="F259" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="260" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A260" t="s">
+        <v>199</v>
+      </c>
+      <c r="B260" s="2">
+        <v>45520</v>
+      </c>
+      <c r="C260" t="s">
+        <v>185</v>
+      </c>
+      <c r="D260">
+        <v>5</v>
+      </c>
+      <c r="F260" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="261" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A261" t="s">
+        <v>199</v>
+      </c>
+      <c r="B261" s="2">
+        <v>45520</v>
+      </c>
+      <c r="C261" t="s">
+        <v>185</v>
+      </c>
+      <c r="D261">
+        <v>5</v>
+      </c>
+      <c r="F261" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="262" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A262" t="s">
+        <v>199</v>
+      </c>
+      <c r="B262" s="2">
+        <v>45521</v>
+      </c>
+      <c r="C262" t="s">
+        <v>185</v>
+      </c>
+      <c r="D262">
+        <v>6</v>
+      </c>
+      <c r="F262" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="263" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A263" t="s">
+        <v>199</v>
+      </c>
+      <c r="B263" s="2">
+        <v>45521</v>
+      </c>
+      <c r="C263" t="s">
+        <v>185</v>
+      </c>
+      <c r="D263">
+        <v>6</v>
+      </c>
+      <c r="F263" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="264" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A264" t="s">
+        <v>199</v>
+      </c>
+      <c r="B264" s="2">
+        <v>45523</v>
+      </c>
+      <c r="C264" t="s">
+        <v>185</v>
+      </c>
+      <c r="D264">
+        <v>7</v>
+      </c>
+      <c r="F264" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="265" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A265" t="s">
+        <v>199</v>
+      </c>
+      <c r="B265" s="2">
+        <v>45523</v>
+      </c>
+      <c r="C265" t="s">
+        <v>185</v>
+      </c>
+      <c r="D265">
+        <v>7</v>
+      </c>
+      <c r="F265" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="266" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A266" t="s">
+        <v>199</v>
+      </c>
+      <c r="B266" s="2">
+        <v>45524</v>
+      </c>
+      <c r="C266" t="s">
+        <v>185</v>
+      </c>
+      <c r="D266">
+        <v>8</v>
+      </c>
+      <c r="F266" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="267" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A267" t="s">
+        <v>199</v>
+      </c>
+      <c r="B267" s="2">
+        <v>45524</v>
+      </c>
+      <c r="C267" t="s">
+        <v>185</v>
+      </c>
+      <c r="D267">
+        <v>8</v>
+      </c>
+      <c r="F267" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="268" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A268" t="s">
+        <v>202</v>
+      </c>
+      <c r="B268" s="2">
+        <v>45583</v>
+      </c>
+      <c r="C268" t="s">
+        <v>194</v>
+      </c>
+      <c r="D268">
+        <v>1</v>
+      </c>
+      <c r="F268" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="269" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A269" t="s">
+        <v>202</v>
+      </c>
+      <c r="B269" s="2">
+        <v>45583</v>
+      </c>
+      <c r="C269" t="s">
+        <v>194</v>
+      </c>
+      <c r="D269">
+        <v>1</v>
+      </c>
+      <c r="F269" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="270" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A270" t="s">
+        <v>202</v>
+      </c>
+      <c r="B270" s="2">
+        <v>45584</v>
+      </c>
+      <c r="C270" t="s">
+        <v>194</v>
+      </c>
+      <c r="D270">
+        <v>2</v>
+      </c>
+      <c r="F270" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="271" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A271" t="s">
+        <v>202</v>
+      </c>
+      <c r="B271" s="2">
+        <v>45584</v>
+      </c>
+      <c r="C271" t="s">
+        <v>194</v>
+      </c>
+      <c r="D271">
+        <v>2</v>
+      </c>
+      <c r="F271" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="272" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A272" t="s">
+        <v>202</v>
+      </c>
+      <c r="B272" s="2">
+        <v>45585</v>
+      </c>
+      <c r="C272" t="s">
+        <v>194</v>
+      </c>
+      <c r="D272">
+        <v>3</v>
+      </c>
+      <c r="F272" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="273" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A273" t="s">
+        <v>202</v>
+      </c>
+      <c r="B273" s="2">
+        <v>45585</v>
+      </c>
+      <c r="C273" t="s">
+        <v>194</v>
+      </c>
+      <c r="D273">
+        <v>3</v>
+      </c>
+      <c r="F273" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="274" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A274" t="s">
+        <v>202</v>
+      </c>
+      <c r="B274" s="2">
+        <v>45590</v>
+      </c>
+      <c r="C274" t="s">
+        <v>195</v>
+      </c>
+      <c r="D274">
+        <v>1</v>
+      </c>
+      <c r="F274" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="275" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A275" t="s">
+        <v>202</v>
+      </c>
+      <c r="B275" s="2">
+        <v>45590</v>
+      </c>
+      <c r="C275" t="s">
+        <v>195</v>
+      </c>
+      <c r="D275">
+        <v>1</v>
+      </c>
+      <c r="F275" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="276" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A276" t="s">
+        <v>202</v>
+      </c>
+      <c r="B276" s="2">
+        <v>45591</v>
+      </c>
+      <c r="C276" t="s">
+        <v>195</v>
+      </c>
+      <c r="D276">
+        <v>2</v>
+      </c>
+      <c r="F276" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="277" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A277" t="s">
+        <v>202</v>
+      </c>
+      <c r="B277" s="2">
+        <v>45591</v>
+      </c>
+      <c r="C277" t="s">
+        <v>195</v>
+      </c>
+      <c r="D277">
+        <v>2</v>
+      </c>
+      <c r="F277" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="278" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A278" t="s">
+        <v>202</v>
+      </c>
+      <c r="B278" s="2">
+        <v>45592</v>
+      </c>
+      <c r="C278" t="s">
+        <v>195</v>
+      </c>
+      <c r="D278">
+        <v>3</v>
+      </c>
+      <c r="F278" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="279" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A279" t="s">
+        <v>202</v>
+      </c>
+      <c r="B279" s="2">
+        <v>45592</v>
+      </c>
+      <c r="C279" t="s">
+        <v>195</v>
+      </c>
+      <c r="D279">
+        <v>3</v>
+      </c>
+      <c r="F279" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="280" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A280" t="s">
+        <v>202</v>
+      </c>
+      <c r="B280" s="2">
+        <v>45597</v>
+      </c>
+      <c r="C280" t="s">
+        <v>196</v>
+      </c>
+      <c r="D280">
+        <v>1</v>
+      </c>
+      <c r="F280" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="281" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A281" t="s">
+        <v>202</v>
+      </c>
+      <c r="B281" s="2">
+        <v>45597</v>
+      </c>
+      <c r="C281" t="s">
+        <v>196</v>
+      </c>
+      <c r="D281">
+        <v>1</v>
+      </c>
+      <c r="F281" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="282" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A282" t="s">
+        <v>202</v>
+      </c>
+      <c r="B282" s="2">
+        <v>45598</v>
+      </c>
+      <c r="C282" t="s">
+        <v>196</v>
+      </c>
+      <c r="D282">
+        <v>2</v>
+      </c>
+      <c r="F282" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="283" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A283" t="s">
+        <v>202</v>
+      </c>
+      <c r="B283" s="2">
+        <v>45598</v>
+      </c>
+      <c r="C283" t="s">
+        <v>196</v>
+      </c>
+      <c r="D283">
+        <v>2</v>
+      </c>
+      <c r="F283" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="284" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A284" t="s">
+        <v>202</v>
+      </c>
+      <c r="B284" s="2">
+        <v>45599</v>
+      </c>
+      <c r="C284" t="s">
+        <v>196</v>
+      </c>
+      <c r="D284">
+        <v>3</v>
+      </c>
+      <c r="F284" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="285" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A285" t="s">
+        <v>202</v>
+      </c>
+      <c r="B285" s="2">
+        <v>45599</v>
+      </c>
+      <c r="C285" t="s">
+        <v>196</v>
+      </c>
+      <c r="D285">
+        <v>3</v>
+      </c>
+      <c r="F285" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="286" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A286" t="s">
+        <v>202</v>
+      </c>
+      <c r="B286" s="2">
+        <v>45610</v>
+      </c>
+      <c r="C286" t="s">
+        <v>197</v>
+      </c>
+      <c r="D286">
+        <v>1</v>
+      </c>
+      <c r="F286" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="287" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A287" t="s">
+        <v>202</v>
+      </c>
+      <c r="B287" s="2">
+        <v>45610</v>
+      </c>
+      <c r="C287" t="s">
+        <v>197</v>
+      </c>
+      <c r="D287">
+        <v>1</v>
+      </c>
+      <c r="F287" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="288" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A288" t="s">
+        <v>202</v>
+      </c>
+      <c r="B288" s="2">
+        <v>45611</v>
+      </c>
+      <c r="C288" t="s">
+        <v>197</v>
+      </c>
+      <c r="D288">
+        <v>2</v>
+      </c>
+      <c r="F288" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="289" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A289" t="s">
+        <v>202</v>
+      </c>
+      <c r="B289" s="2">
+        <v>45611</v>
+      </c>
+      <c r="C289" t="s">
+        <v>197</v>
+      </c>
+      <c r="D289">
+        <v>2</v>
+      </c>
+      <c r="F289" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="290" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A290" t="s">
+        <v>202</v>
+      </c>
+      <c r="B290" s="2">
+        <v>45612</v>
+      </c>
+      <c r="C290" t="s">
+        <v>197</v>
+      </c>
+      <c r="D290">
+        <v>3</v>
+      </c>
+      <c r="F290" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="291" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A291" t="s">
+        <v>202</v>
+      </c>
+      <c r="B291" s="2">
+        <v>45612</v>
+      </c>
+      <c r="C291" t="s">
+        <v>197</v>
+      </c>
+      <c r="D291">
+        <v>3</v>
+      </c>
+      <c r="F291" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="292" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A292" t="s">
+        <v>202</v>
+      </c>
+      <c r="B292" s="2">
+        <v>45617</v>
+      </c>
+      <c r="C292" t="s">
+        <v>197</v>
+      </c>
+      <c r="D292">
+        <v>4</v>
+      </c>
+      <c r="F292" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="293" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A293" t="s">
+        <v>202</v>
+      </c>
+      <c r="B293" s="2">
+        <v>45617</v>
+      </c>
+      <c r="C293" t="s">
+        <v>197</v>
+      </c>
+      <c r="D293">
+        <v>4</v>
+      </c>
+      <c r="F293" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="294" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A294" t="s">
+        <v>202</v>
+      </c>
+      <c r="B294" s="2">
+        <v>45618</v>
+      </c>
+      <c r="C294" t="s">
+        <v>197</v>
+      </c>
+      <c r="D294">
+        <v>5</v>
+      </c>
+      <c r="F294" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="295" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A295" t="s">
+        <v>202</v>
+      </c>
+      <c r="B295" s="2">
+        <v>45618</v>
+      </c>
+      <c r="C295" t="s">
+        <v>197</v>
+      </c>
+      <c r="D295">
+        <v>5</v>
+      </c>
+      <c r="F295" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="296" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A296" t="s">
+        <v>202</v>
+      </c>
+      <c r="B296" s="2">
+        <v>45619</v>
+      </c>
+      <c r="C296" t="s">
+        <v>197</v>
+      </c>
+      <c r="D296">
+        <v>6</v>
+      </c>
+      <c r="F296" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="297" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A297" t="s">
+        <v>202</v>
+      </c>
+      <c r="B297" s="2">
+        <v>45619</v>
+      </c>
+      <c r="C297" t="s">
+        <v>197</v>
+      </c>
+      <c r="D297">
+        <v>6</v>
+      </c>
+      <c r="F297" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="298" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A298" t="s">
+        <v>202</v>
+      </c>
+      <c r="B298" s="2">
+        <v>45632</v>
+      </c>
+      <c r="C298" t="s">
+        <v>198</v>
+      </c>
+      <c r="D298">
+        <v>1</v>
+      </c>
+      <c r="F298" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="299" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A299" t="s">
+        <v>202</v>
+      </c>
+      <c r="B299" s="2">
+        <v>45632</v>
+      </c>
+      <c r="C299" t="s">
+        <v>198</v>
+      </c>
+      <c r="D299">
+        <v>1</v>
+      </c>
+      <c r="F299" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="300" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A300" t="s">
+        <v>202</v>
+      </c>
+      <c r="B300" s="2">
+        <v>45633</v>
+      </c>
+      <c r="C300" t="s">
+        <v>198</v>
+      </c>
+      <c r="D300">
+        <v>2</v>
+      </c>
+      <c r="F300" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="301" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A301" t="s">
+        <v>202</v>
+      </c>
+      <c r="B301" s="2">
+        <v>45633</v>
+      </c>
+      <c r="C301" t="s">
+        <v>198</v>
+      </c>
+      <c r="D301">
+        <v>2</v>
+      </c>
+      <c r="F301" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="302" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A302" t="s">
+        <v>202</v>
+      </c>
+      <c r="B302" s="2">
+        <v>45634</v>
+      </c>
+      <c r="C302" t="s">
+        <v>198</v>
+      </c>
+      <c r="D302">
+        <v>3</v>
+      </c>
+      <c r="F302" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="303" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A303" t="s">
+        <v>202</v>
+      </c>
+      <c r="B303" s="2">
+        <v>45634</v>
+      </c>
+      <c r="C303" t="s">
+        <v>198</v>
+      </c>
+      <c r="D303">
+        <v>3</v>
+      </c>
+      <c r="F303" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add melbourne surprise songs
</commit_message>
<xml_diff>
--- a/data-raw/surprise-songs.xlsx
+++ b/data-raw/surprise-songs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakethompson/Documents/GIT/packages/taylor/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41803AED-9336-9E48-A5A2-2D46F03F46E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CF5D27D-31C4-5947-BF60-1218D199693C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="15660" windowHeight="17500" xr2:uid="{23F40540-2069-D04D-A50F-51228CFC4AB9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1207" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1215" uniqueCount="207">
   <si>
     <t>date</t>
   </si>
@@ -651,6 +651,12 @@
   </si>
   <si>
     <t>You're Losing Me (From The Vault)</t>
+  </si>
+  <si>
+    <t>mashup</t>
+  </si>
+  <si>
+    <t>august; The Other Side Of The Door (Taylor's Version)</t>
   </si>
 </sst>
 </file>
@@ -1008,11 +1014,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04F0F9D9-7CA5-0C41-BC65-3D3349CBCA23}">
-  <dimension ref="A1:H303"/>
+  <dimension ref="A1:I303"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A121" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G144" sqref="G144"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H145" sqref="H145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1021,11 +1027,12 @@
     <col min="2" max="2" width="12.1640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="52.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="52.5" customWidth="1"/>
+    <col min="9" max="9" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>68</v>
       </c>
@@ -1048,10 +1055,13 @@
         <v>4</v>
       </c>
       <c r="H1" t="s">
+        <v>205</v>
+      </c>
+      <c r="I1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>201</v>
       </c>
@@ -1074,7 +1084,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>201</v>
       </c>
@@ -1097,7 +1107,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>201</v>
       </c>
@@ -1120,7 +1130,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>201</v>
       </c>
@@ -1143,7 +1153,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>201</v>
       </c>
@@ -1166,7 +1176,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>201</v>
       </c>
@@ -1189,7 +1199,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>201</v>
       </c>
@@ -1211,11 +1221,11 @@
       <c r="G8" t="s">
         <v>16</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>201</v>
       </c>
@@ -1238,7 +1248,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>201</v>
       </c>
@@ -1261,7 +1271,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>201</v>
       </c>
@@ -1284,7 +1294,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>201</v>
       </c>
@@ -1307,7 +1317,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>201</v>
       </c>
@@ -1330,7 +1340,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>201</v>
       </c>
@@ -1353,7 +1363,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>201</v>
       </c>
@@ -1376,7 +1386,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>201</v>
       </c>
@@ -1399,7 +1409,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>201</v>
       </c>
@@ -1422,7 +1432,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>201</v>
       </c>
@@ -1444,11 +1454,11 @@
       <c r="G18" t="s">
         <v>33</v>
       </c>
-      <c r="H18" t="s">
+      <c r="I18" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>201</v>
       </c>
@@ -1471,7 +1481,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>201</v>
       </c>
@@ -1493,11 +1503,11 @@
       <c r="G20" t="s">
         <v>35</v>
       </c>
-      <c r="H20" t="s">
+      <c r="I20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>201</v>
       </c>
@@ -1520,7 +1530,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>201</v>
       </c>
@@ -1543,7 +1553,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>201</v>
       </c>
@@ -1566,7 +1576,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>201</v>
       </c>
@@ -1589,7 +1599,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>201</v>
       </c>
@@ -1612,7 +1622,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>201</v>
       </c>
@@ -1635,7 +1645,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>201</v>
       </c>
@@ -1658,7 +1668,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>201</v>
       </c>
@@ -1681,7 +1691,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>201</v>
       </c>
@@ -1704,7 +1714,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>201</v>
       </c>
@@ -1727,7 +1737,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>201</v>
       </c>
@@ -1750,7 +1760,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>201</v>
       </c>
@@ -1773,7 +1783,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>201</v>
       </c>
@@ -1796,7 +1806,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>201</v>
       </c>
@@ -1819,7 +1829,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>201</v>
       </c>
@@ -1842,7 +1852,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>201</v>
       </c>
@@ -1865,7 +1875,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>201</v>
       </c>
@@ -1888,7 +1898,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>201</v>
       </c>
@@ -1910,11 +1920,11 @@
       <c r="G38" t="s">
         <v>49</v>
       </c>
-      <c r="H38" t="s">
+      <c r="I38" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>201</v>
       </c>
@@ -1937,7 +1947,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>201</v>
       </c>
@@ -1960,7 +1970,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>201</v>
       </c>
@@ -1983,7 +1993,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>201</v>
       </c>
@@ -2006,7 +2016,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>201</v>
       </c>
@@ -2029,7 +2039,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>201</v>
       </c>
@@ -2052,7 +2062,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>201</v>
       </c>
@@ -2075,7 +2085,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>201</v>
       </c>
@@ -2098,7 +2108,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>201</v>
       </c>
@@ -2121,7 +2131,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>201</v>
       </c>
@@ -2144,7 +2154,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>201</v>
       </c>
@@ -2167,7 +2177,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>201</v>
       </c>
@@ -2190,7 +2200,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>201</v>
       </c>
@@ -2213,7 +2223,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>201</v>
       </c>
@@ -2235,11 +2245,11 @@
       <c r="G52" t="s">
         <v>74</v>
       </c>
-      <c r="H52" t="s">
+      <c r="I52" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>201</v>
       </c>
@@ -2262,7 +2272,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>201</v>
       </c>
@@ -2285,7 +2295,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>201</v>
       </c>
@@ -2308,7 +2318,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>201</v>
       </c>
@@ -2331,7 +2341,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>201</v>
       </c>
@@ -2354,7 +2364,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>201</v>
       </c>
@@ -2377,7 +2387,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>201</v>
       </c>
@@ -2400,7 +2410,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>201</v>
       </c>
@@ -2422,11 +2432,11 @@
       <c r="G60" t="s">
         <v>129</v>
       </c>
-      <c r="H60" t="s">
+      <c r="I60" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>201</v>
       </c>
@@ -2449,7 +2459,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>201</v>
       </c>
@@ -2472,7 +2482,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>201</v>
       </c>
@@ -2495,7 +2505,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>201</v>
       </c>
@@ -2518,7 +2528,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>201</v>
       </c>
@@ -2541,7 +2551,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>201</v>
       </c>
@@ -2564,7 +2574,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>201</v>
       </c>
@@ -2587,7 +2597,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>201</v>
       </c>
@@ -2610,7 +2620,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>201</v>
       </c>
@@ -2633,7 +2643,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>201</v>
       </c>
@@ -2655,11 +2665,11 @@
       <c r="G70" t="s">
         <v>88</v>
       </c>
-      <c r="H70" t="s">
+      <c r="I70" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>201</v>
       </c>
@@ -2682,7 +2692,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>201</v>
       </c>
@@ -2705,7 +2715,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>201</v>
       </c>
@@ -2728,7 +2738,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>201</v>
       </c>
@@ -2751,7 +2761,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>201</v>
       </c>
@@ -2774,7 +2784,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>201</v>
       </c>
@@ -2797,7 +2807,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>201</v>
       </c>
@@ -2820,7 +2830,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>201</v>
       </c>
@@ -2842,11 +2852,11 @@
       <c r="G78" t="s">
         <v>95</v>
       </c>
-      <c r="H78" t="s">
+      <c r="I78" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>201</v>
       </c>
@@ -2869,7 +2879,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>201</v>
       </c>
@@ -2892,7 +2902,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>201</v>
       </c>
@@ -2915,7 +2925,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>201</v>
       </c>
@@ -2938,7 +2948,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>201</v>
       </c>
@@ -2961,7 +2971,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>201</v>
       </c>
@@ -2984,7 +2994,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>201</v>
       </c>
@@ -3007,7 +3017,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>201</v>
       </c>
@@ -3030,7 +3040,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>201</v>
       </c>
@@ -3053,7 +3063,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>201</v>
       </c>
@@ -3076,7 +3086,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>201</v>
       </c>
@@ -3099,7 +3109,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>201</v>
       </c>
@@ -3122,7 +3132,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>201</v>
       </c>
@@ -3145,7 +3155,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>201</v>
       </c>
@@ -3167,11 +3177,11 @@
       <c r="G92" t="s">
         <v>108</v>
       </c>
-      <c r="H92" t="s">
+      <c r="I92" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>201</v>
       </c>
@@ -3194,7 +3204,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>201</v>
       </c>
@@ -3217,7 +3227,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>201</v>
       </c>
@@ -3240,7 +3250,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>201</v>
       </c>
@@ -3631,7 +3641,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>201</v>
       </c>
@@ -3654,7 +3664,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>201</v>
       </c>
@@ -3677,7 +3687,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>201</v>
       </c>
@@ -3700,7 +3710,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>145</v>
       </c>
@@ -3723,7 +3733,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>145</v>
       </c>
@@ -3746,7 +3756,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>145</v>
       </c>
@@ -3768,8 +3778,11 @@
       <c r="G118" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H118" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>145</v>
       </c>
@@ -3792,7 +3805,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>145</v>
       </c>
@@ -3815,7 +3828,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>145</v>
       </c>
@@ -3838,7 +3851,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>145</v>
       </c>
@@ -3861,7 +3874,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>145</v>
       </c>
@@ -3884,7 +3897,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>145</v>
       </c>
@@ -3907,7 +3920,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>145</v>
       </c>
@@ -3930,7 +3943,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>145</v>
       </c>
@@ -3953,7 +3966,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>145</v>
       </c>
@@ -3976,7 +3989,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>145</v>
       </c>
@@ -3999,7 +4012,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>145</v>
       </c>
@@ -4022,7 +4035,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>145</v>
       </c>
@@ -4045,7 +4058,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>145</v>
       </c>
@@ -4068,7 +4081,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>145</v>
       </c>
@@ -4091,7 +4104,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>145</v>
       </c>
@@ -4114,7 +4127,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>167</v>
       </c>
@@ -4137,7 +4150,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>167</v>
       </c>
@@ -4160,7 +4173,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>167</v>
       </c>
@@ -4183,7 +4196,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>167</v>
       </c>
@@ -4206,7 +4219,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>167</v>
       </c>
@@ -4229,7 +4242,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>167</v>
       </c>
@@ -4252,7 +4265,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>167</v>
       </c>
@@ -4275,7 +4288,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>167</v>
       </c>
@@ -4298,7 +4311,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>167</v>
       </c>
@@ -4321,7 +4334,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>167</v>
       </c>
@@ -4344,7 +4357,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>167</v>
       </c>
@@ -4360,8 +4373,14 @@
       <c r="F144" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G144" t="s">
+        <v>74</v>
+      </c>
+      <c r="H144" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>167</v>
       </c>
@@ -4377,8 +4396,11 @@
       <c r="F145" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G145" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>167</v>
       </c>
@@ -4394,8 +4416,14 @@
       <c r="F146" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G146" t="s">
+        <v>127</v>
+      </c>
+      <c r="H146" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>167</v>
       </c>
@@ -4411,8 +4439,11 @@
       <c r="F147" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G147" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>167</v>
       </c>
@@ -4429,7 +4460,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>167</v>
       </c>
@@ -4446,7 +4477,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>167</v>
       </c>
@@ -4463,7 +4494,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>167</v>
       </c>
@@ -4480,7 +4511,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>167</v>
       </c>
@@ -4497,7 +4528,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>167</v>
       </c>
@@ -4514,7 +4545,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>167</v>
       </c>
@@ -4531,7 +4562,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>167</v>
       </c>
@@ -4548,7 +4579,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>167</v>
       </c>
@@ -4565,7 +4596,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>167</v>
       </c>
@@ -4582,7 +4613,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>167</v>
       </c>
@@ -4599,7 +4630,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>167</v>
       </c>
@@ -4616,7 +4647,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>167</v>
       </c>

</xml_diff>

<commit_message>
add singapore surprise songs
</commit_message>
<xml_diff>
--- a/data-raw/surprise-songs.xlsx
+++ b/data-raw/surprise-songs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakethompson/Documents/GIT/packages/taylor/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{327F74C9-3B39-E346-9B85-08B629F93D73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ED334C9-A159-2746-B1BA-634B22B2892F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26240" windowHeight="17500" xr2:uid="{23F40540-2069-D04D-A50F-51228CFC4AB9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1243" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1279" uniqueCount="213">
   <si>
     <t>date</t>
   </si>
@@ -663,6 +663,18 @@
   </si>
   <si>
     <t>peace</t>
+  </si>
+  <si>
+    <t>long story short</t>
+  </si>
+  <si>
+    <t>Foolish One (Taylor's Version) [From The Vault]</t>
+  </si>
+  <si>
+    <t>Babe (Taylor's Version) [From The Vault]</t>
+  </si>
+  <si>
+    <t>epiphany</t>
   </si>
 </sst>
 </file>
@@ -724,9 +736,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -764,7 +776,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -870,7 +882,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1012,7 +1024,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1023,8 +1035,8 @@
   <dimension ref="A1:I303"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H151" sqref="H151"/>
+      <pane ySplit="1" topLeftCell="A141" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G164" sqref="G164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4682,8 +4694,17 @@
       <c r="D156">
         <v>1</v>
       </c>
+      <c r="E156" t="s">
+        <v>143</v>
+      </c>
       <c r="F156" t="s">
         <v>7</v>
+      </c>
+      <c r="G156" t="s">
+        <v>50</v>
+      </c>
+      <c r="H156" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.2">
@@ -4699,8 +4720,17 @@
       <c r="D157">
         <v>1</v>
       </c>
+      <c r="E157" t="s">
+        <v>143</v>
+      </c>
       <c r="F157" t="s">
         <v>8</v>
+      </c>
+      <c r="G157" t="s">
+        <v>81</v>
+      </c>
+      <c r="H157" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.2">
@@ -4716,8 +4746,17 @@
       <c r="D158">
         <v>2</v>
       </c>
+      <c r="E158" t="s">
+        <v>142</v>
+      </c>
       <c r="F158" t="s">
         <v>7</v>
+      </c>
+      <c r="G158" t="s">
+        <v>209</v>
+      </c>
+      <c r="H158" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.2">
@@ -4733,8 +4772,17 @@
       <c r="D159">
         <v>2</v>
       </c>
+      <c r="E159" t="s">
+        <v>142</v>
+      </c>
       <c r="F159" t="s">
         <v>8</v>
+      </c>
+      <c r="G159" t="s">
+        <v>28</v>
+      </c>
+      <c r="H159" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.2">
@@ -4750,11 +4798,20 @@
       <c r="D160">
         <v>3</v>
       </c>
+      <c r="E160" t="s">
+        <v>141</v>
+      </c>
       <c r="F160" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G160" t="s">
+        <v>210</v>
+      </c>
+      <c r="H160" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>167</v>
       </c>
@@ -4767,11 +4824,20 @@
       <c r="D161">
         <v>3</v>
       </c>
+      <c r="E161" t="s">
+        <v>141</v>
+      </c>
       <c r="F161" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G161" t="s">
+        <v>53</v>
+      </c>
+      <c r="H161" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>167</v>
       </c>
@@ -4784,11 +4850,20 @@
       <c r="D162">
         <v>4</v>
       </c>
+      <c r="E162" t="s">
+        <v>141</v>
+      </c>
       <c r="F162" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G162" t="s">
+        <v>27</v>
+      </c>
+      <c r="H162" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>167</v>
       </c>
@@ -4801,11 +4876,20 @@
       <c r="D163">
         <v>4</v>
       </c>
+      <c r="E163" t="s">
+        <v>141</v>
+      </c>
       <c r="F163" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G163" t="s">
+        <v>138</v>
+      </c>
+      <c r="H163" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>167</v>
       </c>
@@ -4818,11 +4902,20 @@
       <c r="D164">
         <v>5</v>
       </c>
+      <c r="E164" t="s">
+        <v>143</v>
+      </c>
       <c r="F164" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G164" t="s">
+        <v>46</v>
+      </c>
+      <c r="H164" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>167</v>
       </c>
@@ -4835,11 +4928,20 @@
       <c r="D165">
         <v>5</v>
       </c>
+      <c r="E165" t="s">
+        <v>143</v>
+      </c>
       <c r="F165" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G165" t="s">
+        <v>77</v>
+      </c>
+      <c r="H165" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>167</v>
       </c>
@@ -4852,11 +4954,20 @@
       <c r="D166">
         <v>6</v>
       </c>
+      <c r="E166" t="s">
+        <v>144</v>
+      </c>
       <c r="F166" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G166" t="s">
+        <v>10</v>
+      </c>
+      <c r="H166" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>167</v>
       </c>
@@ -4869,11 +4980,20 @@
       <c r="D167">
         <v>6</v>
       </c>
+      <c r="E167" t="s">
+        <v>144</v>
+      </c>
       <c r="F167" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G167" t="s">
+        <v>9</v>
+      </c>
+      <c r="H167" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>199</v>
       </c>
@@ -4890,7 +5010,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>199</v>
       </c>
@@ -4907,7 +5027,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>199</v>
       </c>
@@ -4924,7 +5044,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>199</v>
       </c>
@@ -4941,7 +5061,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>199</v>
       </c>
@@ -4958,7 +5078,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>199</v>
       </c>
@@ -4975,7 +5095,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>199</v>
       </c>
@@ -4992,7 +5112,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>199</v>
       </c>
@@ -5009,7 +5129,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>199</v>
       </c>

</xml_diff>

<commit_message>
add paris surprise songs
</commit_message>
<xml_diff>
--- a/data-raw/surprise-songs.xlsx
+++ b/data-raw/surprise-songs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakethompson/Documents/GIT/packages/taylor/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ED334C9-A159-2746-B1BA-634B22B2892F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EC020C1-DA3D-5E45-B43C-68E2644EC341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26240" windowHeight="17500" xr2:uid="{23F40540-2069-D04D-A50F-51228CFC4AB9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1279" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1298" uniqueCount="220">
   <si>
     <t>date</t>
   </si>
@@ -675,6 +675,27 @@
   </si>
   <si>
     <t>epiphany</t>
+  </si>
+  <si>
+    <t>pink</t>
+  </si>
+  <si>
+    <t>Paris</t>
+  </si>
+  <si>
+    <t>loml</t>
+  </si>
+  <si>
+    <t>My Boy Only Breaks His Favorite Toys</t>
+  </si>
+  <si>
+    <t>The Alchemy</t>
+  </si>
+  <si>
+    <t>orange</t>
+  </si>
+  <si>
+    <t>new blue</t>
   </si>
 </sst>
 </file>
@@ -1035,8 +1056,8 @@
   <dimension ref="A1:I303"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A141" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G164" sqref="G164"/>
+      <pane ySplit="1" topLeftCell="A144" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E176" sqref="E176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5006,8 +5027,14 @@
       <c r="D168">
         <v>1</v>
       </c>
+      <c r="E168" t="s">
+        <v>213</v>
+      </c>
       <c r="F168" t="s">
         <v>7</v>
+      </c>
+      <c r="G168" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.2">
@@ -5023,8 +5050,14 @@
       <c r="D169">
         <v>1</v>
       </c>
+      <c r="E169" t="s">
+        <v>213</v>
+      </c>
       <c r="F169" t="s">
         <v>8</v>
+      </c>
+      <c r="G169" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.2">
@@ -5040,8 +5073,17 @@
       <c r="D170">
         <v>2</v>
       </c>
+      <c r="E170" t="s">
+        <v>219</v>
+      </c>
       <c r="F170" t="s">
         <v>7</v>
+      </c>
+      <c r="G170" t="s">
+        <v>151</v>
+      </c>
+      <c r="H170" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.2">
@@ -5057,8 +5099,14 @@
       <c r="D171">
         <v>2</v>
       </c>
+      <c r="E171" t="s">
+        <v>219</v>
+      </c>
       <c r="F171" t="s">
         <v>8</v>
+      </c>
+      <c r="G171" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.2">
@@ -5074,8 +5122,14 @@
       <c r="D172">
         <v>3</v>
       </c>
+      <c r="E172" t="s">
+        <v>218</v>
+      </c>
       <c r="F172" t="s">
         <v>7</v>
+      </c>
+      <c r="G172" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.2">
@@ -5091,8 +5145,14 @@
       <c r="D173">
         <v>3</v>
       </c>
+      <c r="E173" t="s">
+        <v>218</v>
+      </c>
       <c r="F173" t="s">
         <v>8</v>
+      </c>
+      <c r="G173" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.2">
@@ -5108,8 +5168,17 @@
       <c r="D174">
         <v>4</v>
       </c>
+      <c r="E174" t="s">
+        <v>219</v>
+      </c>
       <c r="F174" t="s">
         <v>7</v>
+      </c>
+      <c r="G174" t="s">
+        <v>217</v>
+      </c>
+      <c r="H174" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.2">
@@ -5125,8 +5194,17 @@
       <c r="D175">
         <v>4</v>
       </c>
+      <c r="E175" t="s">
+        <v>219</v>
+      </c>
       <c r="F175" t="s">
         <v>8</v>
+      </c>
+      <c r="G175" t="s">
+        <v>40</v>
+      </c>
+      <c r="H175" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
add lisbon surprise songs
</commit_message>
<xml_diff>
--- a/data-raw/surprise-songs.xlsx
+++ b/data-raw/surprise-songs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakethompson/Documents/GIT/packages/taylor/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72363F26-2610-3746-9D79-697420FA749A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DB46E7D-7E60-AE46-806A-840A615CF5CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26240" windowHeight="17500" xr2:uid="{23F40540-2069-D04D-A50F-51228CFC4AB9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1313" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1325" uniqueCount="229">
   <si>
     <t>date</t>
   </si>
@@ -711,6 +711,18 @@
   </si>
   <si>
     <t>How Did It End?</t>
+  </si>
+  <si>
+    <t>The Way I Loved You (Taylor's Version); The Other Side Of The Door (Taylor's Version)</t>
+  </si>
+  <si>
+    <t>Fresh Out The Slammer</t>
+  </si>
+  <si>
+    <t>The Tortured Poets Department</t>
+  </si>
+  <si>
+    <t>Long Live (Taylor's Version)</t>
   </si>
 </sst>
 </file>
@@ -1072,7 +1084,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A155" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E182" sqref="E182"/>
+      <selection pane="bottomLeft" activeCell="E186" sqref="E186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5382,8 +5394,17 @@
       <c r="D182">
         <v>1</v>
       </c>
+      <c r="E182" t="s">
+        <v>218</v>
+      </c>
       <c r="F182" t="s">
         <v>7</v>
+      </c>
+      <c r="G182" t="s">
+        <v>127</v>
+      </c>
+      <c r="H182" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.2">
@@ -5399,8 +5420,17 @@
       <c r="D183">
         <v>1</v>
       </c>
+      <c r="E183" t="s">
+        <v>218</v>
+      </c>
       <c r="F183" t="s">
         <v>8</v>
+      </c>
+      <c r="G183" t="s">
+        <v>226</v>
+      </c>
+      <c r="H183" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.2">
@@ -5416,8 +5446,17 @@
       <c r="D184">
         <v>2</v>
       </c>
+      <c r="E184" t="s">
+        <v>213</v>
+      </c>
       <c r="F184" t="s">
         <v>7</v>
+      </c>
+      <c r="G184" t="s">
+        <v>227</v>
+      </c>
+      <c r="H184" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.2">
@@ -5433,8 +5472,17 @@
       <c r="D185">
         <v>2</v>
       </c>
+      <c r="E185" t="s">
+        <v>213</v>
+      </c>
       <c r="F185" t="s">
         <v>8</v>
+      </c>
+      <c r="G185" t="s">
+        <v>123</v>
+      </c>
+      <c r="H185" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
add madrid surprise songs
</commit_message>
<xml_diff>
--- a/data-raw/surprise-songs.xlsx
+++ b/data-raw/surprise-songs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakethompson/Documents/GIT/packages/taylor/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DB46E7D-7E60-AE46-806A-840A615CF5CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63F2FB5B-5671-5A41-9EEE-F292F4224D46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26240" windowHeight="17500" xr2:uid="{23F40540-2069-D04D-A50F-51228CFC4AB9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1325" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1342" uniqueCount="231">
   <si>
     <t>date</t>
   </si>
@@ -723,6 +723,12 @@
   </si>
   <si>
     <t>Long Live (Taylor's Version)</t>
+  </si>
+  <si>
+    <t>I Can Fix Him (No Really I Can)</t>
+  </si>
+  <si>
+    <t>I Look In People's Windows</t>
   </si>
 </sst>
 </file>
@@ -1080,11 +1086,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04F0F9D9-7CA5-0C41-BC65-3D3349CBCA23}">
-  <dimension ref="A1:I303"/>
+  <dimension ref="A1:I305"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A155" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E186" sqref="E186"/>
+      <selection pane="bottomLeft" activeCell="G187" sqref="G187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5490,7 +5496,7 @@
         <v>199</v>
       </c>
       <c r="B186" s="2">
-        <v>45442</v>
+        <v>45441</v>
       </c>
       <c r="C186" t="s">
         <v>180</v>
@@ -5498,8 +5504,17 @@
       <c r="D186">
         <v>1</v>
       </c>
+      <c r="E186" t="s">
+        <v>218</v>
+      </c>
       <c r="F186" t="s">
         <v>7</v>
+      </c>
+      <c r="G186" t="s">
+        <v>46</v>
+      </c>
+      <c r="H186" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.2">
@@ -5507,7 +5522,7 @@
         <v>199</v>
       </c>
       <c r="B187" s="2">
-        <v>45442</v>
+        <v>45441</v>
       </c>
       <c r="C187" t="s">
         <v>180</v>
@@ -5515,8 +5530,17 @@
       <c r="D187">
         <v>1</v>
       </c>
+      <c r="E187" t="s">
+        <v>218</v>
+      </c>
       <c r="F187" t="s">
         <v>8</v>
+      </c>
+      <c r="G187" t="s">
+        <v>230</v>
+      </c>
+      <c r="H187" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="188" spans="1:8" x14ac:dyDescent="0.2">
@@ -5524,16 +5548,25 @@
         <v>199</v>
       </c>
       <c r="B188" s="2">
-        <v>45445</v>
+        <v>45442</v>
       </c>
       <c r="C188" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D188">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="E188" t="s">
+        <v>219</v>
       </c>
       <c r="F188" t="s">
         <v>7</v>
+      </c>
+      <c r="G188" t="s">
+        <v>13</v>
+      </c>
+      <c r="H188" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="189" spans="1:8" x14ac:dyDescent="0.2">
@@ -5541,16 +5574,22 @@
         <v>199</v>
       </c>
       <c r="B189" s="2">
-        <v>45445</v>
+        <v>45442</v>
       </c>
       <c r="C189" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D189">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="E189" t="s">
+        <v>219</v>
       </c>
       <c r="F189" t="s">
         <v>8</v>
+      </c>
+      <c r="G189" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.2">
@@ -5558,13 +5597,13 @@
         <v>199</v>
       </c>
       <c r="B190" s="2">
-        <v>45446</v>
+        <v>45445</v>
       </c>
       <c r="C190" t="s">
         <v>181</v>
       </c>
       <c r="D190">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F190" t="s">
         <v>7</v>
@@ -5575,13 +5614,13 @@
         <v>199</v>
       </c>
       <c r="B191" s="2">
-        <v>45446</v>
+        <v>45445</v>
       </c>
       <c r="C191" t="s">
         <v>181</v>
       </c>
       <c r="D191">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F191" t="s">
         <v>8</v>
@@ -5592,13 +5631,13 @@
         <v>199</v>
       </c>
       <c r="B192" s="2">
-        <v>45450</v>
+        <v>45446</v>
       </c>
       <c r="C192" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D192">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F192" t="s">
         <v>7</v>
@@ -5609,13 +5648,13 @@
         <v>199</v>
       </c>
       <c r="B193" s="2">
-        <v>45450</v>
+        <v>45446</v>
       </c>
       <c r="C193" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D193">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F193" t="s">
         <v>8</v>
@@ -5626,13 +5665,13 @@
         <v>199</v>
       </c>
       <c r="B194" s="2">
-        <v>45451</v>
+        <v>45450</v>
       </c>
       <c r="C194" t="s">
         <v>182</v>
       </c>
       <c r="D194">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F194" t="s">
         <v>7</v>
@@ -5643,13 +5682,13 @@
         <v>199</v>
       </c>
       <c r="B195" s="2">
-        <v>45451</v>
+        <v>45450</v>
       </c>
       <c r="C195" t="s">
         <v>182</v>
       </c>
       <c r="D195">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F195" t="s">
         <v>8</v>
@@ -5660,13 +5699,13 @@
         <v>199</v>
       </c>
       <c r="B196" s="2">
-        <v>45452</v>
+        <v>45451</v>
       </c>
       <c r="C196" t="s">
         <v>182</v>
       </c>
       <c r="D196">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F196" t="s">
         <v>7</v>
@@ -5677,13 +5716,13 @@
         <v>199</v>
       </c>
       <c r="B197" s="2">
-        <v>45452</v>
+        <v>45451</v>
       </c>
       <c r="C197" t="s">
         <v>182</v>
       </c>
       <c r="D197">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F197" t="s">
         <v>8</v>
@@ -5694,13 +5733,13 @@
         <v>199</v>
       </c>
       <c r="B198" s="2">
-        <v>45456</v>
+        <v>45452</v>
       </c>
       <c r="C198" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D198">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F198" t="s">
         <v>7</v>
@@ -5711,13 +5750,13 @@
         <v>199</v>
       </c>
       <c r="B199" s="2">
-        <v>45456</v>
+        <v>45452</v>
       </c>
       <c r="C199" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D199">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F199" t="s">
         <v>8</v>
@@ -5728,13 +5767,13 @@
         <v>199</v>
       </c>
       <c r="B200" s="2">
-        <v>45457</v>
+        <v>45456</v>
       </c>
       <c r="C200" t="s">
         <v>183</v>
       </c>
       <c r="D200">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F200" t="s">
         <v>7</v>
@@ -5745,13 +5784,13 @@
         <v>199</v>
       </c>
       <c r="B201" s="2">
-        <v>45457</v>
+        <v>45456</v>
       </c>
       <c r="C201" t="s">
         <v>183</v>
       </c>
       <c r="D201">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F201" t="s">
         <v>8</v>
@@ -5762,13 +5801,13 @@
         <v>199</v>
       </c>
       <c r="B202" s="2">
-        <v>45458</v>
+        <v>45457</v>
       </c>
       <c r="C202" t="s">
         <v>183</v>
       </c>
       <c r="D202">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F202" t="s">
         <v>7</v>
@@ -5779,13 +5818,13 @@
         <v>199</v>
       </c>
       <c r="B203" s="2">
-        <v>45458</v>
+        <v>45457</v>
       </c>
       <c r="C203" t="s">
         <v>183</v>
       </c>
       <c r="D203">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F203" t="s">
         <v>8</v>
@@ -5796,13 +5835,13 @@
         <v>199</v>
       </c>
       <c r="B204" s="2">
-        <v>45461</v>
+        <v>45458</v>
       </c>
       <c r="C204" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D204">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F204" t="s">
         <v>7</v>
@@ -5813,13 +5852,13 @@
         <v>199</v>
       </c>
       <c r="B205" s="2">
-        <v>45461</v>
+        <v>45458</v>
       </c>
       <c r="C205" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D205">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F205" t="s">
         <v>8</v>
@@ -5830,10 +5869,10 @@
         <v>199</v>
       </c>
       <c r="B206" s="2">
-        <v>45464</v>
+        <v>45461</v>
       </c>
       <c r="C206" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D206">
         <v>1</v>
@@ -5847,10 +5886,10 @@
         <v>199</v>
       </c>
       <c r="B207" s="2">
-        <v>45464</v>
+        <v>45461</v>
       </c>
       <c r="C207" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D207">
         <v>1</v>
@@ -5864,13 +5903,13 @@
         <v>199</v>
       </c>
       <c r="B208" s="2">
-        <v>45465</v>
+        <v>45464</v>
       </c>
       <c r="C208" t="s">
         <v>185</v>
       </c>
       <c r="D208">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F208" t="s">
         <v>7</v>
@@ -5881,13 +5920,13 @@
         <v>199</v>
       </c>
       <c r="B209" s="2">
-        <v>45465</v>
+        <v>45464</v>
       </c>
       <c r="C209" t="s">
         <v>185</v>
       </c>
       <c r="D209">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F209" t="s">
         <v>8</v>
@@ -5898,13 +5937,13 @@
         <v>199</v>
       </c>
       <c r="B210" s="2">
-        <v>45466</v>
+        <v>45465</v>
       </c>
       <c r="C210" t="s">
         <v>185</v>
       </c>
       <c r="D210">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F210" t="s">
         <v>7</v>
@@ -5915,13 +5954,13 @@
         <v>199</v>
       </c>
       <c r="B211" s="2">
-        <v>45466</v>
+        <v>45465</v>
       </c>
       <c r="C211" t="s">
         <v>185</v>
       </c>
       <c r="D211">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F211" t="s">
         <v>8</v>
@@ -5932,13 +5971,13 @@
         <v>199</v>
       </c>
       <c r="B212" s="2">
-        <v>45471</v>
+        <v>45466</v>
       </c>
       <c r="C212" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D212">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F212" t="s">
         <v>7</v>
@@ -5949,13 +5988,13 @@
         <v>199</v>
       </c>
       <c r="B213" s="2">
-        <v>45471</v>
+        <v>45466</v>
       </c>
       <c r="C213" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D213">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F213" t="s">
         <v>8</v>
@@ -5966,13 +6005,13 @@
         <v>199</v>
       </c>
       <c r="B214" s="2">
-        <v>45472</v>
+        <v>45471</v>
       </c>
       <c r="C214" t="s">
         <v>186</v>
       </c>
       <c r="D214">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F214" t="s">
         <v>7</v>
@@ -5983,13 +6022,13 @@
         <v>199</v>
       </c>
       <c r="B215" s="2">
-        <v>45472</v>
+        <v>45471</v>
       </c>
       <c r="C215" t="s">
         <v>186</v>
       </c>
       <c r="D215">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F215" t="s">
         <v>8</v>
@@ -6000,13 +6039,13 @@
         <v>199</v>
       </c>
       <c r="B216" s="2">
-        <v>45473</v>
+        <v>45472</v>
       </c>
       <c r="C216" t="s">
         <v>186</v>
       </c>
       <c r="D216">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F216" t="s">
         <v>7</v>
@@ -6017,13 +6056,13 @@
         <v>199</v>
       </c>
       <c r="B217" s="2">
-        <v>45473</v>
+        <v>45472</v>
       </c>
       <c r="C217" t="s">
         <v>186</v>
       </c>
       <c r="D217">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F217" t="s">
         <v>8</v>
@@ -6034,13 +6073,13 @@
         <v>199</v>
       </c>
       <c r="B218" s="2">
-        <v>45477</v>
+        <v>45473</v>
       </c>
       <c r="C218" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D218">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F218" t="s">
         <v>7</v>
@@ -6051,13 +6090,13 @@
         <v>199</v>
       </c>
       <c r="B219" s="2">
-        <v>45477</v>
+        <v>45473</v>
       </c>
       <c r="C219" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D219">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F219" t="s">
         <v>8</v>
@@ -6068,13 +6107,13 @@
         <v>199</v>
       </c>
       <c r="B220" s="2">
-        <v>45478</v>
+        <v>45477</v>
       </c>
       <c r="C220" t="s">
         <v>187</v>
       </c>
       <c r="D220">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F220" t="s">
         <v>7</v>
@@ -6085,13 +6124,13 @@
         <v>199</v>
       </c>
       <c r="B221" s="2">
-        <v>45478</v>
+        <v>45477</v>
       </c>
       <c r="C221" t="s">
         <v>187</v>
       </c>
       <c r="D221">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F221" t="s">
         <v>8</v>
@@ -6102,13 +6141,13 @@
         <v>199</v>
       </c>
       <c r="B222" s="2">
-        <v>45479</v>
+        <v>45478</v>
       </c>
       <c r="C222" t="s">
         <v>187</v>
       </c>
       <c r="D222">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F222" t="s">
         <v>7</v>
@@ -6119,13 +6158,13 @@
         <v>199</v>
       </c>
       <c r="B223" s="2">
-        <v>45479</v>
+        <v>45478</v>
       </c>
       <c r="C223" t="s">
         <v>187</v>
       </c>
       <c r="D223">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F223" t="s">
         <v>8</v>
@@ -6136,13 +6175,13 @@
         <v>199</v>
       </c>
       <c r="B224" s="2">
-        <v>45482</v>
+        <v>45479</v>
       </c>
       <c r="C224" t="s">
-        <v>200</v>
+        <v>187</v>
       </c>
       <c r="D224">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F224" t="s">
         <v>7</v>
@@ -6153,13 +6192,13 @@
         <v>199</v>
       </c>
       <c r="B225" s="2">
-        <v>45482</v>
+        <v>45479</v>
       </c>
       <c r="C225" t="s">
-        <v>200</v>
+        <v>187</v>
       </c>
       <c r="D225">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F225" t="s">
         <v>8</v>
@@ -6170,13 +6209,13 @@
         <v>199</v>
       </c>
       <c r="B226" s="2">
-        <v>45483</v>
+        <v>45482</v>
       </c>
       <c r="C226" t="s">
         <v>200</v>
       </c>
       <c r="D226">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F226" t="s">
         <v>7</v>
@@ -6187,13 +6226,13 @@
         <v>199</v>
       </c>
       <c r="B227" s="2">
-        <v>45483</v>
+        <v>45482</v>
       </c>
       <c r="C227" t="s">
         <v>200</v>
       </c>
       <c r="D227">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F227" t="s">
         <v>8</v>
@@ -6204,13 +6243,13 @@
         <v>199</v>
       </c>
       <c r="B228" s="2">
-        <v>45486</v>
+        <v>45483</v>
       </c>
       <c r="C228" t="s">
-        <v>188</v>
+        <v>200</v>
       </c>
       <c r="D228">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F228" t="s">
         <v>7</v>
@@ -6221,13 +6260,13 @@
         <v>199</v>
       </c>
       <c r="B229" s="2">
-        <v>45486</v>
+        <v>45483</v>
       </c>
       <c r="C229" t="s">
-        <v>188</v>
+        <v>200</v>
       </c>
       <c r="D229">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F229" t="s">
         <v>8</v>
@@ -6238,13 +6277,13 @@
         <v>199</v>
       </c>
       <c r="B230" s="2">
-        <v>45487</v>
+        <v>45486</v>
       </c>
       <c r="C230" t="s">
         <v>188</v>
       </c>
       <c r="D230">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F230" t="s">
         <v>7</v>
@@ -6255,13 +6294,13 @@
         <v>199</v>
       </c>
       <c r="B231" s="2">
-        <v>45487</v>
+        <v>45486</v>
       </c>
       <c r="C231" t="s">
         <v>188</v>
       </c>
       <c r="D231">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F231" t="s">
         <v>8</v>
@@ -6272,13 +6311,13 @@
         <v>199</v>
       </c>
       <c r="B232" s="2">
-        <v>45490</v>
+        <v>45487</v>
       </c>
       <c r="C232" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D232">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F232" t="s">
         <v>7</v>
@@ -6289,13 +6328,13 @@
         <v>199</v>
       </c>
       <c r="B233" s="2">
-        <v>45490</v>
+        <v>45487</v>
       </c>
       <c r="C233" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D233">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F233" t="s">
         <v>8</v>
@@ -6306,13 +6345,13 @@
         <v>199</v>
       </c>
       <c r="B234" s="2">
-        <v>45491</v>
+        <v>45490</v>
       </c>
       <c r="C234" t="s">
         <v>189</v>
       </c>
       <c r="D234">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F234" t="s">
         <v>7</v>
@@ -6323,13 +6362,13 @@
         <v>199</v>
       </c>
       <c r="B235" s="2">
-        <v>45491</v>
+        <v>45490</v>
       </c>
       <c r="C235" t="s">
         <v>189</v>
       </c>
       <c r="D235">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F235" t="s">
         <v>8</v>
@@ -6340,13 +6379,13 @@
         <v>199</v>
       </c>
       <c r="B236" s="2">
-        <v>45492</v>
+        <v>45491</v>
       </c>
       <c r="C236" t="s">
         <v>189</v>
       </c>
       <c r="D236">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F236" t="s">
         <v>7</v>
@@ -6357,13 +6396,13 @@
         <v>199</v>
       </c>
       <c r="B237" s="2">
-        <v>45492</v>
+        <v>45491</v>
       </c>
       <c r="C237" t="s">
         <v>189</v>
       </c>
       <c r="D237">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F237" t="s">
         <v>8</v>
@@ -6374,13 +6413,13 @@
         <v>199</v>
       </c>
       <c r="B238" s="2">
-        <v>45496</v>
+        <v>45492</v>
       </c>
       <c r="C238" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D238">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F238" t="s">
         <v>7</v>
@@ -6391,13 +6430,13 @@
         <v>199</v>
       </c>
       <c r="B239" s="2">
-        <v>45496</v>
+        <v>45492</v>
       </c>
       <c r="C239" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D239">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F239" t="s">
         <v>8</v>
@@ -6408,13 +6447,13 @@
         <v>199</v>
       </c>
       <c r="B240" s="2">
-        <v>45497</v>
+        <v>45496</v>
       </c>
       <c r="C240" t="s">
         <v>190</v>
       </c>
       <c r="D240">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F240" t="s">
         <v>7</v>
@@ -6425,13 +6464,13 @@
         <v>199</v>
       </c>
       <c r="B241" s="2">
-        <v>45497</v>
+        <v>45496</v>
       </c>
       <c r="C241" t="s">
         <v>190</v>
       </c>
       <c r="D241">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F241" t="s">
         <v>8</v>
@@ -6442,13 +6481,13 @@
         <v>199</v>
       </c>
       <c r="B242" s="2">
-        <v>45500</v>
+        <v>45497</v>
       </c>
       <c r="C242" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D242">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F242" t="s">
         <v>7</v>
@@ -6459,13 +6498,13 @@
         <v>199</v>
       </c>
       <c r="B243" s="2">
-        <v>45500</v>
+        <v>45497</v>
       </c>
       <c r="C243" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D243">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F243" t="s">
         <v>8</v>
@@ -6476,13 +6515,13 @@
         <v>199</v>
       </c>
       <c r="B244" s="2">
-        <v>45501</v>
+        <v>45500</v>
       </c>
       <c r="C244" t="s">
         <v>191</v>
       </c>
       <c r="D244">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F244" t="s">
         <v>7</v>
@@ -6493,13 +6532,13 @@
         <v>199</v>
       </c>
       <c r="B245" s="2">
-        <v>45501</v>
+        <v>45500</v>
       </c>
       <c r="C245" t="s">
         <v>191</v>
       </c>
       <c r="D245">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F245" t="s">
         <v>8</v>
@@ -6510,13 +6549,13 @@
         <v>199</v>
       </c>
       <c r="B246" s="2">
-        <v>45505</v>
+        <v>45501</v>
       </c>
       <c r="C246" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D246">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F246" t="s">
         <v>7</v>
@@ -6527,13 +6566,13 @@
         <v>199</v>
       </c>
       <c r="B247" s="2">
-        <v>45505</v>
+        <v>45501</v>
       </c>
       <c r="C247" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D247">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F247" t="s">
         <v>8</v>
@@ -6544,13 +6583,13 @@
         <v>199</v>
       </c>
       <c r="B248" s="2">
-        <v>45506</v>
+        <v>45505</v>
       </c>
       <c r="C248" t="s">
         <v>192</v>
       </c>
       <c r="D248">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F248" t="s">
         <v>7</v>
@@ -6561,13 +6600,13 @@
         <v>199</v>
       </c>
       <c r="B249" s="2">
-        <v>45506</v>
+        <v>45505</v>
       </c>
       <c r="C249" t="s">
         <v>192</v>
       </c>
       <c r="D249">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F249" t="s">
         <v>8</v>
@@ -6578,13 +6617,13 @@
         <v>199</v>
       </c>
       <c r="B250" s="2">
-        <v>45507</v>
+        <v>45506</v>
       </c>
       <c r="C250" t="s">
         <v>192</v>
       </c>
       <c r="D250">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F250" t="s">
         <v>7</v>
@@ -6595,13 +6634,13 @@
         <v>199</v>
       </c>
       <c r="B251" s="2">
-        <v>45507</v>
+        <v>45506</v>
       </c>
       <c r="C251" t="s">
         <v>192</v>
       </c>
       <c r="D251">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F251" t="s">
         <v>8</v>
@@ -6612,13 +6651,13 @@
         <v>199</v>
       </c>
       <c r="B252" s="2">
-        <v>45512</v>
+        <v>45507</v>
       </c>
       <c r="C252" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D252">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F252" t="s">
         <v>7</v>
@@ -6629,13 +6668,13 @@
         <v>199</v>
       </c>
       <c r="B253" s="2">
-        <v>45512</v>
+        <v>45507</v>
       </c>
       <c r="C253" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D253">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F253" t="s">
         <v>8</v>
@@ -6646,13 +6685,13 @@
         <v>199</v>
       </c>
       <c r="B254" s="2">
-        <v>45513</v>
+        <v>45512</v>
       </c>
       <c r="C254" t="s">
         <v>193</v>
       </c>
       <c r="D254">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F254" t="s">
         <v>7</v>
@@ -6663,13 +6702,13 @@
         <v>199</v>
       </c>
       <c r="B255" s="2">
-        <v>45513</v>
+        <v>45512</v>
       </c>
       <c r="C255" t="s">
         <v>193</v>
       </c>
       <c r="D255">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F255" t="s">
         <v>8</v>
@@ -6680,13 +6719,13 @@
         <v>199</v>
       </c>
       <c r="B256" s="2">
-        <v>45514</v>
+        <v>45513</v>
       </c>
       <c r="C256" t="s">
         <v>193</v>
       </c>
       <c r="D256">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F256" t="s">
         <v>7</v>
@@ -6697,13 +6736,13 @@
         <v>199</v>
       </c>
       <c r="B257" s="2">
-        <v>45514</v>
+        <v>45513</v>
       </c>
       <c r="C257" t="s">
         <v>193</v>
       </c>
       <c r="D257">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F257" t="s">
         <v>8</v>
@@ -6714,13 +6753,13 @@
         <v>199</v>
       </c>
       <c r="B258" s="2">
-        <v>45519</v>
+        <v>45514</v>
       </c>
       <c r="C258" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="D258">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F258" t="s">
         <v>7</v>
@@ -6731,13 +6770,13 @@
         <v>199</v>
       </c>
       <c r="B259" s="2">
-        <v>45519</v>
+        <v>45514</v>
       </c>
       <c r="C259" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="D259">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F259" t="s">
         <v>8</v>
@@ -6748,13 +6787,13 @@
         <v>199</v>
       </c>
       <c r="B260" s="2">
-        <v>45520</v>
+        <v>45519</v>
       </c>
       <c r="C260" t="s">
         <v>185</v>
       </c>
       <c r="D260">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F260" t="s">
         <v>7</v>
@@ -6765,13 +6804,13 @@
         <v>199</v>
       </c>
       <c r="B261" s="2">
-        <v>45520</v>
+        <v>45519</v>
       </c>
       <c r="C261" t="s">
         <v>185</v>
       </c>
       <c r="D261">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F261" t="s">
         <v>8</v>
@@ -6782,13 +6821,13 @@
         <v>199</v>
       </c>
       <c r="B262" s="2">
-        <v>45521</v>
+        <v>45520</v>
       </c>
       <c r="C262" t="s">
         <v>185</v>
       </c>
       <c r="D262">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F262" t="s">
         <v>7</v>
@@ -6799,13 +6838,13 @@
         <v>199</v>
       </c>
       <c r="B263" s="2">
-        <v>45521</v>
+        <v>45520</v>
       </c>
       <c r="C263" t="s">
         <v>185</v>
       </c>
       <c r="D263">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F263" t="s">
         <v>8</v>
@@ -6816,13 +6855,13 @@
         <v>199</v>
       </c>
       <c r="B264" s="2">
-        <v>45523</v>
+        <v>45521</v>
       </c>
       <c r="C264" t="s">
         <v>185</v>
       </c>
       <c r="D264">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F264" t="s">
         <v>7</v>
@@ -6833,13 +6872,13 @@
         <v>199</v>
       </c>
       <c r="B265" s="2">
-        <v>45523</v>
+        <v>45521</v>
       </c>
       <c r="C265" t="s">
         <v>185</v>
       </c>
       <c r="D265">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F265" t="s">
         <v>8</v>
@@ -6850,13 +6889,13 @@
         <v>199</v>
       </c>
       <c r="B266" s="2">
-        <v>45524</v>
+        <v>45523</v>
       </c>
       <c r="C266" t="s">
         <v>185</v>
       </c>
       <c r="D266">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F266" t="s">
         <v>7</v>
@@ -6867,13 +6906,13 @@
         <v>199</v>
       </c>
       <c r="B267" s="2">
-        <v>45524</v>
+        <v>45523</v>
       </c>
       <c r="C267" t="s">
         <v>185</v>
       </c>
       <c r="D267">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F267" t="s">
         <v>8</v>
@@ -6881,16 +6920,16 @@
     </row>
     <row r="268" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B268" s="2">
-        <v>45583</v>
+        <v>45524</v>
       </c>
       <c r="C268" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="D268">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F268" t="s">
         <v>7</v>
@@ -6898,16 +6937,16 @@
     </row>
     <row r="269" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B269" s="2">
-        <v>45583</v>
+        <v>45524</v>
       </c>
       <c r="C269" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="D269">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F269" t="s">
         <v>8</v>
@@ -6918,13 +6957,13 @@
         <v>202</v>
       </c>
       <c r="B270" s="2">
-        <v>45584</v>
+        <v>45583</v>
       </c>
       <c r="C270" t="s">
         <v>194</v>
       </c>
       <c r="D270">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F270" t="s">
         <v>7</v>
@@ -6935,13 +6974,13 @@
         <v>202</v>
       </c>
       <c r="B271" s="2">
-        <v>45584</v>
+        <v>45583</v>
       </c>
       <c r="C271" t="s">
         <v>194</v>
       </c>
       <c r="D271">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F271" t="s">
         <v>8</v>
@@ -6952,13 +6991,13 @@
         <v>202</v>
       </c>
       <c r="B272" s="2">
-        <v>45585</v>
+        <v>45584</v>
       </c>
       <c r="C272" t="s">
         <v>194</v>
       </c>
       <c r="D272">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F272" t="s">
         <v>7</v>
@@ -6969,13 +7008,13 @@
         <v>202</v>
       </c>
       <c r="B273" s="2">
-        <v>45585</v>
+        <v>45584</v>
       </c>
       <c r="C273" t="s">
         <v>194</v>
       </c>
       <c r="D273">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F273" t="s">
         <v>8</v>
@@ -6986,13 +7025,13 @@
         <v>202</v>
       </c>
       <c r="B274" s="2">
-        <v>45590</v>
+        <v>45585</v>
       </c>
       <c r="C274" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D274">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F274" t="s">
         <v>7</v>
@@ -7003,13 +7042,13 @@
         <v>202</v>
       </c>
       <c r="B275" s="2">
-        <v>45590</v>
+        <v>45585</v>
       </c>
       <c r="C275" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D275">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F275" t="s">
         <v>8</v>
@@ -7020,13 +7059,13 @@
         <v>202</v>
       </c>
       <c r="B276" s="2">
-        <v>45591</v>
+        <v>45590</v>
       </c>
       <c r="C276" t="s">
         <v>195</v>
       </c>
       <c r="D276">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F276" t="s">
         <v>7</v>
@@ -7037,13 +7076,13 @@
         <v>202</v>
       </c>
       <c r="B277" s="2">
-        <v>45591</v>
+        <v>45590</v>
       </c>
       <c r="C277" t="s">
         <v>195</v>
       </c>
       <c r="D277">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F277" t="s">
         <v>8</v>
@@ -7054,13 +7093,13 @@
         <v>202</v>
       </c>
       <c r="B278" s="2">
-        <v>45592</v>
+        <v>45591</v>
       </c>
       <c r="C278" t="s">
         <v>195</v>
       </c>
       <c r="D278">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F278" t="s">
         <v>7</v>
@@ -7071,13 +7110,13 @@
         <v>202</v>
       </c>
       <c r="B279" s="2">
-        <v>45592</v>
+        <v>45591</v>
       </c>
       <c r="C279" t="s">
         <v>195</v>
       </c>
       <c r="D279">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F279" t="s">
         <v>8</v>
@@ -7088,13 +7127,13 @@
         <v>202</v>
       </c>
       <c r="B280" s="2">
-        <v>45597</v>
+        <v>45592</v>
       </c>
       <c r="C280" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D280">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F280" t="s">
         <v>7</v>
@@ -7105,13 +7144,13 @@
         <v>202</v>
       </c>
       <c r="B281" s="2">
-        <v>45597</v>
+        <v>45592</v>
       </c>
       <c r="C281" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D281">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F281" t="s">
         <v>8</v>
@@ -7122,13 +7161,13 @@
         <v>202</v>
       </c>
       <c r="B282" s="2">
-        <v>45598</v>
+        <v>45597</v>
       </c>
       <c r="C282" t="s">
         <v>196</v>
       </c>
       <c r="D282">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F282" t="s">
         <v>7</v>
@@ -7139,13 +7178,13 @@
         <v>202</v>
       </c>
       <c r="B283" s="2">
-        <v>45598</v>
+        <v>45597</v>
       </c>
       <c r="C283" t="s">
         <v>196</v>
       </c>
       <c r="D283">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F283" t="s">
         <v>8</v>
@@ -7156,13 +7195,13 @@
         <v>202</v>
       </c>
       <c r="B284" s="2">
-        <v>45599</v>
+        <v>45598</v>
       </c>
       <c r="C284" t="s">
         <v>196</v>
       </c>
       <c r="D284">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F284" t="s">
         <v>7</v>
@@ -7173,13 +7212,13 @@
         <v>202</v>
       </c>
       <c r="B285" s="2">
-        <v>45599</v>
+        <v>45598</v>
       </c>
       <c r="C285" t="s">
         <v>196</v>
       </c>
       <c r="D285">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F285" t="s">
         <v>8</v>
@@ -7190,13 +7229,13 @@
         <v>202</v>
       </c>
       <c r="B286" s="2">
-        <v>45610</v>
+        <v>45599</v>
       </c>
       <c r="C286" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D286">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F286" t="s">
         <v>7</v>
@@ -7207,13 +7246,13 @@
         <v>202</v>
       </c>
       <c r="B287" s="2">
-        <v>45610</v>
+        <v>45599</v>
       </c>
       <c r="C287" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D287">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F287" t="s">
         <v>8</v>
@@ -7224,13 +7263,13 @@
         <v>202</v>
       </c>
       <c r="B288" s="2">
-        <v>45611</v>
+        <v>45610</v>
       </c>
       <c r="C288" t="s">
         <v>197</v>
       </c>
       <c r="D288">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F288" t="s">
         <v>7</v>
@@ -7241,13 +7280,13 @@
         <v>202</v>
       </c>
       <c r="B289" s="2">
-        <v>45611</v>
+        <v>45610</v>
       </c>
       <c r="C289" t="s">
         <v>197</v>
       </c>
       <c r="D289">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F289" t="s">
         <v>8</v>
@@ -7258,13 +7297,13 @@
         <v>202</v>
       </c>
       <c r="B290" s="2">
-        <v>45612</v>
+        <v>45611</v>
       </c>
       <c r="C290" t="s">
         <v>197</v>
       </c>
       <c r="D290">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F290" t="s">
         <v>7</v>
@@ -7275,13 +7314,13 @@
         <v>202</v>
       </c>
       <c r="B291" s="2">
-        <v>45612</v>
+        <v>45611</v>
       </c>
       <c r="C291" t="s">
         <v>197</v>
       </c>
       <c r="D291">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F291" t="s">
         <v>8</v>
@@ -7292,13 +7331,13 @@
         <v>202</v>
       </c>
       <c r="B292" s="2">
-        <v>45617</v>
+        <v>45612</v>
       </c>
       <c r="C292" t="s">
         <v>197</v>
       </c>
       <c r="D292">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F292" t="s">
         <v>7</v>
@@ -7309,13 +7348,13 @@
         <v>202</v>
       </c>
       <c r="B293" s="2">
-        <v>45617</v>
+        <v>45612</v>
       </c>
       <c r="C293" t="s">
         <v>197</v>
       </c>
       <c r="D293">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F293" t="s">
         <v>8</v>
@@ -7326,13 +7365,13 @@
         <v>202</v>
       </c>
       <c r="B294" s="2">
-        <v>45618</v>
+        <v>45617</v>
       </c>
       <c r="C294" t="s">
         <v>197</v>
       </c>
       <c r="D294">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F294" t="s">
         <v>7</v>
@@ -7343,13 +7382,13 @@
         <v>202</v>
       </c>
       <c r="B295" s="2">
-        <v>45618</v>
+        <v>45617</v>
       </c>
       <c r="C295" t="s">
         <v>197</v>
       </c>
       <c r="D295">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F295" t="s">
         <v>8</v>
@@ -7360,13 +7399,13 @@
         <v>202</v>
       </c>
       <c r="B296" s="2">
-        <v>45619</v>
+        <v>45618</v>
       </c>
       <c r="C296" t="s">
         <v>197</v>
       </c>
       <c r="D296">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F296" t="s">
         <v>7</v>
@@ -7377,13 +7416,13 @@
         <v>202</v>
       </c>
       <c r="B297" s="2">
-        <v>45619</v>
+        <v>45618</v>
       </c>
       <c r="C297" t="s">
         <v>197</v>
       </c>
       <c r="D297">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F297" t="s">
         <v>8</v>
@@ -7394,13 +7433,13 @@
         <v>202</v>
       </c>
       <c r="B298" s="2">
-        <v>45632</v>
+        <v>45619</v>
       </c>
       <c r="C298" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D298">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F298" t="s">
         <v>7</v>
@@ -7411,13 +7450,13 @@
         <v>202</v>
       </c>
       <c r="B299" s="2">
-        <v>45632</v>
+        <v>45619</v>
       </c>
       <c r="C299" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D299">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F299" t="s">
         <v>8</v>
@@ -7428,13 +7467,13 @@
         <v>202</v>
       </c>
       <c r="B300" s="2">
-        <v>45633</v>
+        <v>45632</v>
       </c>
       <c r="C300" t="s">
         <v>198</v>
       </c>
       <c r="D300">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F300" t="s">
         <v>7</v>
@@ -7445,13 +7484,13 @@
         <v>202</v>
       </c>
       <c r="B301" s="2">
-        <v>45633</v>
+        <v>45632</v>
       </c>
       <c r="C301" t="s">
         <v>198</v>
       </c>
       <c r="D301">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F301" t="s">
         <v>8</v>
@@ -7462,13 +7501,13 @@
         <v>202</v>
       </c>
       <c r="B302" s="2">
-        <v>45634</v>
+        <v>45633</v>
       </c>
       <c r="C302" t="s">
         <v>198</v>
       </c>
       <c r="D302">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F302" t="s">
         <v>7</v>
@@ -7479,15 +7518,49 @@
         <v>202</v>
       </c>
       <c r="B303" s="2">
-        <v>45634</v>
+        <v>45633</v>
       </c>
       <c r="C303" t="s">
         <v>198</v>
       </c>
       <c r="D303">
+        <v>2</v>
+      </c>
+      <c r="F303" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="304" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A304" t="s">
+        <v>202</v>
+      </c>
+      <c r="B304" s="2">
+        <v>45634</v>
+      </c>
+      <c r="C304" t="s">
+        <v>198</v>
+      </c>
+      <c r="D304">
         <v>3</v>
       </c>
-      <c r="F303" t="s">
+      <c r="F304" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="305" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A305" t="s">
+        <v>202</v>
+      </c>
+      <c r="B305" s="2">
+        <v>45634</v>
+      </c>
+      <c r="C305" t="s">
+        <v>198</v>
+      </c>
+      <c r="D305">
+        <v>3</v>
+      </c>
+      <c r="F305" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add edinburgh surprise songs
</commit_message>
<xml_diff>
--- a/data-raw/surprise-songs.xlsx
+++ b/data-raw/surprise-songs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakethompson/Documents/GIT/packages/taylor/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE2AC47C-CD9E-2549-BFEF-FE52E3607A23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB55C63F-8D9D-FD44-9815-0A91B6D06514}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26240" windowHeight="17500" xr2:uid="{23F40540-2069-D04D-A50F-51228CFC4AB9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1353" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1371" uniqueCount="238">
   <si>
     <t>date</t>
   </si>
@@ -738,6 +738,18 @@
   </si>
   <si>
     <t>Glitch</t>
+  </si>
+  <si>
+    <t>'tis the damn season</t>
+  </si>
+  <si>
+    <t>The Bolter</t>
+  </si>
+  <si>
+    <t>Crazier</t>
+  </si>
+  <si>
+    <t>It's Nice To Have A Friend</t>
   </si>
 </sst>
 </file>
@@ -777,10 +789,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1099,7 +1112,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A163" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F193" sqref="F193"/>
+      <selection pane="bottomLeft" activeCell="E200" sqref="E200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5679,7 +5692,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>199</v>
       </c>
@@ -5702,7 +5715,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>199</v>
       </c>
@@ -5715,11 +5728,20 @@
       <c r="D194">
         <v>1</v>
       </c>
+      <c r="E194" t="s">
+        <v>219</v>
+      </c>
       <c r="F194" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G194" t="s">
+        <v>49</v>
+      </c>
+      <c r="H194" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="195" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>199</v>
       </c>
@@ -5732,11 +5754,20 @@
       <c r="D195">
         <v>1</v>
       </c>
+      <c r="E195" t="s">
+        <v>219</v>
+      </c>
       <c r="F195" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G195" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="H195" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="196" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>199</v>
       </c>
@@ -5749,11 +5780,20 @@
       <c r="D196">
         <v>2</v>
       </c>
+      <c r="E196" t="s">
+        <v>218</v>
+      </c>
       <c r="F196" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G196" t="s">
+        <v>235</v>
+      </c>
+      <c r="H196" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="197" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>199</v>
       </c>
@@ -5766,11 +5806,20 @@
       <c r="D197">
         <v>2</v>
       </c>
+      <c r="E197" t="s">
+        <v>218</v>
+      </c>
       <c r="F197" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G197" t="s">
+        <v>110</v>
+      </c>
+      <c r="H197" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="198" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>199</v>
       </c>
@@ -5783,11 +5832,20 @@
       <c r="D198">
         <v>3</v>
       </c>
+      <c r="E198" t="s">
+        <v>213</v>
+      </c>
       <c r="F198" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G198" t="s">
+        <v>237</v>
+      </c>
+      <c r="H198" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="199" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>199</v>
       </c>
@@ -5800,11 +5858,20 @@
       <c r="D199">
         <v>3</v>
       </c>
+      <c r="E199" t="s">
+        <v>213</v>
+      </c>
       <c r="F199" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G199" t="s">
+        <v>84</v>
+      </c>
+      <c r="H199" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="200" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>199</v>
       </c>
@@ -5821,7 +5888,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>199</v>
       </c>
@@ -5838,7 +5905,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>199</v>
       </c>
@@ -5855,7 +5922,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>199</v>
       </c>
@@ -5872,7 +5939,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>199</v>
       </c>
@@ -5889,7 +5956,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>199</v>
       </c>
@@ -5906,7 +5973,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>199</v>
       </c>
@@ -5923,7 +5990,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>199</v>
       </c>
@@ -5940,7 +6007,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>199</v>
       </c>

</xml_diff>

<commit_message>
add liverpool surprise songs
</commit_message>
<xml_diff>
--- a/data-raw/surprise-songs.xlsx
+++ b/data-raw/surprise-songs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakethompson/Documents/GIT/packages/taylor/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB55C63F-8D9D-FD44-9815-0A91B6D06514}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06B86907-2832-CF46-994F-27E43D32DA2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26240" windowHeight="17500" xr2:uid="{23F40540-2069-D04D-A50F-51228CFC4AB9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1371" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1389" uniqueCount="242">
   <si>
     <t>date</t>
   </si>
@@ -750,6 +750,18 @@
   </si>
   <si>
     <t>It's Nice To Have A Friend</t>
+  </si>
+  <si>
+    <t>This Is What You Came For</t>
+  </si>
+  <si>
+    <t>Carolina</t>
+  </si>
+  <si>
+    <t>no body, no crime</t>
+  </si>
+  <si>
+    <t>The Manuscript</t>
   </si>
 </sst>
 </file>
@@ -1111,8 +1123,8 @@
   <dimension ref="A1:I305"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A163" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E200" sqref="E200"/>
+      <pane ySplit="1" topLeftCell="A170" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E206" sqref="E206"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5884,8 +5896,17 @@
       <c r="D200">
         <v>1</v>
       </c>
+      <c r="E200" t="s">
+        <v>213</v>
+      </c>
       <c r="F200" t="s">
         <v>7</v>
+      </c>
+      <c r="G200" t="s">
+        <v>125</v>
+      </c>
+      <c r="H200" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="201" spans="1:8" x14ac:dyDescent="0.2">
@@ -5901,8 +5922,17 @@
       <c r="D201">
         <v>1</v>
       </c>
+      <c r="E201" t="s">
+        <v>213</v>
+      </c>
       <c r="F201" t="s">
         <v>8</v>
+      </c>
+      <c r="G201" t="s">
+        <v>121</v>
+      </c>
+      <c r="H201" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="202" spans="1:8" x14ac:dyDescent="0.2">
@@ -5918,8 +5948,17 @@
       <c r="D202">
         <v>2</v>
       </c>
+      <c r="E202" t="s">
+        <v>219</v>
+      </c>
       <c r="F202" t="s">
         <v>7</v>
+      </c>
+      <c r="G202" t="s">
+        <v>238</v>
+      </c>
+      <c r="H202" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="203" spans="1:8" x14ac:dyDescent="0.2">
@@ -5935,8 +5974,17 @@
       <c r="D203">
         <v>2</v>
       </c>
+      <c r="E203" t="s">
+        <v>219</v>
+      </c>
       <c r="F203" t="s">
         <v>8</v>
+      </c>
+      <c r="G203" t="s">
+        <v>33</v>
+      </c>
+      <c r="H203" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="204" spans="1:8" x14ac:dyDescent="0.2">
@@ -5952,8 +6000,17 @@
       <c r="D204">
         <v>3</v>
       </c>
+      <c r="E204" t="s">
+        <v>218</v>
+      </c>
       <c r="F204" t="s">
         <v>7</v>
+      </c>
+      <c r="G204" t="s">
+        <v>239</v>
+      </c>
+      <c r="H204" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="205" spans="1:8" x14ac:dyDescent="0.2">
@@ -5969,8 +6026,17 @@
       <c r="D205">
         <v>3</v>
       </c>
+      <c r="E205" t="s">
+        <v>218</v>
+      </c>
       <c r="F205" t="s">
         <v>8</v>
+      </c>
+      <c r="G205" t="s">
+        <v>241</v>
+      </c>
+      <c r="H205" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="206" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
add cardiff surprise songs
</commit_message>
<xml_diff>
--- a/data-raw/surprise-songs.xlsx
+++ b/data-raw/surprise-songs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakethompson/Documents/GIT/packages/taylor/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06B86907-2832-CF46-994F-27E43D32DA2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{200151D7-5D7B-E845-B969-8448DFE45E74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26240" windowHeight="17500" xr2:uid="{23F40540-2069-D04D-A50F-51228CFC4AB9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1389" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1395" uniqueCount="243">
   <si>
     <t>date</t>
   </si>
@@ -762,6 +762,9 @@
   </si>
   <si>
     <t>The Manuscript</t>
+  </si>
+  <si>
+    <t>I Hate It Here</t>
   </si>
 </sst>
 </file>
@@ -1123,8 +1126,8 @@
   <dimension ref="A1:I305"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A170" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E206" sqref="E206"/>
+      <pane ySplit="1" topLeftCell="A186" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E207" sqref="E207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6052,8 +6055,17 @@
       <c r="D206">
         <v>1</v>
       </c>
+      <c r="E206" t="s">
+        <v>218</v>
+      </c>
       <c r="F206" t="s">
         <v>7</v>
+      </c>
+      <c r="G206" t="s">
+        <v>118</v>
+      </c>
+      <c r="H206" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="207" spans="1:8" x14ac:dyDescent="0.2">
@@ -6069,8 +6081,17 @@
       <c r="D207">
         <v>1</v>
       </c>
+      <c r="E207" t="s">
+        <v>218</v>
+      </c>
       <c r="F207" t="s">
         <v>8</v>
+      </c>
+      <c r="G207" t="s">
+        <v>242</v>
+      </c>
+      <c r="H207" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="208" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
add London round 1 surprise songs
</commit_message>
<xml_diff>
--- a/data-raw/surprise-songs.xlsx
+++ b/data-raw/surprise-songs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakethompson/Documents/GIT/packages/taylor/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{200151D7-5D7B-E845-B969-8448DFE45E74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{055BBF84-773C-CB46-8C88-987AA9310A73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26240" windowHeight="17500" xr2:uid="{23F40540-2069-D04D-A50F-51228CFC4AB9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1395" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1413" uniqueCount="250">
   <si>
     <t>date</t>
   </si>
@@ -765,6 +765,27 @@
   </si>
   <si>
     <t>I Hate It Here</t>
+  </si>
+  <si>
+    <t>The Black Dog</t>
+  </si>
+  <si>
+    <t>Come Back...Be Here (Taylor's Version); Maroon</t>
+  </si>
+  <si>
+    <t>thanK you aIMee</t>
+  </si>
+  <si>
+    <t>Hayley Williams</t>
+  </si>
+  <si>
+    <t>us.</t>
+  </si>
+  <si>
+    <t>Gracie Abrams</t>
+  </si>
+  <si>
+    <t>Is It Over Now? (Taylor's Version) [From The Vault]; Clean (Taylor's Version)</t>
   </si>
 </sst>
 </file>
@@ -1126,8 +1147,8 @@
   <dimension ref="A1:I305"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A186" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E207" sqref="E207"/>
+      <pane ySplit="1" topLeftCell="A187" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G214" sqref="G214"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6107,11 +6128,20 @@
       <c r="D208">
         <v>1</v>
       </c>
+      <c r="E208" t="s">
+        <v>218</v>
+      </c>
       <c r="F208" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G208" t="s">
+        <v>82</v>
+      </c>
+      <c r="H208" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="209" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>199</v>
       </c>
@@ -6124,11 +6154,20 @@
       <c r="D209">
         <v>1</v>
       </c>
+      <c r="E209" t="s">
+        <v>218</v>
+      </c>
       <c r="F209" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G209" t="s">
+        <v>243</v>
+      </c>
+      <c r="H209" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="210" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>199</v>
       </c>
@@ -6141,11 +6180,20 @@
       <c r="D210">
         <v>2</v>
       </c>
+      <c r="E210" t="s">
+        <v>219</v>
+      </c>
       <c r="F210" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G210" t="s">
+        <v>245</v>
+      </c>
+      <c r="H210" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="211" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>199</v>
       </c>
@@ -6158,11 +6206,20 @@
       <c r="D211">
         <v>2</v>
       </c>
+      <c r="E211" t="s">
+        <v>219</v>
+      </c>
       <c r="F211" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G211" t="s">
+        <v>134</v>
+      </c>
+      <c r="I211" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="212" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>199</v>
       </c>
@@ -6175,11 +6232,20 @@
       <c r="D212">
         <v>3</v>
       </c>
+      <c r="E212" t="s">
+        <v>213</v>
+      </c>
       <c r="F212" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G212" t="s">
+        <v>247</v>
+      </c>
+      <c r="I212" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="213" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>199</v>
       </c>
@@ -6192,11 +6258,20 @@
       <c r="D213">
         <v>3</v>
       </c>
+      <c r="E213" t="s">
+        <v>213</v>
+      </c>
       <c r="F213" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G213" t="s">
+        <v>48</v>
+      </c>
+      <c r="H213" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="214" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>199</v>
       </c>
@@ -6213,7 +6288,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>199</v>
       </c>
@@ -6230,7 +6305,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>199</v>
       </c>
@@ -6247,7 +6322,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>199</v>
       </c>
@@ -6264,7 +6339,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>199</v>
       </c>
@@ -6281,7 +6356,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>199</v>
       </c>
@@ -6298,7 +6373,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="220" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>199</v>
       </c>
@@ -6315,7 +6390,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>199</v>
       </c>
@@ -6332,7 +6407,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="222" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>199</v>
       </c>
@@ -6349,7 +6424,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="223" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>199</v>
       </c>
@@ -6366,7 +6441,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="224" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>199</v>
       </c>

</xml_diff>

<commit_message>
add dublin surprise songs
</commit_message>
<xml_diff>
--- a/data-raw/surprise-songs.xlsx
+++ b/data-raw/surprise-songs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakethompson/Documents/GIT/packages/taylor/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{055BBF84-773C-CB46-8C88-987AA9310A73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FFA744C-4B7A-CE43-9983-CD2105F74A79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26240" windowHeight="17500" xr2:uid="{23F40540-2069-D04D-A50F-51228CFC4AB9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1413" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1430" uniqueCount="253">
   <si>
     <t>date</t>
   </si>
@@ -677,9 +677,6 @@
     <t>epiphany</t>
   </si>
   <si>
-    <t>pink</t>
-  </si>
-  <si>
     <t>Paris</t>
   </si>
   <si>
@@ -692,12 +689,6 @@
     <t>The Alchemy</t>
   </si>
   <si>
-    <t>orange</t>
-  </si>
-  <si>
-    <t>new blue</t>
-  </si>
-  <si>
     <t>Peter</t>
   </si>
   <si>
@@ -786,6 +777,24 @@
   </si>
   <si>
     <t>Is It Over Now? (Taylor's Version) [From The Vault]; Clean (Taylor's Version)</t>
+  </si>
+  <si>
+    <t>hoax</t>
+  </si>
+  <si>
+    <t>The Albatross</t>
+  </si>
+  <si>
+    <t>Clara Bow</t>
+  </si>
+  <si>
+    <t>ocean blue</t>
+  </si>
+  <si>
+    <t>bright pink</t>
+  </si>
+  <si>
+    <t>sunset</t>
   </si>
 </sst>
 </file>
@@ -1147,8 +1156,8 @@
   <dimension ref="A1:I305"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A187" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G214" sqref="G214"/>
+      <pane ySplit="1" topLeftCell="A191" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F219" sqref="F219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5119,13 +5128,13 @@
         <v>1</v>
       </c>
       <c r="E168" t="s">
+        <v>251</v>
+      </c>
+      <c r="F168" t="s">
+        <v>7</v>
+      </c>
+      <c r="G168" t="s">
         <v>213</v>
-      </c>
-      <c r="F168" t="s">
-        <v>7</v>
-      </c>
-      <c r="G168" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.2">
@@ -5142,13 +5151,13 @@
         <v>1</v>
       </c>
       <c r="E169" t="s">
-        <v>213</v>
+        <v>251</v>
       </c>
       <c r="F169" t="s">
         <v>8</v>
       </c>
       <c r="G169" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.2">
@@ -5165,7 +5174,7 @@
         <v>2</v>
       </c>
       <c r="E170" t="s">
-        <v>219</v>
+        <v>250</v>
       </c>
       <c r="F170" t="s">
         <v>7</v>
@@ -5191,13 +5200,13 @@
         <v>2</v>
       </c>
       <c r="E171" t="s">
-        <v>219</v>
+        <v>250</v>
       </c>
       <c r="F171" t="s">
         <v>8</v>
       </c>
       <c r="G171" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.2">
@@ -5214,7 +5223,7 @@
         <v>3</v>
       </c>
       <c r="E172" t="s">
-        <v>218</v>
+        <v>252</v>
       </c>
       <c r="F172" t="s">
         <v>7</v>
@@ -5237,7 +5246,7 @@
         <v>3</v>
       </c>
       <c r="E173" t="s">
-        <v>218</v>
+        <v>252</v>
       </c>
       <c r="F173" t="s">
         <v>8</v>
@@ -5260,13 +5269,13 @@
         <v>4</v>
       </c>
       <c r="E174" t="s">
-        <v>219</v>
+        <v>250</v>
       </c>
       <c r="F174" t="s">
         <v>7</v>
       </c>
       <c r="G174" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H174" t="s">
         <v>30</v>
@@ -5286,7 +5295,7 @@
         <v>4</v>
       </c>
       <c r="E175" t="s">
-        <v>219</v>
+        <v>250</v>
       </c>
       <c r="F175" t="s">
         <v>8</v>
@@ -5295,7 +5304,7 @@
         <v>40</v>
       </c>
       <c r="H175" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.2">
@@ -5312,7 +5321,7 @@
         <v>1</v>
       </c>
       <c r="E176" t="s">
-        <v>213</v>
+        <v>251</v>
       </c>
       <c r="F176" t="s">
         <v>7</v>
@@ -5338,13 +5347,13 @@
         <v>1</v>
       </c>
       <c r="E177" t="s">
-        <v>213</v>
+        <v>251</v>
       </c>
       <c r="F177" t="s">
         <v>8</v>
       </c>
       <c r="G177" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.2">
@@ -5361,13 +5370,13 @@
         <v>2</v>
       </c>
       <c r="E178" t="s">
+        <v>252</v>
+      </c>
+      <c r="F178" t="s">
+        <v>7</v>
+      </c>
+      <c r="G178" t="s">
         <v>218</v>
-      </c>
-      <c r="F178" t="s">
-        <v>7</v>
-      </c>
-      <c r="G178" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.2">
@@ -5384,7 +5393,7 @@
         <v>2</v>
       </c>
       <c r="E179" t="s">
-        <v>218</v>
+        <v>252</v>
       </c>
       <c r="F179" t="s">
         <v>8</v>
@@ -5393,7 +5402,7 @@
         <v>166</v>
       </c>
       <c r="H179" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.2">
@@ -5410,7 +5419,7 @@
         <v>3</v>
       </c>
       <c r="E180" t="s">
-        <v>219</v>
+        <v>250</v>
       </c>
       <c r="F180" t="s">
         <v>7</v>
@@ -5419,7 +5428,7 @@
         <v>133</v>
       </c>
       <c r="H180" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.2">
@@ -5436,13 +5445,13 @@
         <v>3</v>
       </c>
       <c r="E181" t="s">
-        <v>219</v>
+        <v>250</v>
       </c>
       <c r="F181" t="s">
         <v>8</v>
       </c>
       <c r="G181" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.2">
@@ -5459,7 +5468,7 @@
         <v>1</v>
       </c>
       <c r="E182" t="s">
-        <v>218</v>
+        <v>252</v>
       </c>
       <c r="F182" t="s">
         <v>7</v>
@@ -5468,7 +5477,7 @@
         <v>127</v>
       </c>
       <c r="H182" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.2">
@@ -5485,13 +5494,13 @@
         <v>1</v>
       </c>
       <c r="E183" t="s">
-        <v>218</v>
+        <v>252</v>
       </c>
       <c r="F183" t="s">
         <v>8</v>
       </c>
       <c r="G183" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="H183" t="s">
         <v>43</v>
@@ -5511,13 +5520,13 @@
         <v>2</v>
       </c>
       <c r="E184" t="s">
-        <v>213</v>
+        <v>251</v>
       </c>
       <c r="F184" t="s">
         <v>7</v>
       </c>
       <c r="G184" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="H184" t="s">
         <v>162</v>
@@ -5537,7 +5546,7 @@
         <v>2</v>
       </c>
       <c r="E185" t="s">
-        <v>213</v>
+        <v>251</v>
       </c>
       <c r="F185" t="s">
         <v>8</v>
@@ -5546,7 +5555,7 @@
         <v>123</v>
       </c>
       <c r="H185" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.2">
@@ -5563,7 +5572,7 @@
         <v>1</v>
       </c>
       <c r="E186" t="s">
-        <v>218</v>
+        <v>252</v>
       </c>
       <c r="F186" t="s">
         <v>7</v>
@@ -5572,7 +5581,7 @@
         <v>46</v>
       </c>
       <c r="H186" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.2">
@@ -5589,13 +5598,13 @@
         <v>1</v>
       </c>
       <c r="E187" t="s">
-        <v>218</v>
+        <v>252</v>
       </c>
       <c r="F187" t="s">
         <v>8</v>
       </c>
       <c r="G187" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="H187" t="s">
         <v>15</v>
@@ -5615,7 +5624,7 @@
         <v>2</v>
       </c>
       <c r="E188" t="s">
-        <v>219</v>
+        <v>250</v>
       </c>
       <c r="F188" t="s">
         <v>7</v>
@@ -5641,7 +5650,7 @@
         <v>2</v>
       </c>
       <c r="E189" t="s">
-        <v>219</v>
+        <v>250</v>
       </c>
       <c r="F189" t="s">
         <v>8</v>
@@ -5664,13 +5673,13 @@
         <v>1</v>
       </c>
       <c r="E190" t="s">
-        <v>213</v>
+        <v>251</v>
       </c>
       <c r="F190" t="s">
         <v>7</v>
       </c>
       <c r="G190" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="H190" t="s">
         <v>209</v>
@@ -5690,7 +5699,7 @@
         <v>1</v>
       </c>
       <c r="E191" t="s">
-        <v>213</v>
+        <v>251</v>
       </c>
       <c r="F191" t="s">
         <v>8</v>
@@ -5716,13 +5725,13 @@
         <v>2</v>
       </c>
       <c r="E192" t="s">
-        <v>218</v>
+        <v>252</v>
       </c>
       <c r="F192" t="s">
         <v>7</v>
       </c>
       <c r="G192" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="H192" t="s">
         <v>104</v>
@@ -5742,13 +5751,13 @@
         <v>2</v>
       </c>
       <c r="E193" t="s">
-        <v>218</v>
+        <v>252</v>
       </c>
       <c r="F193" t="s">
         <v>8</v>
       </c>
       <c r="G193" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.2">
@@ -5765,7 +5774,7 @@
         <v>1</v>
       </c>
       <c r="E194" t="s">
-        <v>219</v>
+        <v>250</v>
       </c>
       <c r="F194" t="s">
         <v>7</v>
@@ -5791,13 +5800,13 @@
         <v>1</v>
       </c>
       <c r="E195" t="s">
-        <v>219</v>
+        <v>250</v>
       </c>
       <c r="F195" t="s">
         <v>8</v>
       </c>
       <c r="G195" s="3" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="H195" t="s">
         <v>92</v>
@@ -5817,13 +5826,13 @@
         <v>2</v>
       </c>
       <c r="E196" t="s">
-        <v>218</v>
+        <v>252</v>
       </c>
       <c r="F196" t="s">
         <v>7</v>
       </c>
       <c r="G196" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="H196" t="s">
         <v>74</v>
@@ -5843,7 +5852,7 @@
         <v>2</v>
       </c>
       <c r="E197" t="s">
-        <v>218</v>
+        <v>252</v>
       </c>
       <c r="F197" t="s">
         <v>8</v>
@@ -5852,7 +5861,7 @@
         <v>110</v>
       </c>
       <c r="H197" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="198" spans="1:8" x14ac:dyDescent="0.2">
@@ -5869,13 +5878,13 @@
         <v>3</v>
       </c>
       <c r="E198" t="s">
-        <v>213</v>
+        <v>251</v>
       </c>
       <c r="F198" t="s">
         <v>7</v>
       </c>
       <c r="G198" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="H198" t="s">
         <v>99</v>
@@ -5895,7 +5904,7 @@
         <v>3</v>
       </c>
       <c r="E199" t="s">
-        <v>213</v>
+        <v>251</v>
       </c>
       <c r="F199" t="s">
         <v>8</v>
@@ -5921,7 +5930,7 @@
         <v>1</v>
       </c>
       <c r="E200" t="s">
-        <v>213</v>
+        <v>251</v>
       </c>
       <c r="F200" t="s">
         <v>7</v>
@@ -5947,7 +5956,7 @@
         <v>1</v>
       </c>
       <c r="E201" t="s">
-        <v>213</v>
+        <v>251</v>
       </c>
       <c r="F201" t="s">
         <v>8</v>
@@ -5973,13 +5982,13 @@
         <v>2</v>
       </c>
       <c r="E202" t="s">
-        <v>219</v>
+        <v>250</v>
       </c>
       <c r="F202" t="s">
         <v>7</v>
       </c>
       <c r="G202" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="H202" t="s">
         <v>51</v>
@@ -5999,7 +6008,7 @@
         <v>2</v>
       </c>
       <c r="E203" t="s">
-        <v>219</v>
+        <v>250</v>
       </c>
       <c r="F203" t="s">
         <v>8</v>
@@ -6025,16 +6034,16 @@
         <v>3</v>
       </c>
       <c r="E204" t="s">
-        <v>218</v>
+        <v>252</v>
       </c>
       <c r="F204" t="s">
         <v>7</v>
       </c>
       <c r="G204" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="H204" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="205" spans="1:8" x14ac:dyDescent="0.2">
@@ -6051,13 +6060,13 @@
         <v>3</v>
       </c>
       <c r="E205" t="s">
-        <v>218</v>
+        <v>252</v>
       </c>
       <c r="F205" t="s">
         <v>8</v>
       </c>
       <c r="G205" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="H205" t="s">
         <v>73</v>
@@ -6077,7 +6086,7 @@
         <v>1</v>
       </c>
       <c r="E206" t="s">
-        <v>218</v>
+        <v>252</v>
       </c>
       <c r="F206" t="s">
         <v>7</v>
@@ -6103,13 +6112,13 @@
         <v>1</v>
       </c>
       <c r="E207" t="s">
-        <v>218</v>
+        <v>252</v>
       </c>
       <c r="F207" t="s">
         <v>8</v>
       </c>
       <c r="G207" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="H207" t="s">
         <v>80</v>
@@ -6129,7 +6138,7 @@
         <v>1</v>
       </c>
       <c r="E208" t="s">
-        <v>218</v>
+        <v>252</v>
       </c>
       <c r="F208" t="s">
         <v>7</v>
@@ -6155,16 +6164,16 @@
         <v>1</v>
       </c>
       <c r="E209" t="s">
-        <v>218</v>
+        <v>252</v>
       </c>
       <c r="F209" t="s">
         <v>8</v>
       </c>
       <c r="G209" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="H209" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="210" spans="1:9" x14ac:dyDescent="0.2">
@@ -6181,13 +6190,13 @@
         <v>2</v>
       </c>
       <c r="E210" t="s">
-        <v>219</v>
+        <v>250</v>
       </c>
       <c r="F210" t="s">
         <v>7</v>
       </c>
       <c r="G210" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="H210" t="s">
         <v>36</v>
@@ -6207,7 +6216,7 @@
         <v>2</v>
       </c>
       <c r="E211" t="s">
-        <v>219</v>
+        <v>250</v>
       </c>
       <c r="F211" t="s">
         <v>8</v>
@@ -6216,7 +6225,7 @@
         <v>134</v>
       </c>
       <c r="I211" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="212" spans="1:9" x14ac:dyDescent="0.2">
@@ -6233,16 +6242,16 @@
         <v>3</v>
       </c>
       <c r="E212" t="s">
-        <v>213</v>
+        <v>251</v>
       </c>
       <c r="F212" t="s">
         <v>7</v>
       </c>
       <c r="G212" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="I212" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="213" spans="1:9" x14ac:dyDescent="0.2">
@@ -6259,7 +6268,7 @@
         <v>3</v>
       </c>
       <c r="E213" t="s">
-        <v>213</v>
+        <v>251</v>
       </c>
       <c r="F213" t="s">
         <v>8</v>
@@ -6268,7 +6277,7 @@
         <v>48</v>
       </c>
       <c r="H213" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="214" spans="1:9" x14ac:dyDescent="0.2">
@@ -6284,8 +6293,17 @@
       <c r="D214">
         <v>1</v>
       </c>
+      <c r="E214" t="s">
+        <v>250</v>
+      </c>
       <c r="F214" t="s">
         <v>7</v>
+      </c>
+      <c r="G214" t="s">
+        <v>14</v>
+      </c>
+      <c r="H214" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="215" spans="1:9" x14ac:dyDescent="0.2">
@@ -6301,8 +6319,17 @@
       <c r="D215">
         <v>1</v>
       </c>
+      <c r="E215" t="s">
+        <v>250</v>
+      </c>
       <c r="F215" t="s">
         <v>8</v>
+      </c>
+      <c r="G215" t="s">
+        <v>119</v>
+      </c>
+      <c r="H215" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="216" spans="1:9" x14ac:dyDescent="0.2">
@@ -6318,8 +6345,17 @@
       <c r="D216">
         <v>2</v>
       </c>
+      <c r="E216" t="s">
+        <v>251</v>
+      </c>
       <c r="F216" t="s">
         <v>7</v>
+      </c>
+      <c r="G216" t="s">
+        <v>248</v>
+      </c>
+      <c r="H216" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="217" spans="1:9" x14ac:dyDescent="0.2">
@@ -6335,8 +6371,17 @@
       <c r="D217">
         <v>2</v>
       </c>
+      <c r="E217" t="s">
+        <v>251</v>
+      </c>
       <c r="F217" t="s">
         <v>8</v>
+      </c>
+      <c r="G217" t="s">
+        <v>53</v>
+      </c>
+      <c r="H217" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="218" spans="1:9" x14ac:dyDescent="0.2">
@@ -6352,8 +6397,17 @@
       <c r="D218">
         <v>3</v>
       </c>
+      <c r="E218" t="s">
+        <v>252</v>
+      </c>
       <c r="F218" t="s">
         <v>7</v>
+      </c>
+      <c r="G218" t="s">
+        <v>249</v>
+      </c>
+      <c r="H218" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="219" spans="1:9" x14ac:dyDescent="0.2">
@@ -6369,8 +6423,14 @@
       <c r="D219">
         <v>3</v>
       </c>
+      <c r="E219" t="s">
+        <v>252</v>
+      </c>
       <c r="F219" t="s">
         <v>8</v>
+      </c>
+      <c r="G219" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="220" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
add amsterdam surprise songs
</commit_message>
<xml_diff>
--- a/data-raw/surprise-songs.xlsx
+++ b/data-raw/surprise-songs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakethompson/Documents/GIT/packages/taylor/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FFA744C-4B7A-CE43-9983-CD2105F74A79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFD6C2D8-B7EA-F343-8FD4-B2CBDEC00D5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26240" windowHeight="17500" xr2:uid="{23F40540-2069-D04D-A50F-51228CFC4AB9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1430" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1448" uniqueCount="258">
   <si>
     <t>date</t>
   </si>
@@ -795,6 +795,21 @@
   </si>
   <si>
     <t>sunset</t>
+  </si>
+  <si>
+    <t>The Archer</t>
+  </si>
+  <si>
+    <t>imgonnagetyouback</t>
+  </si>
+  <si>
+    <t>Sweeter Than Fiction (Taylor's Version)</t>
+  </si>
+  <si>
+    <t>So High School; Everything Has Changed (Taylor's Version)</t>
+  </si>
+  <si>
+    <t>Mary's Song (Oh My My My)</t>
   </si>
 </sst>
 </file>
@@ -1156,8 +1171,8 @@
   <dimension ref="A1:I305"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A191" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F219" sqref="F219"/>
+      <pane ySplit="1" topLeftCell="A199" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G226" sqref="G226"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6446,8 +6461,17 @@
       <c r="D220">
         <v>1</v>
       </c>
+      <c r="E220" t="s">
+        <v>252</v>
+      </c>
       <c r="F220" t="s">
         <v>7</v>
+      </c>
+      <c r="G220" t="s">
+        <v>218</v>
+      </c>
+      <c r="H220" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="221" spans="1:9" x14ac:dyDescent="0.2">
@@ -6463,8 +6487,17 @@
       <c r="D221">
         <v>1</v>
       </c>
+      <c r="E221" t="s">
+        <v>252</v>
+      </c>
       <c r="F221" t="s">
         <v>8</v>
+      </c>
+      <c r="G221" t="s">
+        <v>253</v>
+      </c>
+      <c r="H221" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="222" spans="1:9" x14ac:dyDescent="0.2">
@@ -6480,8 +6513,17 @@
       <c r="D222">
         <v>2</v>
       </c>
+      <c r="E222" t="s">
+        <v>250</v>
+      </c>
       <c r="F222" t="s">
         <v>7</v>
+      </c>
+      <c r="G222" t="s">
+        <v>254</v>
+      </c>
+      <c r="H222" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="223" spans="1:9" x14ac:dyDescent="0.2">
@@ -6497,8 +6539,17 @@
       <c r="D223">
         <v>2</v>
       </c>
+      <c r="E223" t="s">
+        <v>250</v>
+      </c>
       <c r="F223" t="s">
         <v>8</v>
+      </c>
+      <c r="G223" t="s">
+        <v>111</v>
+      </c>
+      <c r="H223" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="224" spans="1:9" x14ac:dyDescent="0.2">
@@ -6514,11 +6565,20 @@
       <c r="D224">
         <v>3</v>
       </c>
+      <c r="E224" t="s">
+        <v>251</v>
+      </c>
       <c r="F224" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G224" t="s">
+        <v>255</v>
+      </c>
+      <c r="H224" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="225" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>199</v>
       </c>
@@ -6531,11 +6591,20 @@
       <c r="D225">
         <v>3</v>
       </c>
+      <c r="E225" t="s">
+        <v>251</v>
+      </c>
       <c r="F225" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G225" t="s">
+        <v>257</v>
+      </c>
+      <c r="H225" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="226" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>199</v>
       </c>
@@ -6552,7 +6621,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>199</v>
       </c>
@@ -6569,7 +6638,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>199</v>
       </c>
@@ -6586,7 +6655,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="229" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>199</v>
       </c>
@@ -6603,7 +6672,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="230" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>199</v>
       </c>
@@ -6620,7 +6689,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="231" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>199</v>
       </c>
@@ -6637,7 +6706,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="232" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>199</v>
       </c>
@@ -6654,7 +6723,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="233" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>199</v>
       </c>
@@ -6671,7 +6740,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="234" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>199</v>
       </c>
@@ -6688,7 +6757,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="235" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>199</v>
       </c>
@@ -6705,7 +6774,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="236" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>199</v>
       </c>
@@ -6722,7 +6791,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="237" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>199</v>
       </c>
@@ -6739,7 +6808,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="238" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>199</v>
       </c>
@@ -6756,7 +6825,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="239" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>199</v>
       </c>
@@ -6773,7 +6842,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="240" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>199</v>
       </c>

</xml_diff>

<commit_message>
add Zurich surprise songs
</commit_message>
<xml_diff>
--- a/data-raw/surprise-songs.xlsx
+++ b/data-raw/surprise-songs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakethompson/Documents/GIT/packages/taylor/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFD6C2D8-B7EA-F343-8FD4-B2CBDEC00D5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{879A3E56-D61A-3048-8215-999BEE56FE6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26240" windowHeight="17500" xr2:uid="{23F40540-2069-D04D-A50F-51228CFC4AB9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1448" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1460" uniqueCount="261">
   <si>
     <t>date</t>
   </si>
@@ -810,6 +810,15 @@
   </si>
   <si>
     <t>Mary's Song (Oh My My My)</t>
+  </si>
+  <si>
+    <t>closure</t>
+  </si>
+  <si>
+    <t>A Perfectly Good Heart</t>
+  </si>
+  <si>
+    <t>Robin</t>
   </si>
 </sst>
 </file>
@@ -1171,8 +1180,8 @@
   <dimension ref="A1:I305"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A199" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G226" sqref="G226"/>
+      <pane ySplit="1" topLeftCell="A202" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G229" sqref="G229"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6617,8 +6626,17 @@
       <c r="D226">
         <v>1</v>
       </c>
+      <c r="E226" t="s">
+        <v>252</v>
+      </c>
       <c r="F226" t="s">
         <v>7</v>
+      </c>
+      <c r="G226" t="s">
+        <v>108</v>
+      </c>
+      <c r="H226" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="227" spans="1:8" x14ac:dyDescent="0.2">
@@ -6634,8 +6652,17 @@
       <c r="D227">
         <v>1</v>
       </c>
+      <c r="E227" t="s">
+        <v>252</v>
+      </c>
       <c r="F227" t="s">
         <v>8</v>
+      </c>
+      <c r="G227" t="s">
+        <v>98</v>
+      </c>
+      <c r="H227" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="228" spans="1:8" x14ac:dyDescent="0.2">
@@ -6651,8 +6678,17 @@
       <c r="D228">
         <v>2</v>
       </c>
+      <c r="E228" t="s">
+        <v>251</v>
+      </c>
       <c r="F228" t="s">
         <v>7</v>
+      </c>
+      <c r="G228" t="s">
+        <v>258</v>
+      </c>
+      <c r="H228" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="229" spans="1:8" x14ac:dyDescent="0.2">
@@ -6668,8 +6704,17 @@
       <c r="D229">
         <v>2</v>
       </c>
+      <c r="E229" t="s">
+        <v>251</v>
+      </c>
       <c r="F229" t="s">
         <v>8</v>
+      </c>
+      <c r="G229" t="s">
+        <v>260</v>
+      </c>
+      <c r="H229" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="230" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
add Milan surprise songs
</commit_message>
<xml_diff>
--- a/data-raw/surprise-songs.xlsx
+++ b/data-raw/surprise-songs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakethompson/Documents/GIT/packages/taylor/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{879A3E56-D61A-3048-8215-999BEE56FE6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2B7F6C5-6881-0B4F-B525-B330CF5491BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26240" windowHeight="17500" xr2:uid="{23F40540-2069-D04D-A50F-51228CFC4AB9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1460" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1472" uniqueCount="262">
   <si>
     <t>date</t>
   </si>
@@ -819,6 +819,9 @@
   </si>
   <si>
     <t>Robin</t>
+  </si>
+  <si>
+    <t>the 1</t>
   </si>
 </sst>
 </file>
@@ -1181,7 +1184,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A202" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G229" sqref="G229"/>
+      <selection pane="bottomLeft" activeCell="E234" sqref="E234"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6730,8 +6733,17 @@
       <c r="D230">
         <v>1</v>
       </c>
+      <c r="E230" t="s">
+        <v>252</v>
+      </c>
       <c r="F230" t="s">
         <v>7</v>
+      </c>
+      <c r="G230" t="s">
+        <v>261</v>
+      </c>
+      <c r="H230" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="231" spans="1:8" x14ac:dyDescent="0.2">
@@ -6747,8 +6759,17 @@
       <c r="D231">
         <v>1</v>
       </c>
+      <c r="E231" t="s">
+        <v>252</v>
+      </c>
       <c r="F231" t="s">
         <v>8</v>
+      </c>
+      <c r="G231" t="s">
+        <v>85</v>
+      </c>
+      <c r="H231" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="232" spans="1:8" x14ac:dyDescent="0.2">
@@ -6764,8 +6785,17 @@
       <c r="D232">
         <v>2</v>
       </c>
+      <c r="E232" t="s">
+        <v>250</v>
+      </c>
       <c r="F232" t="s">
         <v>7</v>
+      </c>
+      <c r="G232" t="s">
+        <v>130</v>
+      </c>
+      <c r="H232" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="233" spans="1:8" x14ac:dyDescent="0.2">
@@ -6781,8 +6811,17 @@
       <c r="D233">
         <v>2</v>
       </c>
+      <c r="E233" t="s">
+        <v>250</v>
+      </c>
       <c r="F233" t="s">
         <v>8</v>
+      </c>
+      <c r="G233" t="s">
+        <v>74</v>
+      </c>
+      <c r="H233" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="234" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
add gelsenkirchen surprise songs
</commit_message>
<xml_diff>
--- a/data-raw/surprise-songs.xlsx
+++ b/data-raw/surprise-songs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakethompson/Documents/GIT/packages/taylor/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2B7F6C5-6881-0B4F-B525-B330CF5491BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F87B2934-B8CE-DC46-B214-D2F28DE06BA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26240" windowHeight="17500" xr2:uid="{23F40540-2069-D04D-A50F-51228CFC4AB9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1472" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1490" uniqueCount="264">
   <si>
     <t>date</t>
   </si>
@@ -822,6 +822,12 @@
   </si>
   <si>
     <t>the 1</t>
+  </si>
+  <si>
+    <t>invisible string</t>
+  </si>
+  <si>
+    <t>SuperStar (Taylor's Version)</t>
   </si>
 </sst>
 </file>
@@ -1183,8 +1189,8 @@
   <dimension ref="A1:I305"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A202" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E234" sqref="E234"/>
+      <pane ySplit="1" topLeftCell="A215" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E243" sqref="E243"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6837,8 +6843,17 @@
       <c r="D234">
         <v>1</v>
       </c>
+      <c r="E234" t="s">
+        <v>252</v>
+      </c>
       <c r="F234" t="s">
         <v>7</v>
+      </c>
+      <c r="G234" t="s">
+        <v>263</v>
+      </c>
+      <c r="H234" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="235" spans="1:8" x14ac:dyDescent="0.2">
@@ -6854,8 +6869,17 @@
       <c r="D235">
         <v>1</v>
       </c>
+      <c r="E235" t="s">
+        <v>252</v>
+      </c>
       <c r="F235" t="s">
         <v>8</v>
+      </c>
+      <c r="G235" t="s">
+        <v>154</v>
+      </c>
+      <c r="H235" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="236" spans="1:8" x14ac:dyDescent="0.2">
@@ -6871,8 +6895,17 @@
       <c r="D236">
         <v>2</v>
       </c>
+      <c r="E236" t="s">
+        <v>250</v>
+      </c>
       <c r="F236" t="s">
         <v>7</v>
+      </c>
+      <c r="G236" t="s">
+        <v>29</v>
+      </c>
+      <c r="H236" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="237" spans="1:8" x14ac:dyDescent="0.2">
@@ -6888,8 +6921,17 @@
       <c r="D237">
         <v>2</v>
       </c>
+      <c r="E237" t="s">
+        <v>250</v>
+      </c>
       <c r="F237" t="s">
         <v>8</v>
+      </c>
+      <c r="G237" t="s">
+        <v>11</v>
+      </c>
+      <c r="H237" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="238" spans="1:8" x14ac:dyDescent="0.2">
@@ -6905,8 +6947,17 @@
       <c r="D238">
         <v>3</v>
       </c>
+      <c r="E238" t="s">
+        <v>251</v>
+      </c>
       <c r="F238" t="s">
         <v>7</v>
+      </c>
+      <c r="G238" t="s">
+        <v>90</v>
+      </c>
+      <c r="H238" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="239" spans="1:8" x14ac:dyDescent="0.2">
@@ -6922,8 +6973,17 @@
       <c r="D239">
         <v>3</v>
       </c>
+      <c r="E239" t="s">
+        <v>251</v>
+      </c>
       <c r="F239" t="s">
         <v>8</v>
+      </c>
+      <c r="G239" t="s">
+        <v>161</v>
+      </c>
+      <c r="H239" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="240" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
add hamburg surprise songs
</commit_message>
<xml_diff>
--- a/data-raw/surprise-songs.xlsx
+++ b/data-raw/surprise-songs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakethompson/Documents/GIT/packages/taylor/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F87B2934-B8CE-DC46-B214-D2F28DE06BA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C66BE50-2AD9-CC47-AA21-86B6E3564494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26240" windowHeight="17500" xr2:uid="{23F40540-2069-D04D-A50F-51228CFC4AB9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1490" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1502" uniqueCount="269">
   <si>
     <t>date</t>
   </si>
@@ -828,6 +828,21 @@
   </si>
   <si>
     <t>SuperStar (Taylor's Version)</t>
+  </si>
+  <si>
+    <t>the last great american dynasty</t>
+  </si>
+  <si>
+    <t>Run (Taylor's Version) [From The Vault]</t>
+  </si>
+  <si>
+    <t>Nothing New (Taylor's Version) [From The Vault]</t>
+  </si>
+  <si>
+    <t>happiness</t>
+  </si>
+  <si>
+    <t>We Were Happy (Taylor's Version) [From The Vault]</t>
   </si>
 </sst>
 </file>
@@ -1190,7 +1205,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A215" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E243" sqref="E243"/>
+      <selection pane="bottomLeft" activeCell="E242" sqref="E242"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6999,11 +7014,20 @@
       <c r="D240">
         <v>1</v>
       </c>
+      <c r="E240" t="s">
+        <v>252</v>
+      </c>
       <c r="F240" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="241" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G240" t="s">
+        <v>47</v>
+      </c>
+      <c r="H240" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="241" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>199</v>
       </c>
@@ -7016,11 +7040,20 @@
       <c r="D241">
         <v>1</v>
       </c>
+      <c r="E241" t="s">
+        <v>252</v>
+      </c>
       <c r="F241" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="242" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G241" t="s">
+        <v>268</v>
+      </c>
+      <c r="H241" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="242" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>199</v>
       </c>
@@ -7033,11 +7066,20 @@
       <c r="D242">
         <v>2</v>
       </c>
+      <c r="E242" t="s">
+        <v>250</v>
+      </c>
       <c r="F242" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="243" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G242" t="s">
+        <v>264</v>
+      </c>
+      <c r="H242" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="243" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>199</v>
       </c>
@@ -7050,11 +7092,20 @@
       <c r="D243">
         <v>2</v>
       </c>
+      <c r="E243" t="s">
+        <v>250</v>
+      </c>
       <c r="F243" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="244" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G243" t="s">
+        <v>266</v>
+      </c>
+      <c r="H243" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="244" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>199</v>
       </c>
@@ -7071,7 +7122,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="245" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>199</v>
       </c>
@@ -7088,7 +7139,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="246" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>199</v>
       </c>
@@ -7105,7 +7156,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="247" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>199</v>
       </c>
@@ -7122,7 +7173,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="248" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>199</v>
       </c>
@@ -7139,7 +7190,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="249" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>199</v>
       </c>
@@ -7156,7 +7207,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="250" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>199</v>
       </c>
@@ -7173,7 +7224,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="251" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>199</v>
       </c>
@@ -7190,7 +7241,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="252" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>199</v>
       </c>
@@ -7207,7 +7258,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="253" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>199</v>
       </c>
@@ -7224,7 +7275,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="254" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>199</v>
       </c>
@@ -7241,7 +7292,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="255" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>199</v>
       </c>
@@ -7258,7 +7309,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="256" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>199</v>
       </c>

</xml_diff>

<commit_message>
add munich surprise songs
</commit_message>
<xml_diff>
--- a/data-raw/surprise-songs.xlsx
+++ b/data-raw/surprise-songs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakethompson/Documents/GIT/packages/taylor/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C66BE50-2AD9-CC47-AA21-86B6E3564494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{340CC3D8-C9B6-7448-8A26-9C86A0D9771C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26240" windowHeight="17500" xr2:uid="{23F40540-2069-D04D-A50F-51228CFC4AB9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1502" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1514" uniqueCount="270">
   <si>
     <t>date</t>
   </si>
@@ -843,6 +843,9 @@
   </si>
   <si>
     <t>We Were Happy (Taylor's Version) [From The Vault]</t>
+  </si>
+  <si>
+    <t>Don't You (Taylor's Version) [From The Vault]</t>
   </si>
 </sst>
 </file>
@@ -1204,8 +1207,8 @@
   <dimension ref="A1:I305"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A215" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E242" sqref="E242"/>
+      <pane ySplit="1" topLeftCell="A235" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E248" sqref="E248"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7118,8 +7121,17 @@
       <c r="D244">
         <v>1</v>
       </c>
+      <c r="E244" t="s">
+        <v>251</v>
+      </c>
       <c r="F244" t="s">
         <v>7</v>
+      </c>
+      <c r="G244" t="s">
+        <v>223</v>
+      </c>
+      <c r="H244" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="245" spans="1:8" x14ac:dyDescent="0.2">
@@ -7135,8 +7147,17 @@
       <c r="D245">
         <v>1</v>
       </c>
+      <c r="E245" t="s">
+        <v>251</v>
+      </c>
       <c r="F245" t="s">
         <v>8</v>
+      </c>
+      <c r="G245" t="s">
+        <v>95</v>
+      </c>
+      <c r="H245" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="246" spans="1:8" x14ac:dyDescent="0.2">
@@ -7152,8 +7173,17 @@
       <c r="D246">
         <v>2</v>
       </c>
+      <c r="E246" t="s">
+        <v>252</v>
+      </c>
       <c r="F246" t="s">
         <v>7</v>
+      </c>
+      <c r="G246" t="s">
+        <v>81</v>
+      </c>
+      <c r="H246" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="247" spans="1:8" x14ac:dyDescent="0.2">
@@ -7169,8 +7199,17 @@
       <c r="D247">
         <v>2</v>
       </c>
+      <c r="E247" t="s">
+        <v>252</v>
+      </c>
       <c r="F247" t="s">
         <v>8</v>
+      </c>
+      <c r="G247" t="s">
+        <v>214</v>
+      </c>
+      <c r="H247" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="248" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
add warsaw surprise songs
</commit_message>
<xml_diff>
--- a/data-raw/surprise-songs.xlsx
+++ b/data-raw/surprise-songs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakethompson/Documents/GIT/packages/taylor/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{340CC3D8-C9B6-7448-8A26-9C86A0D9771C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F876D63F-A32F-854E-96FF-6069232099F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26240" windowHeight="17500" xr2:uid="{23F40540-2069-D04D-A50F-51228CFC4AB9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1514" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1532" uniqueCount="270">
   <si>
     <t>date</t>
   </si>
@@ -1208,7 +1208,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A235" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E248" sqref="E248"/>
+      <selection pane="bottomLeft" activeCell="E254" sqref="E254"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7225,8 +7225,17 @@
       <c r="D248">
         <v>1</v>
       </c>
+      <c r="E248" t="s">
+        <v>250</v>
+      </c>
       <c r="F248" t="s">
         <v>7</v>
+      </c>
+      <c r="G248" t="s">
+        <v>9</v>
+      </c>
+      <c r="H248" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="249" spans="1:8" x14ac:dyDescent="0.2">
@@ -7242,8 +7251,17 @@
       <c r="D249">
         <v>1</v>
       </c>
+      <c r="E249" t="s">
+        <v>250</v>
+      </c>
       <c r="F249" t="s">
         <v>8</v>
+      </c>
+      <c r="G249" t="s">
+        <v>156</v>
+      </c>
+      <c r="H249" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="250" spans="1:8" x14ac:dyDescent="0.2">
@@ -7259,8 +7277,17 @@
       <c r="D250">
         <v>2</v>
       </c>
+      <c r="E250" t="s">
+        <v>252</v>
+      </c>
       <c r="F250" t="s">
         <v>7</v>
+      </c>
+      <c r="G250" t="s">
+        <v>226</v>
+      </c>
+      <c r="H250" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="251" spans="1:8" x14ac:dyDescent="0.2">
@@ -7276,8 +7303,17 @@
       <c r="D251">
         <v>2</v>
       </c>
+      <c r="E251" t="s">
+        <v>252</v>
+      </c>
       <c r="F251" t="s">
         <v>8</v>
+      </c>
+      <c r="G251" t="s">
+        <v>73</v>
+      </c>
+      <c r="H251" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="252" spans="1:8" x14ac:dyDescent="0.2">
@@ -7293,8 +7329,17 @@
       <c r="D252">
         <v>3</v>
       </c>
+      <c r="E252" t="s">
+        <v>251</v>
+      </c>
       <c r="F252" t="s">
         <v>7</v>
+      </c>
+      <c r="G252" t="s">
+        <v>39</v>
+      </c>
+      <c r="H252" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="253" spans="1:8" x14ac:dyDescent="0.2">
@@ -7310,8 +7355,17 @@
       <c r="D253">
         <v>3</v>
       </c>
+      <c r="E253" t="s">
+        <v>251</v>
+      </c>
       <c r="F253" t="s">
         <v>8</v>
+      </c>
+      <c r="G253" t="s">
+        <v>240</v>
+      </c>
+      <c r="H253" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="254" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
add london (4-8) surprise songs
</commit_message>
<xml_diff>
--- a/data-raw/surprise-songs.xlsx
+++ b/data-raw/surprise-songs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakethompson/Documents/GIT/packages/taylor/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B1852ED-D6F0-3241-9BAB-54FB42222535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64FA7D14-950A-E04E-8A6F-62E57800665D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26240" windowHeight="17500" xr2:uid="{23F40540-2069-D04D-A50F-51228CFC4AB9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1514" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1543" uniqueCount="275">
   <si>
     <t>date</t>
   </si>
@@ -843,6 +843,24 @@
   </si>
   <si>
     <t>Don't You (Taylor's Version) [From The Vault]</t>
+  </si>
+  <si>
+    <t>End Game; Thinking Out Loud</t>
+  </si>
+  <si>
+    <t>Ed Sheeran</t>
+  </si>
+  <si>
+    <t>London Boy</t>
+  </si>
+  <si>
+    <t>I Did Something Bad</t>
+  </si>
+  <si>
+    <t>Change (Taylor's Version)</t>
+  </si>
+  <si>
+    <t>So Long, London</t>
   </si>
 </sst>
 </file>
@@ -1205,7 +1223,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A235" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E262" sqref="E262"/>
+      <selection pane="bottomLeft" activeCell="E264" sqref="E264"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7027,7 +7045,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="241" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>198</v>
       </c>
@@ -7053,7 +7071,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="242" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>198</v>
       </c>
@@ -7079,7 +7097,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="243" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>198</v>
       </c>
@@ -7105,7 +7123,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="244" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>198</v>
       </c>
@@ -7131,7 +7149,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="245" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>198</v>
       </c>
@@ -7157,7 +7175,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="246" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>198</v>
       </c>
@@ -7183,7 +7201,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="247" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>198</v>
       </c>
@@ -7209,7 +7227,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="248" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>198</v>
       </c>
@@ -7235,7 +7253,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="249" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>198</v>
       </c>
@@ -7261,7 +7279,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="250" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>198</v>
       </c>
@@ -7287,7 +7305,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="251" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>198</v>
       </c>
@@ -7313,7 +7331,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="252" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>198</v>
       </c>
@@ -7339,7 +7357,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="253" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>198</v>
       </c>
@@ -7365,7 +7383,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="254" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>198</v>
       </c>
@@ -7378,11 +7396,23 @@
       <c r="D254">
         <v>4</v>
       </c>
+      <c r="E254" t="s">
+        <v>249</v>
+      </c>
       <c r="F254" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="255" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G254" t="s">
+        <v>104</v>
+      </c>
+      <c r="H254" t="s">
+        <v>269</v>
+      </c>
+      <c r="I254" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="255" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>198</v>
       </c>
@@ -7395,11 +7425,20 @@
       <c r="D255">
         <v>4</v>
       </c>
+      <c r="E255" t="s">
+        <v>249</v>
+      </c>
       <c r="F255" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="256" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G255" t="s">
+        <v>115</v>
+      </c>
+      <c r="H255" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="256" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>198</v>
       </c>
@@ -7412,11 +7451,17 @@
       <c r="D256">
         <v>5</v>
       </c>
+      <c r="E256" t="s">
+        <v>250</v>
+      </c>
       <c r="F256" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="257" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G256" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="257" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>198</v>
       </c>
@@ -7429,11 +7474,20 @@
       <c r="D257">
         <v>5</v>
       </c>
+      <c r="E257" t="s">
+        <v>250</v>
+      </c>
       <c r="F257" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="258" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G257" t="s">
+        <v>91</v>
+      </c>
+      <c r="H257" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="258" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>198</v>
       </c>
@@ -7446,11 +7500,17 @@
       <c r="D258">
         <v>6</v>
       </c>
+      <c r="E258" t="s">
+        <v>251</v>
+      </c>
       <c r="F258" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="259" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G258" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="259" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>198</v>
       </c>
@@ -7463,11 +7523,20 @@
       <c r="D259">
         <v>6</v>
       </c>
+      <c r="E259" t="s">
+        <v>251</v>
+      </c>
       <c r="F259" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="260" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G259" t="s">
+        <v>214</v>
+      </c>
+      <c r="H259" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="260" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>198</v>
       </c>
@@ -7480,11 +7549,20 @@
       <c r="D260">
         <v>7</v>
       </c>
+      <c r="E260" t="s">
+        <v>250</v>
+      </c>
       <c r="F260" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="261" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G260" t="s">
+        <v>224</v>
+      </c>
+      <c r="H260" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="261" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>198</v>
       </c>
@@ -7497,11 +7575,20 @@
       <c r="D261">
         <v>7</v>
       </c>
+      <c r="E261" t="s">
+        <v>250</v>
+      </c>
       <c r="F261" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="262" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G261" t="s">
+        <v>252</v>
+      </c>
+      <c r="H261" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="262" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>198</v>
       </c>
@@ -7514,11 +7601,23 @@
       <c r="D262">
         <v>8</v>
       </c>
+      <c r="E262" t="s">
+        <v>251</v>
+      </c>
       <c r="F262" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="263" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G262" t="s">
+        <v>27</v>
+      </c>
+      <c r="H262" t="s">
+        <v>74</v>
+      </c>
+      <c r="I262" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="263" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>198</v>
       </c>
@@ -7531,11 +7630,17 @@
       <c r="D263">
         <v>8</v>
       </c>
+      <c r="E263" t="s">
+        <v>251</v>
+      </c>
       <c r="F263" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="264" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G263" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="264" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
         <v>201</v>
       </c>
@@ -7552,7 +7657,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="265" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>201</v>
       </c>
@@ -7569,7 +7674,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="266" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
         <v>201</v>
       </c>
@@ -7586,7 +7691,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="267" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
         <v>201</v>
       </c>
@@ -7603,7 +7708,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="268" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
         <v>201</v>
       </c>
@@ -7620,7 +7725,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="269" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
         <v>201</v>
       </c>
@@ -7637,7 +7742,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="270" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
         <v>201</v>
       </c>
@@ -7654,7 +7759,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="271" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
         <v>201</v>
       </c>
@@ -7671,7 +7776,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="272" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
         <v>201</v>
       </c>

</xml_diff>

<commit_message>
add miami surprise songs
</commit_message>
<xml_diff>
--- a/data-raw/surprise-songs.xlsx
+++ b/data-raw/surprise-songs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakethompson/Documents/GIT/packages/taylor/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64FA7D14-950A-E04E-8A6F-62E57800665D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5799B1B1-9A4A-7F47-A043-6EFB10581412}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26240" windowHeight="17500" xr2:uid="{23F40540-2069-D04D-A50F-51228CFC4AB9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1543" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1561" uniqueCount="278">
   <si>
     <t>date</t>
   </si>
@@ -861,6 +861,15 @@
   </si>
   <si>
     <t>So Long, London</t>
+  </si>
+  <si>
+    <t>betta fish</t>
+  </si>
+  <si>
+    <t>supernova</t>
+  </si>
+  <si>
+    <t>sunrise boulevard</t>
   </si>
 </sst>
 </file>
@@ -1222,8 +1231,8 @@
   <dimension ref="A1:I299"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A235" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E264" sqref="E264"/>
+      <pane ySplit="1" topLeftCell="A240" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H264" sqref="H264"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7653,8 +7662,17 @@
       <c r="D264">
         <v>1</v>
       </c>
+      <c r="E264" t="s">
+        <v>275</v>
+      </c>
       <c r="F264" t="s">
         <v>7</v>
+      </c>
+      <c r="G264" t="s">
+        <v>10</v>
+      </c>
+      <c r="H264" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="265" spans="1:9" x14ac:dyDescent="0.2">
@@ -7670,8 +7688,17 @@
       <c r="D265">
         <v>1</v>
       </c>
+      <c r="E265" t="s">
+        <v>275</v>
+      </c>
       <c r="F265" t="s">
         <v>8</v>
+      </c>
+      <c r="G265" t="s">
+        <v>11</v>
+      </c>
+      <c r="H265" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="266" spans="1:9" x14ac:dyDescent="0.2">
@@ -7687,8 +7714,17 @@
       <c r="D266">
         <v>2</v>
       </c>
+      <c r="E266" t="s">
+        <v>276</v>
+      </c>
       <c r="F266" t="s">
         <v>7</v>
+      </c>
+      <c r="G266" t="s">
+        <v>70</v>
+      </c>
+      <c r="H266" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="267" spans="1:9" x14ac:dyDescent="0.2">
@@ -7704,8 +7740,17 @@
       <c r="D267">
         <v>2</v>
       </c>
+      <c r="E267" t="s">
+        <v>276</v>
+      </c>
       <c r="F267" t="s">
         <v>8</v>
+      </c>
+      <c r="G267" t="s">
+        <v>213</v>
+      </c>
+      <c r="H267" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="268" spans="1:9" x14ac:dyDescent="0.2">
@@ -7721,8 +7766,17 @@
       <c r="D268">
         <v>3</v>
       </c>
+      <c r="E268" t="s">
+        <v>277</v>
+      </c>
       <c r="F268" t="s">
         <v>7</v>
+      </c>
+      <c r="G268" t="s">
+        <v>48</v>
+      </c>
+      <c r="H268" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="269" spans="1:9" x14ac:dyDescent="0.2">
@@ -7738,8 +7792,17 @@
       <c r="D269">
         <v>3</v>
       </c>
+      <c r="E269" t="s">
+        <v>277</v>
+      </c>
       <c r="F269" t="s">
         <v>8</v>
+      </c>
+      <c r="G269" t="s">
+        <v>9</v>
+      </c>
+      <c r="H269" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="270" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
add new orleans surprise songs
</commit_message>
<xml_diff>
--- a/data-raw/surprise-songs.xlsx
+++ b/data-raw/surprise-songs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakethompson/Documents/GIT/packages/taylor/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5799B1B1-9A4A-7F47-A043-6EFB10581412}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E964CFA1-7713-1F4B-AB96-C9A7761E3419}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26240" windowHeight="17500" xr2:uid="{23F40540-2069-D04D-A50F-51228CFC4AB9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1561" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1580" uniqueCount="281">
   <si>
     <t>date</t>
   </si>
@@ -870,6 +870,15 @@
   </si>
   <si>
     <t>sunrise boulevard</t>
+  </si>
+  <si>
+    <t>Espresso</t>
+  </si>
+  <si>
+    <t>Is It Over Now? (Taylor's Version) [From The Vault]; Please Please Please</t>
+  </si>
+  <si>
+    <t>koi fish</t>
   </si>
 </sst>
 </file>
@@ -1230,9 +1239,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04F0F9D9-7CA5-0C41-BC65-3D3349CBCA23}">
   <dimension ref="A1:I299"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A240" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H264" sqref="H264"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A250" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E276" sqref="E276"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7818,8 +7827,17 @@
       <c r="D270">
         <v>1</v>
       </c>
+      <c r="E270" t="s">
+        <v>280</v>
+      </c>
       <c r="F270" t="s">
         <v>7</v>
+      </c>
+      <c r="G270" t="s">
+        <v>13</v>
+      </c>
+      <c r="H270" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="271" spans="1:9" x14ac:dyDescent="0.2">
@@ -7835,8 +7853,17 @@
       <c r="D271">
         <v>1</v>
       </c>
+      <c r="E271" t="s">
+        <v>280</v>
+      </c>
       <c r="F271" t="s">
         <v>8</v>
+      </c>
+      <c r="G271" t="s">
+        <v>239</v>
+      </c>
+      <c r="H271" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="272" spans="1:9" x14ac:dyDescent="0.2">
@@ -7852,11 +7879,23 @@
       <c r="D272">
         <v>2</v>
       </c>
+      <c r="E272" t="s">
+        <v>251</v>
+      </c>
       <c r="F272" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="273" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G272" t="s">
+        <v>278</v>
+      </c>
+      <c r="H272" t="s">
+        <v>279</v>
+      </c>
+      <c r="I272" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="273" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>201</v>
       </c>
@@ -7869,11 +7908,20 @@
       <c r="D273">
         <v>2</v>
       </c>
+      <c r="E273" t="s">
+        <v>251</v>
+      </c>
       <c r="F273" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="274" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G273" t="s">
+        <v>82</v>
+      </c>
+      <c r="H273" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="274" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>201</v>
       </c>
@@ -7886,11 +7934,20 @@
       <c r="D274">
         <v>3</v>
       </c>
+      <c r="E274" t="s">
+        <v>276</v>
+      </c>
       <c r="F274" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="275" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G274" t="s">
+        <v>122</v>
+      </c>
+      <c r="H274" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="275" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>201</v>
       </c>
@@ -7903,11 +7960,20 @@
       <c r="D275">
         <v>3</v>
       </c>
+      <c r="E275" t="s">
+        <v>276</v>
+      </c>
       <c r="F275" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="276" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G275" t="s">
+        <v>45</v>
+      </c>
+      <c r="H275" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="276" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>201</v>
       </c>
@@ -7924,7 +7990,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="277" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>201</v>
       </c>
@@ -7941,7 +8007,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="278" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>201</v>
       </c>
@@ -7958,7 +8024,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="279" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>201</v>
       </c>
@@ -7975,7 +8041,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="280" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
         <v>201</v>
       </c>
@@ -7992,7 +8058,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="281" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
         <v>201</v>
       </c>
@@ -8009,7 +8075,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="282" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>201</v>
       </c>
@@ -8026,7 +8092,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="283" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
         <v>201</v>
       </c>
@@ -8043,7 +8109,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="284" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
         <v>201</v>
       </c>
@@ -8060,7 +8126,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="285" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>201</v>
       </c>
@@ -8077,7 +8143,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="286" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
         <v>201</v>
       </c>
@@ -8094,7 +8160,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="287" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
         <v>201</v>
       </c>
@@ -8111,7 +8177,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="288" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
         <v>201</v>
       </c>

</xml_diff>

<commit_message>
finish toronto surprise songs
</commit_message>
<xml_diff>
--- a/data-raw/surprise-songs.xlsx
+++ b/data-raw/surprise-songs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakethompson/Documents/GIT/packages/taylor/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FFF9F25-312F-AD4B-8C81-4CAE1A97DDF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{185A3995-7B90-CA4E-900E-EB3CE848F33D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26240" windowHeight="17500" xr2:uid="{23F40540-2069-D04D-A50F-51228CFC4AB9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1598" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1635" uniqueCount="283">
   <si>
     <t>date</t>
   </si>
@@ -879,6 +879,12 @@
   </si>
   <si>
     <t>koi fish</t>
+  </si>
+  <si>
+    <t>Cassandra</t>
+  </si>
+  <si>
+    <t>mad woman; I Did Something Bad</t>
   </si>
 </sst>
 </file>
@@ -1239,9 +1245,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04F0F9D9-7CA5-0C41-BC65-3D3349CBCA23}">
   <dimension ref="A1:I299"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A250" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E280" sqref="E280"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A272" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G291" sqref="G291"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7895,7 +7901,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="273" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>201</v>
       </c>
@@ -7921,7 +7927,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="274" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>201</v>
       </c>
@@ -7947,7 +7953,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="275" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>201</v>
       </c>
@@ -7973,7 +7979,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="276" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>201</v>
       </c>
@@ -7999,7 +8005,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="277" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>201</v>
       </c>
@@ -8025,7 +8031,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="278" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>201</v>
       </c>
@@ -8051,7 +8057,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="279" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>201</v>
       </c>
@@ -8077,7 +8083,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="280" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
         <v>201</v>
       </c>
@@ -8103,7 +8109,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="281" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
         <v>201</v>
       </c>
@@ -8129,7 +8135,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="282" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>201</v>
       </c>
@@ -8142,11 +8148,20 @@
       <c r="D282">
         <v>1</v>
       </c>
+      <c r="E282" t="s">
+        <v>280</v>
+      </c>
       <c r="F282" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="283" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G282" t="s">
+        <v>214</v>
+      </c>
+      <c r="H282" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="283" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
         <v>201</v>
       </c>
@@ -8159,11 +8174,20 @@
       <c r="D283">
         <v>1</v>
       </c>
+      <c r="E283" t="s">
+        <v>280</v>
+      </c>
       <c r="F283" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="284" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G283" t="s">
+        <v>77</v>
+      </c>
+      <c r="H283" s="3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="284" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
         <v>201</v>
       </c>
@@ -8176,11 +8200,20 @@
       <c r="D284">
         <v>2</v>
       </c>
+      <c r="E284" t="s">
+        <v>276</v>
+      </c>
       <c r="F284" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="285" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G284" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="H284" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="285" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>201</v>
       </c>
@@ -8193,11 +8226,20 @@
       <c r="D285">
         <v>2</v>
       </c>
+      <c r="E285" t="s">
+        <v>276</v>
+      </c>
       <c r="F285" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="286" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G285" t="s">
+        <v>94</v>
+      </c>
+      <c r="H285" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="286" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
         <v>201</v>
       </c>
@@ -8210,11 +8252,23 @@
       <c r="D286">
         <v>3</v>
       </c>
+      <c r="E286" t="s">
+        <v>277</v>
+      </c>
       <c r="F286" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="287" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G286" t="s">
+        <v>243</v>
+      </c>
+      <c r="H286" t="s">
+        <v>48</v>
+      </c>
+      <c r="I286" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="287" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
         <v>201</v>
       </c>
@@ -8227,11 +8281,20 @@
       <c r="D287">
         <v>3</v>
       </c>
+      <c r="E287" t="s">
+        <v>277</v>
+      </c>
       <c r="F287" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="288" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G287" t="s">
+        <v>123</v>
+      </c>
+      <c r="H287" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="288" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
         <v>201</v>
       </c>
@@ -8244,11 +8307,20 @@
       <c r="D288">
         <v>4</v>
       </c>
+      <c r="E288" t="s">
+        <v>275</v>
+      </c>
       <c r="F288" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="289" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G288" t="s">
+        <v>130</v>
+      </c>
+      <c r="H288" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="289" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
         <v>201</v>
       </c>
@@ -8261,11 +8333,20 @@
       <c r="D289">
         <v>4</v>
       </c>
+      <c r="E289" t="s">
+        <v>275</v>
+      </c>
       <c r="F289" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="290" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G289" t="s">
+        <v>14</v>
+      </c>
+      <c r="H289" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="290" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
         <v>201</v>
       </c>
@@ -8278,11 +8359,20 @@
       <c r="D290">
         <v>5</v>
       </c>
+      <c r="E290" t="s">
+        <v>280</v>
+      </c>
       <c r="F290" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="291" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G290" t="s">
+        <v>26</v>
+      </c>
+      <c r="H290" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="291" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
         <v>201</v>
       </c>
@@ -8295,11 +8385,20 @@
       <c r="D291">
         <v>5</v>
       </c>
+      <c r="E291" t="s">
+        <v>280</v>
+      </c>
       <c r="F291" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="292" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G291" t="s">
+        <v>281</v>
+      </c>
+      <c r="H291" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="292" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
         <v>201</v>
       </c>
@@ -8312,11 +8411,20 @@
       <c r="D292">
         <v>6</v>
       </c>
+      <c r="E292" t="s">
+        <v>276</v>
+      </c>
       <c r="F292" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="293" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G292" t="s">
+        <v>46</v>
+      </c>
+      <c r="H292" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="293" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
         <v>201</v>
       </c>
@@ -8329,11 +8437,20 @@
       <c r="D293">
         <v>6</v>
       </c>
+      <c r="E293" t="s">
+        <v>276</v>
+      </c>
       <c r="F293" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="294" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G293" t="s">
+        <v>203</v>
+      </c>
+      <c r="H293" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="294" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
         <v>201</v>
       </c>
@@ -8350,7 +8467,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="295" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
         <v>201</v>
       </c>
@@ -8367,7 +8484,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="296" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
         <v>201</v>
       </c>
@@ -8384,7 +8501,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="297" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
         <v>201</v>
       </c>
@@ -8401,7 +8518,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="298" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
         <v>201</v>
       </c>
@@ -8418,7 +8535,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="299" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
         <v>201</v>
       </c>

</xml_diff>